<commit_message>
EPBDS-9610 Checking name of different types of tables during binding
--HG--
branch : EPBDS-9610_illegal_symbols_in_table_names
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Datatype.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Datatype.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F755E6-4D0D-4876-926E-9537AEA7509F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C62AD75-EF35-4501-A0EB-083141902416}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="6165" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datatypes" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -1182,9 +1184,6 @@
     <t>result</t>
   </si>
   <si>
-    <t>Test evaluate evaluateTest()</t>
-  </si>
-  <si>
     <t>_res_.$equals$result</t>
   </si>
   <si>
@@ -1606,6 +1605,9 @@
   </si>
   <si>
     <t>java.time.Instant</t>
+  </si>
+  <si>
+    <t>Test evaluate evaluateTest</t>
   </si>
 </sst>
 </file>
@@ -1844,39 +1846,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1905,6 +1881,32 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2263,28 +2265,28 @@
       <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="20.68359375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="20.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="37.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.15625" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="32" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="7.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="27.7109375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="52.28515625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="7.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.7109375" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.41796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="37.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.15625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="27.68359375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="19.41796875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="52.26171875" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="7.15625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="24.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="15.68359375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F3" s="13" t="s">
         <v>182</v>
       </c>
@@ -2296,19 +2298,19 @@
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F4" s="21" t="s">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F4" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="N4" s="21" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="N4" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="O4" s="21"/>
-      <c r="P4" s="21"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O4" s="26"/>
+      <c r="P4" s="26"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="13" t="s">
         <v>14</v>
       </c>
@@ -2319,18 +2321,18 @@
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
       <c r="N7" s="13" t="s">
         <v>138</v>
       </c>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="10" t="s">
         <v>192</v>
       </c>
@@ -2368,7 +2370,7 @@
       </c>
       <c r="P8" s="10"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="10" t="s">
         <v>10</v>
       </c>
@@ -2407,7 +2409,7 @@
       </c>
       <c r="P9" s="10"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="10" t="s">
         <v>11</v>
       </c>
@@ -2446,7 +2448,7 @@
       </c>
       <c r="P10" s="10"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="10" t="s">
         <v>0</v>
       </c>
@@ -2485,7 +2487,7 @@
       </c>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
@@ -2524,7 +2526,7 @@
       </c>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
@@ -2563,7 +2565,7 @@
       </c>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="10" t="s">
         <v>8</v>
       </c>
@@ -2602,7 +2604,7 @@
       </c>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="10" t="s">
         <v>15</v>
       </c>
@@ -2641,7 +2643,7 @@
       </c>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="10" t="s">
         <v>16</v>
       </c>
@@ -2680,12 +2682,12 @@
       </c>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>20</v>
@@ -2719,12 +2721,12 @@
       </c>
       <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>95</v>
@@ -2758,12 +2760,12 @@
       </c>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="10" t="s">
+        <v>299</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>300</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>301</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>95</v>
@@ -2781,10 +2783,10 @@
         <v>03/31/2017</v>
       </c>
       <c r="J19" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K19" s="10" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L19" s="1"/>
       <c r="N19" s="10" t="str">
@@ -2797,15 +2799,15 @@
       </c>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F20" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2820,10 +2822,10 @@
         <v>21:30:25</v>
       </c>
       <c r="J20" s="10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K20" s="10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L20" s="1"/>
       <c r="N20" s="10" t="str">
@@ -2836,15 +2838,15 @@
       </c>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F21" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2859,10 +2861,10 @@
         <v>9/20/2019 5:50 AM</v>
       </c>
       <c r="J21" s="10" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K21" s="10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L21" s="1"/>
       <c r="N21" s="10" t="str">
@@ -2875,15 +2877,15 @@
       </c>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>317</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="D22" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>319</v>
       </c>
       <c r="F22" s="10" t="str">
         <f t="shared" si="0"/>
@@ -2898,10 +2900,10 @@
         <v>9/20/2019 5:50 AM America/Los_Angeles</v>
       </c>
       <c r="J22" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="K22" s="10" t="s">
         <v>317</v>
-      </c>
-      <c r="K22" s="10" t="s">
-        <v>318</v>
       </c>
       <c r="L22" s="1"/>
       <c r="N22" s="10" t="str">
@@ -2914,15 +2916,15 @@
       </c>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="C23" s="12" t="s">
         <v>329</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>330</v>
-      </c>
       <c r="D23" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F23" s="12" t="str">
         <f t="shared" ref="F23" si="4">"_res_." &amp; C23</f>
@@ -2937,10 +2939,10 @@
         <v>9/20/2019 5:50 AM America/Los_Angeles</v>
       </c>
       <c r="J23" s="12" t="s">
+        <v>328</v>
+      </c>
+      <c r="K23" s="12" t="s">
         <v>329</v>
-      </c>
-      <c r="K23" s="12" t="s">
-        <v>330</v>
       </c>
       <c r="L23" s="1"/>
       <c r="N23" s="12" t="str">
@@ -2953,12 +2955,12 @@
       </c>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D24" s="10">
         <v>7</v>
@@ -2992,12 +2994,12 @@
       </c>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D25" s="10">
         <v>8</v>
@@ -3031,12 +3033,12 @@
       </c>
       <c r="P25" s="10"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="10" t="s">
         <v>145</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>2</v>
@@ -3067,12 +3069,12 @@
       </c>
       <c r="P26" s="10"/>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>2</v>
@@ -3103,12 +3105,12 @@
       </c>
       <c r="P27" s="10"/>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>2</v>
@@ -3139,12 +3141,12 @@
       </c>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" s="10" t="s">
         <v>37</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>2</v>
@@ -3175,12 +3177,12 @@
       </c>
       <c r="P29" s="10"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>2</v>
@@ -3195,10 +3197,10 @@
       </c>
       <c r="H30" s="10"/>
       <c r="J30" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="K30" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L30" s="10"/>
       <c r="N30" s="10" t="str">
@@ -3211,12 +3213,12 @@
       </c>
       <c r="P30" s="10"/>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>2</v>
@@ -3231,10 +3233,10 @@
       </c>
       <c r="H31" s="10"/>
       <c r="J31" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K31" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L31" s="10"/>
       <c r="N31" s="10" t="str">
@@ -3247,12 +3249,12 @@
       </c>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>2</v>
@@ -3267,10 +3269,10 @@
       </c>
       <c r="H32" s="10"/>
       <c r="J32" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="K32" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L32" s="10"/>
       <c r="N32" s="10" t="str">
@@ -3283,15 +3285,15 @@
       </c>
       <c r="P32" s="10"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="D33" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>252</v>
       </c>
       <c r="F33" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3306,10 +3308,10 @@
         <v>HALF_EVEN</v>
       </c>
       <c r="J33" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="K33" s="10" t="s">
         <v>250</v>
-      </c>
-      <c r="K33" s="10" t="s">
-        <v>251</v>
       </c>
       <c r="L33" s="10"/>
       <c r="N33" s="10" t="str">
@@ -3322,12 +3324,12 @@
       </c>
       <c r="P33" s="10"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" s="10" t="s">
         <v>192</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D34" s="10">
         <v>10.1</v>
@@ -3348,7 +3350,7 @@
         <v>192</v>
       </c>
       <c r="K34" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L34" s="10"/>
       <c r="N34" s="10" t="str">
@@ -3361,12 +3363,12 @@
       </c>
       <c r="P34" s="10"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D35" s="10">
         <v>-3</v>
@@ -3384,10 +3386,10 @@
         <v>-3</v>
       </c>
       <c r="J35" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K35" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L35" s="10"/>
       <c r="N35" s="10" t="str">
@@ -3402,12 +3404,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D36" s="10">
         <v>3.3</v>
@@ -3425,10 +3427,10 @@
         <v>3.3</v>
       </c>
       <c r="J36" s="10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K36" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L36" s="10"/>
       <c r="N36" s="10" t="str">
@@ -3441,15 +3443,15 @@
       </c>
       <c r="P36" s="10"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B37" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C37" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="D37" s="10" t="s">
         <v>276</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>277</v>
       </c>
       <c r="F37" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3464,10 +3466,10 @@
         <v>n</v>
       </c>
       <c r="J37" s="10" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K37" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L37" s="10"/>
       <c r="N37" s="10" t="str">
@@ -3480,15 +3482,15 @@
       </c>
       <c r="P37" s="10"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="C38" s="10" t="s">
-        <v>244</v>
-      </c>
       <c r="D38" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F38" s="10" t="str">
         <f t="shared" si="0"/>
@@ -3503,10 +3505,10 @@
         <v>Male</v>
       </c>
       <c r="J38" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="K38" s="10" t="s">
         <v>243</v>
-      </c>
-      <c r="K38" s="10" t="s">
-        <v>244</v>
       </c>
       <c r="L38" s="10"/>
       <c r="N38" s="10" t="str">
@@ -3519,7 +3521,7 @@
       </c>
       <c r="P38" s="10"/>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B39" s="10" t="s">
         <v>6</v>
       </c>
@@ -3555,12 +3557,12 @@
       </c>
       <c r="P39" s="10"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C40" s="10" t="s">
         <v>210</v>
-      </c>
-      <c r="C40" s="10" t="s">
-        <v>211</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>2</v>
@@ -3575,10 +3577,10 @@
       </c>
       <c r="H40" s="10"/>
       <c r="J40" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="K40" s="10" t="s">
         <v>210</v>
-      </c>
-      <c r="K40" s="10" t="s">
-        <v>211</v>
       </c>
       <c r="L40" s="10"/>
       <c r="N40" s="10" t="str">
@@ -3591,12 +3593,12 @@
       </c>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>2</v>
@@ -3611,10 +3613,10 @@
       </c>
       <c r="H41" s="10"/>
       <c r="J41" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K41" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L41" s="10"/>
       <c r="N41" s="10" t="str">
@@ -3627,76 +3629,76 @@
       </c>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F42" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="G42" s="10" t="s">
         <v>287</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>288</v>
       </c>
       <c r="H42" s="10">
         <v>150</v>
       </c>
     </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F43" s="10" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G43" s="10" t="s">
         <v>6</v>
       </c>
       <c r="H43" s="10"/>
     </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F44" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G44" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H44" s="10">
         <v>150</v>
       </c>
     </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F45" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="G45" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="G45" s="10" t="s">
+      <c r="H45" s="10"/>
+    </row>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F46" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="H45" s="10"/>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F46" s="10" t="s">
+      <c r="G46" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F47" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="G46" s="10" t="s">
-        <v>243</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F47" s="10" t="s">
+      <c r="G47" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="H47" s="10"/>
+    </row>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F48" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="G47" s="10" t="s">
+      <c r="G48" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="H47" s="10"/>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F48" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>298</v>
-      </c>
       <c r="H48" s="10"/>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F51" s="13" t="s">
         <v>181</v>
       </c>
@@ -3708,41 +3710,41 @@
       <c r="O51" s="13"/>
       <c r="P51" s="13"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F52" s="21" t="s">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F52" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="G52" s="21"/>
-      <c r="H52" s="21"/>
-      <c r="N52" s="21" t="s">
+      <c r="G52" s="26"/>
+      <c r="H52" s="26"/>
+      <c r="N52" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="O52" s="21"/>
-      <c r="P52" s="21"/>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O52" s="26"/>
+      <c r="P52" s="26"/>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B55" s="13" t="s">
         <v>88</v>
       </c>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
-      <c r="F55" s="22" t="s">
+      <c r="F55" s="27" t="s">
         <v>163</v>
       </c>
-      <c r="G55" s="22"/>
-      <c r="H55" s="22"/>
-      <c r="J55" s="23" t="s">
+      <c r="G55" s="27"/>
+      <c r="H55" s="27"/>
+      <c r="J55" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="K55" s="23"/>
-      <c r="L55" s="23"/>
-      <c r="N55" s="22" t="s">
+      <c r="K55" s="28"/>
+      <c r="L55" s="28"/>
+      <c r="N55" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="O55" s="22"/>
-      <c r="P55" s="22"/>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O55" s="27"/>
+      <c r="P55" s="27"/>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" s="10" t="s">
         <v>192</v>
       </c>
@@ -3784,7 +3786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B57" s="10" t="s">
         <v>39</v>
       </c>
@@ -3825,7 +3827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B58" s="10" t="s">
         <v>40</v>
       </c>
@@ -3866,7 +3868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B59" s="10" t="s">
         <v>41</v>
       </c>
@@ -3907,7 +3909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B60" s="10" t="s">
         <v>42</v>
       </c>
@@ -3948,7 +3950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B61" s="10" t="s">
         <v>43</v>
       </c>
@@ -3989,7 +3991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B62" s="10" t="s">
         <v>44</v>
       </c>
@@ -4030,7 +4032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B63" s="10" t="s">
         <v>46</v>
       </c>
@@ -4071,7 +4073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B64" s="10" t="s">
         <v>45</v>
       </c>
@@ -4110,7 +4112,7 @@
       </c>
       <c r="P64" s="10"/>
     </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F67" s="13" t="s">
         <v>179</v>
       </c>
@@ -4122,19 +4124,19 @@
       <c r="O67" s="13"/>
       <c r="P67" s="13"/>
     </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F68" s="21" t="s">
+    <row r="68" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F68" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="G68" s="21"/>
-      <c r="H68" s="21"/>
-      <c r="N68" s="21" t="s">
+      <c r="G68" s="26"/>
+      <c r="H68" s="26"/>
+      <c r="N68" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="O68" s="21"/>
-      <c r="P68" s="21"/>
-    </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O68" s="26"/>
+      <c r="P68" s="26"/>
+    </row>
+    <row r="71" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B71" s="13" t="s">
         <v>143</v>
       </c>
@@ -4145,18 +4147,18 @@
       </c>
       <c r="G71" s="13"/>
       <c r="H71" s="13"/>
-      <c r="J71" s="23" t="s">
+      <c r="J71" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="K71" s="23"/>
-      <c r="L71" s="23"/>
+      <c r="K71" s="28"/>
+      <c r="L71" s="28"/>
       <c r="N71" s="13" t="s">
         <v>159</v>
       </c>
       <c r="O71" s="13"/>
       <c r="P71" s="13"/>
     </row>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B72" s="10" t="s">
         <v>192</v>
       </c>
@@ -4198,7 +4200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B73" s="10" t="s">
         <v>98</v>
       </c>
@@ -4237,7 +4239,7 @@
       </c>
       <c r="P73" s="10"/>
     </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B74" s="10" t="s">
         <v>99</v>
       </c>
@@ -4276,7 +4278,7 @@
       </c>
       <c r="P74" s="10"/>
     </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B75" s="10" t="s">
         <v>100</v>
       </c>
@@ -4315,7 +4317,7 @@
       </c>
       <c r="P75" s="10"/>
     </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B76" s="10" t="s">
         <v>101</v>
       </c>
@@ -4354,7 +4356,7 @@
       </c>
       <c r="P76" s="10"/>
     </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B77" s="10" t="s">
         <v>102</v>
       </c>
@@ -4393,7 +4395,7 @@
       </c>
       <c r="P77" s="10"/>
     </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B78" s="10" t="s">
         <v>103</v>
       </c>
@@ -4432,7 +4434,7 @@
       </c>
       <c r="P78" s="10"/>
     </row>
-    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B79" s="10" t="s">
         <v>104</v>
       </c>
@@ -4471,7 +4473,7 @@
       </c>
       <c r="P79" s="10"/>
     </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B80" s="10" t="s">
         <v>105</v>
       </c>
@@ -4510,7 +4512,7 @@
       </c>
       <c r="P80" s="10"/>
     </row>
-    <row r="81" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B81" s="10" t="s">
         <v>58</v>
       </c>
@@ -4549,7 +4551,7 @@
       </c>
       <c r="P81" s="10"/>
     </row>
-    <row r="82" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B82" s="10" t="s">
         <v>59</v>
       </c>
@@ -4588,12 +4590,12 @@
       </c>
       <c r="P82" s="1"/>
     </row>
-    <row r="83" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B83" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>95</v>
@@ -4611,10 +4613,10 @@
         <v>03/31/2017</v>
       </c>
       <c r="J83" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="K83" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L83" s="1"/>
       <c r="N83" s="11" t="str">
@@ -4627,15 +4629,15 @@
       </c>
       <c r="P83" s="1"/>
     </row>
-    <row r="84" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B84" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F84" s="11" t="str">
         <f t="shared" si="18"/>
@@ -4650,10 +4652,10 @@
         <v>21:30:25</v>
       </c>
       <c r="J84" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K84" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L84" s="1"/>
       <c r="N84" s="11" t="str">
@@ -4666,15 +4668,15 @@
       </c>
       <c r="P84" s="1"/>
     </row>
-    <row r="85" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B85" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C85" s="11" t="s">
+        <v>314</v>
+      </c>
+      <c r="D85" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>316</v>
       </c>
       <c r="F85" s="11" t="str">
         <f t="shared" ref="F85:F86" si="23">"_res_." &amp; C85</f>
@@ -4689,10 +4691,10 @@
         <v>9/20/2019 5:50 AM</v>
       </c>
       <c r="J85" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="K85" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L85" s="1"/>
       <c r="N85" s="11" t="str">
@@ -4705,15 +4707,15 @@
       </c>
       <c r="P85" s="1"/>
     </row>
-    <row r="86" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B86" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="C86" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="C86" s="11" t="s">
-        <v>324</v>
-      </c>
       <c r="D86" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F86" s="11" t="str">
         <f t="shared" si="23"/>
@@ -4728,10 +4730,10 @@
         <v>9/20/2019 5:50 AM America/Los_Angeles</v>
       </c>
       <c r="J86" s="11" t="s">
+        <v>322</v>
+      </c>
+      <c r="K86" s="11" t="s">
         <v>323</v>
-      </c>
-      <c r="K86" s="11" t="s">
-        <v>324</v>
       </c>
       <c r="L86" s="1"/>
       <c r="N86" s="11" t="str">
@@ -4744,15 +4746,15 @@
       </c>
       <c r="P86" s="1"/>
     </row>
-    <row r="87" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B87" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="C87" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="C87" s="12" t="s">
-        <v>332</v>
-      </c>
       <c r="D87" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F87" s="12" t="str">
         <f t="shared" ref="F87" si="28">"_res_." &amp; C87</f>
@@ -4767,7 +4769,7 @@
         <v>9/20/2019 5:50 AM America/Los_Angeles</v>
       </c>
       <c r="J87" s="12" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K87" s="12" t="str">
         <f t="shared" ref="K87" si="31">G87</f>
@@ -4784,7 +4786,7 @@
       </c>
       <c r="P87" s="1"/>
     </row>
-    <row r="88" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B88" s="10" t="s">
         <v>60</v>
       </c>
@@ -4823,7 +4825,7 @@
       </c>
       <c r="P88" s="10"/>
     </row>
-    <row r="89" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B89" s="10" t="s">
         <v>61</v>
       </c>
@@ -4862,7 +4864,7 @@
       </c>
       <c r="P89" s="10"/>
     </row>
-    <row r="90" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B90" s="10" t="s">
         <v>148</v>
       </c>
@@ -4898,9 +4900,9 @@
       </c>
       <c r="P90" s="10"/>
     </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B91" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>35</v>
@@ -4934,7 +4936,7 @@
       </c>
       <c r="P91" s="10"/>
     </row>
-    <row r="92" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B92" s="10" t="s">
         <v>116</v>
       </c>
@@ -4970,7 +4972,7 @@
       </c>
       <c r="P92" s="10"/>
     </row>
-    <row r="93" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B93" s="10" t="s">
         <v>117</v>
       </c>
@@ -5006,12 +5008,12 @@
       </c>
       <c r="P93" s="10"/>
     </row>
-    <row r="94" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B94" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C94" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D94" s="10" t="s">
         <v>2</v>
@@ -5026,10 +5028,10 @@
       </c>
       <c r="H94" s="10"/>
       <c r="J94" s="10" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K94" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L94" s="10"/>
       <c r="N94" s="10" t="str">
@@ -5042,12 +5044,12 @@
       </c>
       <c r="P94" s="10"/>
     </row>
-    <row r="95" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B95" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C95" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D95" s="10" t="s">
         <v>2</v>
@@ -5062,10 +5064,10 @@
       </c>
       <c r="H95" s="10"/>
       <c r="J95" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="K95" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L95" s="10"/>
       <c r="N95" s="10" t="str">
@@ -5078,12 +5080,12 @@
       </c>
       <c r="P95" s="10"/>
     </row>
-    <row r="96" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B96" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C96" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D96" s="10" t="s">
         <v>2</v>
@@ -5098,10 +5100,10 @@
       </c>
       <c r="H96" s="10"/>
       <c r="J96" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="K96" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L96" s="10"/>
       <c r="N96" s="10" t="str">
@@ -5114,15 +5116,15 @@
       </c>
       <c r="P96" s="10"/>
     </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B97" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C97" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="F97" s="10" t="str">
         <f t="shared" si="14"/>
@@ -5137,10 +5139,10 @@
         <v>0, 5</v>
       </c>
       <c r="J97" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K97" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L97" s="10"/>
       <c r="N97" s="10" t="str">
@@ -5153,15 +5155,15 @@
       </c>
       <c r="P97" s="10"/>
     </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B98" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C98" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F98" s="10" t="str">
         <f t="shared" si="14"/>
@@ -5176,10 +5178,10 @@
         <v>-1, -5.5, 3.3</v>
       </c>
       <c r="J98" s="10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K98" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L98" s="10"/>
       <c r="N98" s="10" t="str">
@@ -5192,15 +5194,15 @@
       </c>
       <c r="P98" s="10"/>
     </row>
-    <row r="99" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B99" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C99" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D99" s="10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F99" s="10" t="str">
         <f t="shared" si="14"/>
@@ -5215,10 +5217,10 @@
         <v>n,y</v>
       </c>
       <c r="J99" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K99" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L99" s="10"/>
       <c r="N99" s="10" t="str">
@@ -5231,15 +5233,15 @@
       </c>
       <c r="P99" s="10"/>
     </row>
-    <row r="100" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B100" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F100" s="10" t="str">
         <f t="shared" si="14"/>
@@ -5254,10 +5256,10 @@
         <v>Male, Female</v>
       </c>
       <c r="J100" s="10" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K100" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L100" s="10"/>
       <c r="N100" s="10" t="str">
@@ -5270,12 +5272,12 @@
       </c>
       <c r="P100" s="10"/>
     </row>
-    <row r="101" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B101" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D101" s="10" t="s">
         <v>2</v>
@@ -5290,10 +5292,10 @@
       </c>
       <c r="H101" s="10"/>
       <c r="J101" s="10" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K101" s="10" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L101" s="10"/>
       <c r="N101" s="10" t="str">
@@ -5306,9 +5308,9 @@
       </c>
       <c r="P101" s="10"/>
     </row>
-    <row r="102" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B102" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C102" s="10" t="s">
         <v>7</v>
@@ -5326,7 +5328,7 @@
       </c>
       <c r="H102" s="10"/>
       <c r="J102" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="K102" s="10" t="s">
         <v>7</v>
@@ -5342,12 +5344,12 @@
       </c>
       <c r="P102" s="10"/>
     </row>
-    <row r="103" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B103" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C103" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D103" s="10" t="s">
         <v>2</v>
@@ -5362,10 +5364,10 @@
       </c>
       <c r="H103" s="10"/>
       <c r="J103" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K103" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L103" s="10"/>
       <c r="N103" s="10" t="str">
@@ -5378,15 +5380,15 @@
       </c>
       <c r="P103" s="10"/>
     </row>
-    <row r="104" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B104" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>250</v>
+      </c>
+      <c r="D104" s="10" t="s">
         <v>253</v>
-      </c>
-      <c r="C104" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="D104" s="10" t="s">
-        <v>254</v>
       </c>
       <c r="F104" s="10" t="str">
         <f>"_res_." &amp; C104</f>
@@ -5401,10 +5403,10 @@
         <v>UP, DOWN</v>
       </c>
       <c r="J104" s="10" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="K104" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L104" s="10"/>
       <c r="N104" s="10" t="str">
@@ -5417,15 +5419,15 @@
       </c>
       <c r="P104" s="10"/>
     </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B105" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="C105" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>257</v>
-      </c>
-      <c r="C105" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="D105" s="1" t="s">
-        <v>258</v>
       </c>
       <c r="F105" s="10" t="str">
         <f>"_res_." &amp; C105</f>
@@ -5440,10 +5442,10 @@
         <v>10.1, 22.4</v>
       </c>
       <c r="J105" s="10" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K105" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L105" s="10"/>
       <c r="N105" s="10" t="str">
@@ -5456,7 +5458,7 @@
       </c>
       <c r="P105" s="10"/>
     </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F108" s="13" t="s">
         <v>177</v>
       </c>
@@ -5468,19 +5470,19 @@
       <c r="O108" s="13"/>
       <c r="P108" s="13"/>
     </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F109" s="21" t="s">
+    <row r="109" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F109" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="G109" s="21"/>
-      <c r="H109" s="21"/>
-      <c r="N109" s="21" t="s">
+      <c r="G109" s="26"/>
+      <c r="H109" s="26"/>
+      <c r="N109" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="O109" s="21"/>
-      <c r="P109" s="21"/>
-    </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O109" s="26"/>
+      <c r="P109" s="26"/>
+    </row>
+    <row r="112" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B112" s="13" t="s">
         <v>144</v>
       </c>
@@ -5491,18 +5493,18 @@
       </c>
       <c r="G112" s="13"/>
       <c r="H112" s="13"/>
-      <c r="J112" s="23" t="s">
+      <c r="J112" s="28" t="s">
         <v>142</v>
       </c>
-      <c r="K112" s="23"/>
-      <c r="L112" s="23"/>
-      <c r="N112" s="22" t="s">
+      <c r="K112" s="28"/>
+      <c r="L112" s="28"/>
+      <c r="N112" s="27" t="s">
         <v>165</v>
       </c>
-      <c r="O112" s="22"/>
-      <c r="P112" s="22"/>
-    </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O112" s="27"/>
+      <c r="P112" s="27"/>
+    </row>
+    <row r="113" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B113" s="10" t="s">
         <v>192</v>
       </c>
@@ -5544,7 +5546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B114" s="10" t="s">
         <v>47</v>
       </c>
@@ -5582,7 +5584,7 @@
       </c>
       <c r="P114" s="10"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B115" s="10" t="s">
         <v>48</v>
       </c>
@@ -5620,7 +5622,7 @@
       </c>
       <c r="P115" s="10"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B116" s="10" t="s">
         <v>49</v>
       </c>
@@ -5658,7 +5660,7 @@
       </c>
       <c r="P116" s="10"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B117" s="10" t="s">
         <v>50</v>
       </c>
@@ -5696,7 +5698,7 @@
       </c>
       <c r="P117" s="10"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B118" s="10" t="s">
         <v>51</v>
       </c>
@@ -5734,7 +5736,7 @@
       </c>
       <c r="P118" s="10"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B119" s="10" t="s">
         <v>52</v>
       </c>
@@ -5772,7 +5774,7 @@
       </c>
       <c r="P119" s="10"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B120" s="10" t="s">
         <v>53</v>
       </c>
@@ -5810,7 +5812,7 @@
       </c>
       <c r="P120" s="10"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B121" s="10" t="s">
         <v>54</v>
       </c>
@@ -5848,7 +5850,7 @@
       </c>
       <c r="P121" s="10"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F124" s="13" t="s">
         <v>168</v>
       </c>
@@ -5860,19 +5862,19 @@
       <c r="O124" s="13"/>
       <c r="P124" s="13"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F125" s="21" t="s">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F125" s="26" t="s">
         <v>169</v>
       </c>
-      <c r="G125" s="21"/>
-      <c r="H125" s="21"/>
-      <c r="N125" s="21" t="s">
+      <c r="G125" s="26"/>
+      <c r="H125" s="26"/>
+      <c r="N125" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="O125" s="21"/>
-      <c r="P125" s="21"/>
-    </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O125" s="26"/>
+      <c r="P125" s="26"/>
+    </row>
+    <row r="128" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B128" s="13" t="s">
         <v>155</v>
       </c>
@@ -5883,18 +5885,18 @@
       </c>
       <c r="G128" s="13"/>
       <c r="H128" s="13"/>
-      <c r="J128" s="23" t="s">
+      <c r="J128" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="K128" s="23"/>
-      <c r="L128" s="23"/>
+      <c r="K128" s="28"/>
+      <c r="L128" s="28"/>
       <c r="N128" s="13" t="s">
         <v>191</v>
       </c>
       <c r="O128" s="13"/>
       <c r="P128" s="13"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B129" s="10" t="s">
         <v>192</v>
       </c>
@@ -5936,7 +5938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B130" s="10" t="s">
         <v>106</v>
       </c>
@@ -5972,7 +5974,7 @@
       </c>
       <c r="P130" s="10"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B131" s="10" t="s">
         <v>107</v>
       </c>
@@ -6008,7 +6010,7 @@
       </c>
       <c r="P131" s="10"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B132" s="10" t="s">
         <v>108</v>
       </c>
@@ -6044,7 +6046,7 @@
       </c>
       <c r="P132" s="10"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B133" s="10" t="s">
         <v>109</v>
       </c>
@@ -6080,7 +6082,7 @@
       </c>
       <c r="P133" s="10"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B134" s="10" t="s">
         <v>110</v>
       </c>
@@ -6116,7 +6118,7 @@
       </c>
       <c r="P134" s="10"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B135" s="10" t="s">
         <v>111</v>
       </c>
@@ -6152,7 +6154,7 @@
       </c>
       <c r="P135" s="10"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B136" s="10" t="s">
         <v>112</v>
       </c>
@@ -6188,7 +6190,7 @@
       </c>
       <c r="P136" s="10"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B137" s="10" t="s">
         <v>113</v>
       </c>
@@ -6224,7 +6226,7 @@
       </c>
       <c r="P137" s="10"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B138" s="10" t="s">
         <v>71</v>
       </c>
@@ -6260,7 +6262,7 @@
       </c>
       <c r="P138" s="10"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B139" s="10" t="s">
         <v>72</v>
       </c>
@@ -6296,12 +6298,12 @@
       </c>
       <c r="P139" s="1"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B140" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C140" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D140" s="11" t="s">
         <v>2</v>
@@ -6316,10 +6318,10 @@
       </c>
       <c r="H140" s="11"/>
       <c r="J140" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K140" s="11" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L140" s="1"/>
       <c r="N140" s="11" t="str">
@@ -6332,12 +6334,12 @@
       </c>
       <c r="P140" s="1"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B141" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C141" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D141" s="11" t="s">
         <v>2</v>
@@ -6352,10 +6354,10 @@
       </c>
       <c r="H141" s="11"/>
       <c r="J141" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K141" s="11" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L141" s="1"/>
       <c r="N141" s="11" t="str">
@@ -6368,12 +6370,12 @@
       </c>
       <c r="P141" s="1"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B142" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C142" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D142" s="11" t="s">
         <v>2</v>
@@ -6388,10 +6390,10 @@
       </c>
       <c r="H142" s="11"/>
       <c r="J142" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K142" s="11" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L142" s="1"/>
       <c r="N142" s="11" t="str">
@@ -6404,12 +6406,12 @@
       </c>
       <c r="P142" s="1"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B143" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C143" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D143" s="11" t="s">
         <v>2</v>
@@ -6424,10 +6426,10 @@
       </c>
       <c r="H143" s="11"/>
       <c r="J143" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K143" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L143" s="1"/>
       <c r="N143" s="11" t="str">
@@ -6440,12 +6442,12 @@
       </c>
       <c r="P143" s="1"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B144" s="12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C144" s="12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D144" s="12" t="s">
         <v>2</v>
@@ -6460,10 +6462,10 @@
       </c>
       <c r="H144" s="12"/>
       <c r="J144" s="12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K144" s="12" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="L144" s="1"/>
       <c r="N144" s="12" t="str">
@@ -6476,7 +6478,7 @@
       </c>
       <c r="P144" s="1"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B145" s="10" t="s">
         <v>73</v>
       </c>
@@ -6512,7 +6514,7 @@
       </c>
       <c r="P145" s="10"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B146" s="10" t="s">
         <v>74</v>
       </c>
@@ -6548,7 +6550,7 @@
       </c>
       <c r="P146" s="10"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B147" s="10" t="s">
         <v>147</v>
       </c>
@@ -6584,7 +6586,7 @@
       </c>
       <c r="P147" s="10"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B148" s="10" t="s">
         <v>118</v>
       </c>
@@ -6620,7 +6622,7 @@
       </c>
       <c r="P148" s="10"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B149" s="10" t="s">
         <v>119</v>
       </c>
@@ -6656,7 +6658,7 @@
       </c>
       <c r="P149" s="10"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B150" s="10" t="s">
         <v>120</v>
       </c>
@@ -6692,12 +6694,12 @@
       </c>
       <c r="P150" s="10"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B151" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C151" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D151" s="10" t="s">
         <v>2</v>
@@ -6712,10 +6714,10 @@
       </c>
       <c r="H151" s="10"/>
       <c r="J151" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="K151" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L151" s="10"/>
       <c r="N151" s="10" t="str">
@@ -6728,12 +6730,12 @@
       </c>
       <c r="P151" s="10"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B152" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C152" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D152" s="10" t="s">
         <v>2</v>
@@ -6748,10 +6750,10 @@
       </c>
       <c r="H152" s="10"/>
       <c r="J152" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="K152" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="L152" s="10"/>
       <c r="N152" s="10" t="str">
@@ -6764,12 +6766,12 @@
       </c>
       <c r="P152" s="10"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B153" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C153" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D153" s="10" t="s">
         <v>2</v>
@@ -6784,10 +6786,10 @@
       </c>
       <c r="H153" s="10"/>
       <c r="J153" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K153" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L153" s="10"/>
       <c r="N153" s="10" t="str">
@@ -6800,12 +6802,12 @@
       </c>
       <c r="P153" s="10"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B154" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C154" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D154" s="10" t="s">
         <v>2</v>
@@ -6820,10 +6822,10 @@
       </c>
       <c r="H154" s="10"/>
       <c r="J154" s="10" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K154" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L154" s="10"/>
       <c r="N154" s="10" t="str">
@@ -6836,12 +6838,12 @@
       </c>
       <c r="P154" s="10"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B155" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C155" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D155" s="10" t="s">
         <v>2</v>
@@ -6856,10 +6858,10 @@
       </c>
       <c r="H155" s="10"/>
       <c r="J155" s="10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K155" s="10" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="L155" s="10"/>
       <c r="N155" s="10" t="str">
@@ -6872,12 +6874,12 @@
       </c>
       <c r="P155" s="10"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B156" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C156" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D156" s="10" t="s">
         <v>2</v>
@@ -6892,10 +6894,10 @@
       </c>
       <c r="H156" s="10"/>
       <c r="J156" s="10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K156" s="10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="L156" s="10"/>
       <c r="N156" s="10" t="str">
@@ -6908,12 +6910,12 @@
       </c>
       <c r="P156" s="10"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B157" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C157" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D157" s="10" t="s">
         <v>2</v>
@@ -6928,10 +6930,10 @@
       </c>
       <c r="H157" s="10"/>
       <c r="J157" s="10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="K157" s="10" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L157" s="10"/>
       <c r="N157" s="10" t="str">
@@ -6944,12 +6946,12 @@
       </c>
       <c r="P157" s="10"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B158" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="C158" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="C158" s="10" t="s">
-        <v>238</v>
       </c>
       <c r="D158" s="10" t="s">
         <v>2</v>
@@ -6964,10 +6966,10 @@
       </c>
       <c r="H158" s="10"/>
       <c r="J158" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="K158" s="10" t="s">
         <v>237</v>
-      </c>
-      <c r="K158" s="10" t="s">
-        <v>238</v>
       </c>
       <c r="L158" s="10"/>
       <c r="N158" s="10" t="str">
@@ -6980,9 +6982,9 @@
       </c>
       <c r="P158" s="10"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B159" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C159" s="10" t="s">
         <v>7</v>
@@ -7000,7 +7002,7 @@
       </c>
       <c r="H159" s="10"/>
       <c r="J159" s="10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K159" s="10" t="s">
         <v>7</v>
@@ -7016,12 +7018,12 @@
       </c>
       <c r="P159" s="10"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B160" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C160" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D160" s="10" t="s">
         <v>2</v>
@@ -7036,10 +7038,10 @@
       </c>
       <c r="H160" s="10"/>
       <c r="J160" s="10" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K160" s="10" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="L160" s="10"/>
       <c r="N160" s="10" t="str">
@@ -7052,12 +7054,12 @@
       </c>
       <c r="P160" s="10"/>
     </row>
-    <row r="161" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B161" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C161" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D161" s="10" t="s">
         <v>2</v>
@@ -7072,10 +7074,10 @@
       </c>
       <c r="H161" s="10"/>
       <c r="J161" s="10" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K161" s="10" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L161" s="10"/>
       <c r="N161" s="10" t="str">
@@ -7088,12 +7090,12 @@
       </c>
       <c r="P161" s="10"/>
     </row>
-    <row r="162" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B162" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D162" s="10" t="s">
         <v>2</v>
@@ -7108,10 +7110,10 @@
       </c>
       <c r="H162" s="1"/>
       <c r="J162" s="10" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K162" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="L162" s="10"/>
       <c r="N162" s="10" t="str">
@@ -7124,7 +7126,7 @@
       </c>
       <c r="P162" s="10"/>
     </row>
-    <row r="165" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F165" s="13" t="s">
         <v>175</v>
       </c>
@@ -7136,41 +7138,41 @@
       <c r="O165" s="13"/>
       <c r="P165" s="13"/>
     </row>
-    <row r="166" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="F166" s="21" t="s">
+    <row r="166" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="F166" s="26" t="s">
         <v>170</v>
       </c>
-      <c r="G166" s="21"/>
-      <c r="H166" s="21"/>
-      <c r="N166" s="21" t="s">
+      <c r="G166" s="26"/>
+      <c r="H166" s="26"/>
+      <c r="N166" s="26" t="s">
         <v>172</v>
       </c>
-      <c r="O166" s="21"/>
-      <c r="P166" s="21"/>
-    </row>
-    <row r="169" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O166" s="26"/>
+      <c r="P166" s="26"/>
+    </row>
+    <row r="169" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B169" s="13" t="s">
         <v>152</v>
       </c>
       <c r="C169" s="13"/>
       <c r="D169" s="13"/>
-      <c r="F169" s="22" t="s">
+      <c r="F169" s="27" t="s">
         <v>171</v>
       </c>
-      <c r="G169" s="22"/>
-      <c r="H169" s="22"/>
-      <c r="J169" s="23" t="s">
+      <c r="G169" s="27"/>
+      <c r="H169" s="27"/>
+      <c r="J169" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="K169" s="23"/>
-      <c r="L169" s="23"/>
-      <c r="N169" s="22" t="s">
+      <c r="K169" s="28"/>
+      <c r="L169" s="28"/>
+      <c r="N169" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="O169" s="22"/>
-      <c r="P169" s="22"/>
-    </row>
-    <row r="170" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="O169" s="27"/>
+      <c r="P169" s="27"/>
+    </row>
+    <row r="170" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B170" s="10" t="s">
         <v>192</v>
       </c>
@@ -7212,7 +7214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B171" s="10" t="s">
         <v>63</v>
       </c>
@@ -7248,7 +7250,7 @@
       </c>
       <c r="P171" s="10"/>
     </row>
-    <row r="172" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B172" s="10" t="s">
         <v>64</v>
       </c>
@@ -7284,7 +7286,7 @@
       </c>
       <c r="P172" s="10"/>
     </row>
-    <row r="173" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B173" s="10" t="s">
         <v>65</v>
       </c>
@@ -7320,7 +7322,7 @@
       </c>
       <c r="P173" s="10"/>
     </row>
-    <row r="174" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B174" s="10" t="s">
         <v>66</v>
       </c>
@@ -7356,7 +7358,7 @@
       </c>
       <c r="P174" s="10"/>
     </row>
-    <row r="175" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B175" s="10" t="s">
         <v>67</v>
       </c>
@@ -7392,7 +7394,7 @@
       </c>
       <c r="P175" s="10"/>
     </row>
-    <row r="176" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B176" s="10" t="s">
         <v>68</v>
       </c>
@@ -7428,7 +7430,7 @@
       </c>
       <c r="P176" s="10"/>
     </row>
-    <row r="177" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B177" s="10" t="s">
         <v>69</v>
       </c>
@@ -7464,7 +7466,7 @@
       </c>
       <c r="P177" s="10"/>
     </row>
-    <row r="178" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B178" s="10" t="s">
         <v>70</v>
       </c>
@@ -7500,155 +7502,155 @@
       </c>
       <c r="P178" s="10"/>
     </row>
-    <row r="182" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B182" s="13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C182" s="13"/>
       <c r="D182" s="13"/>
     </row>
-    <row r="183" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B183" s="15">
+    <row r="183" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B183" s="29">
         <v>5</v>
       </c>
-      <c r="C183" s="16"/>
-      <c r="D183" s="17"/>
-    </row>
-    <row r="184" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B184" s="24">
+      <c r="C183" s="30"/>
+      <c r="D183" s="31"/>
+    </row>
+    <row r="184" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B184" s="32">
         <v>-3</v>
       </c>
-      <c r="C184" s="16"/>
-      <c r="D184" s="17"/>
-    </row>
-    <row r="185" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B185" s="15">
+      <c r="C184" s="30"/>
+      <c r="D184" s="31"/>
+    </row>
+    <row r="185" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B185" s="29">
         <v>0</v>
       </c>
-      <c r="C185" s="16"/>
-      <c r="D185" s="17"/>
-    </row>
-    <row r="188" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="C185" s="30"/>
+      <c r="D185" s="31"/>
+    </row>
+    <row r="188" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B188" s="13" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C188" s="13"/>
       <c r="D188" s="13"/>
     </row>
-    <row r="189" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B189" s="15">
+    <row r="189" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B189" s="29">
         <v>-5.5</v>
       </c>
-      <c r="C189" s="16"/>
-      <c r="D189" s="17"/>
-    </row>
-    <row r="190" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B190" s="15">
+      <c r="C189" s="30"/>
+      <c r="D189" s="31"/>
+    </row>
+    <row r="190" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B190" s="29">
         <v>3.3</v>
       </c>
-      <c r="C190" s="16"/>
-      <c r="D190" s="17"/>
-    </row>
-    <row r="191" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B191" s="15">
+      <c r="C190" s="30"/>
+      <c r="D190" s="31"/>
+    </row>
+    <row r="191" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="B191" s="29">
         <v>-1</v>
       </c>
-      <c r="C191" s="16"/>
-      <c r="D191" s="17"/>
-    </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C191" s="30"/>
+      <c r="D191" s="31"/>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B194" s="13" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C194" s="13"/>
       <c r="D194" s="13"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B195" s="15" t="b">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B195" s="29" t="b">
         <v>1</v>
       </c>
-      <c r="C195" s="16"/>
-      <c r="D195" s="17"/>
-    </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B196" s="15" t="b">
+      <c r="C195" s="30"/>
+      <c r="D195" s="31"/>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B196" s="29" t="b">
         <v>0</v>
       </c>
-      <c r="C196" s="16"/>
-      <c r="D196" s="17"/>
-    </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C196" s="30"/>
+      <c r="D196" s="31"/>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B199" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C199" s="13"/>
       <c r="D199" s="13"/>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B200" s="15" t="s">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B200" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="C200" s="30"/>
+      <c r="D200" s="31"/>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B201" s="29" t="s">
         <v>240</v>
       </c>
-      <c r="C200" s="16"/>
-      <c r="D200" s="17"/>
-    </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B201" s="15" t="s">
+      <c r="C201" s="30"/>
+      <c r="D201" s="31"/>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B202" s="29" t="s">
         <v>241</v>
       </c>
-      <c r="C201" s="16"/>
-      <c r="D201" s="17"/>
-    </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B202" s="15" t="s">
-        <v>242</v>
-      </c>
-      <c r="C202" s="16"/>
-      <c r="D202" s="17"/>
-    </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C202" s="30"/>
+      <c r="D202" s="31"/>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B205" s="13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C205" s="13"/>
       <c r="D205" s="13"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B206" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="C206" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="C206" s="10" t="s">
-        <v>244</v>
-      </c>
       <c r="D206" s="10" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B207" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C207" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D207" s="10"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B208" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C208" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D208" s="10"/>
     </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B211" s="13" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C211" s="13"/>
       <c r="D211" s="13"/>
     </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B212" s="10" t="s">
         <v>0</v>
       </c>
@@ -7659,7 +7661,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B213" s="10" t="s">
         <v>4</v>
       </c>
@@ -7668,7 +7670,7 @@
       </c>
       <c r="D213" s="10"/>
     </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B214" s="10" t="s">
         <v>6</v>
       </c>
@@ -7679,14 +7681,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B217" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C217" s="13"/>
       <c r="D217" s="13"/>
     </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B218" s="10" t="s">
         <v>8</v>
       </c>
@@ -7697,18 +7699,18 @@
         <v>150</v>
       </c>
     </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B219" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C219" s="10" t="s">
         <v>210</v>
-      </c>
-      <c r="C219" s="10" t="s">
-        <v>211</v>
       </c>
       <c r="D219" s="10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B220" s="10" t="s">
         <v>6</v>
       </c>
@@ -7717,359 +7719,298 @@
       </c>
       <c r="D220" s="10"/>
     </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B223" s="23" t="s">
-        <v>248</v>
-      </c>
-      <c r="C223" s="23"/>
-      <c r="D223" s="23"/>
-      <c r="E223" s="23"/>
-      <c r="F223" s="23"/>
-    </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B223" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="C223" s="28"/>
+      <c r="D223" s="28"/>
+      <c r="E223" s="28"/>
+      <c r="F223" s="28"/>
+    </row>
+    <row r="224" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B224" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C224" s="25" t="s">
+      <c r="C224" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="D224" s="26"/>
-      <c r="E224" s="26"/>
-      <c r="F224" s="27"/>
-    </row>
-    <row r="225" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D224" s="34"/>
+      <c r="E224" s="34"/>
+      <c r="F224" s="35"/>
+    </row>
+    <row r="225" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B225" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C225" s="15" t="s">
+      <c r="C225" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="D225" s="16"/>
-      <c r="E225" s="16"/>
-      <c r="F225" s="17"/>
-    </row>
-    <row r="226" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D225" s="30"/>
+      <c r="E225" s="30"/>
+      <c r="F225" s="31"/>
+    </row>
+    <row r="226" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B226" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C226" s="18" t="s">
+      <c r="C226" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="D226" s="19"/>
-      <c r="E226" s="19"/>
-      <c r="F226" s="20"/>
-    </row>
-    <row r="227" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D226" s="15"/>
+      <c r="E226" s="15"/>
+      <c r="F226" s="16"/>
+    </row>
+    <row r="227" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B227" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C227" s="14" t="s">
+      <c r="C227" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="D227" s="14"/>
-      <c r="E227" s="14"/>
-      <c r="F227" s="14"/>
-    </row>
-    <row r="228" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D227" s="36"/>
+      <c r="E227" s="36"/>
+      <c r="F227" s="36"/>
+    </row>
+    <row r="228" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B228" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C228" s="28" t="s">
-        <v>249</v>
-      </c>
-      <c r="D228" s="19"/>
-      <c r="E228" s="19"/>
-      <c r="F228" s="20"/>
-    </row>
-    <row r="233" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C228" s="14" t="s">
+        <v>248</v>
+      </c>
+      <c r="D228" s="15"/>
+      <c r="E228" s="15"/>
+      <c r="F228" s="16"/>
+    </row>
+    <row r="233" spans="2:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B233" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C233" s="13"/>
       <c r="D233" s="13"/>
     </row>
-    <row r="234" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B234" s="29" t="s">
+    <row r="234" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B234" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="C234" s="18"/>
+      <c r="D234" s="19"/>
+    </row>
+    <row r="235" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B235" s="20"/>
+      <c r="C235" s="21"/>
+      <c r="D235" s="22"/>
+    </row>
+    <row r="236" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B236" s="20"/>
+      <c r="C236" s="21"/>
+      <c r="D236" s="22"/>
+    </row>
+    <row r="237" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B237" s="20"/>
+      <c r="C237" s="21"/>
+      <c r="D237" s="22"/>
+    </row>
+    <row r="238" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B238" s="20"/>
+      <c r="C238" s="21"/>
+      <c r="D238" s="22"/>
+    </row>
+    <row r="239" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B239" s="20"/>
+      <c r="C239" s="21"/>
+      <c r="D239" s="22"/>
+    </row>
+    <row r="240" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B240" s="20"/>
+      <c r="C240" s="21"/>
+      <c r="D240" s="22"/>
+    </row>
+    <row r="241" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B241" s="20"/>
+      <c r="C241" s="21"/>
+      <c r="D241" s="22"/>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B242" s="20"/>
+      <c r="C242" s="21"/>
+      <c r="D242" s="22"/>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B243" s="20"/>
+      <c r="C243" s="21"/>
+      <c r="D243" s="22"/>
+    </row>
+    <row r="244" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B244" s="20"/>
+      <c r="C244" s="21"/>
+      <c r="D244" s="22"/>
+    </row>
+    <row r="245" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B245" s="23"/>
+      <c r="C245" s="24"/>
+      <c r="D245" s="25"/>
+    </row>
+    <row r="249" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B249" s="13" t="s">
         <v>261</v>
-      </c>
-      <c r="C234" s="30"/>
-      <c r="D234" s="31"/>
-    </row>
-    <row r="235" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B235" s="32"/>
-      <c r="C235" s="33"/>
-      <c r="D235" s="34"/>
-    </row>
-    <row r="236" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B236" s="32"/>
-      <c r="C236" s="33"/>
-      <c r="D236" s="34"/>
-    </row>
-    <row r="237" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B237" s="32"/>
-      <c r="C237" s="33"/>
-      <c r="D237" s="34"/>
-    </row>
-    <row r="238" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B238" s="32"/>
-      <c r="C238" s="33"/>
-      <c r="D238" s="34"/>
-    </row>
-    <row r="239" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B239" s="32"/>
-      <c r="C239" s="33"/>
-      <c r="D239" s="34"/>
-    </row>
-    <row r="240" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B240" s="32"/>
-      <c r="C240" s="33"/>
-      <c r="D240" s="34"/>
-    </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B241" s="32"/>
-      <c r="C241" s="33"/>
-      <c r="D241" s="34"/>
-    </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B242" s="32"/>
-      <c r="C242" s="33"/>
-      <c r="D242" s="34"/>
-    </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B243" s="32"/>
-      <c r="C243" s="33"/>
-      <c r="D243" s="34"/>
-    </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B244" s="32"/>
-      <c r="C244" s="33"/>
-      <c r="D244" s="34"/>
-    </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B245" s="35"/>
-      <c r="C245" s="36"/>
-      <c r="D245" s="37"/>
-    </row>
-    <row r="249" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B249" s="13" t="s">
-        <v>262</v>
       </c>
       <c r="C249" s="13"/>
       <c r="D249" s="13"/>
     </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B250" s="29" t="s">
+    <row r="250" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B250" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="C250" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="D250" s="19" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="251" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B251" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C251" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="D251" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="252" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B252" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C252" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="D252" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="253" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B253" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C253" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="D253" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="254" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B254" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C254" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="D254" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="255" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B255" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C255" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="D255" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="256" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B256" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C256" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="D256" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="257" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B257" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C257" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="D257" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="258" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B258" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C258" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="D258" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="259" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B259" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C259" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="D259" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="260" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B260" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="C260" s="21" t="s">
+        <v>260</v>
+      </c>
+      <c r="D260" s="22" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="261" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B261" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="C261" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="D261" s="25" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="265" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="B265" s="13" t="s">
         <v>263</v>
-      </c>
-      <c r="C250" s="30" t="s">
-        <v>261</v>
-      </c>
-      <c r="D250" s="31" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B251" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="C251" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="D251" s="34" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B252" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="C252" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="D252" s="34" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="253" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B253" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="C253" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="D253" s="34" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="254" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B254" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="C254" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="D254" s="34" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="255" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B255" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="C255" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="D255" s="34" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="256" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B256" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="C256" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="D256" s="34" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="257" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B257" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="C257" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="D257" s="34" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="258" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B258" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="C258" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="D258" s="34" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="259" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B259" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="C259" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="D259" s="34" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="260" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B260" s="32" t="s">
-        <v>261</v>
-      </c>
-      <c r="C260" s="33" t="s">
-        <v>261</v>
-      </c>
-      <c r="D260" s="34" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="261" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B261" s="35" t="s">
-        <v>261</v>
-      </c>
-      <c r="C261" s="36" t="s">
-        <v>261</v>
-      </c>
-      <c r="D261" s="37" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="265" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B265" s="13" t="s">
-        <v>264</v>
       </c>
       <c r="C265" s="13"/>
       <c r="D265" s="13"/>
     </row>
-    <row r="266" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="266" spans="2:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B266" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="C266" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="C266" s="10" t="s">
+      <c r="D266" s="1" t="s">
         <v>266</v>
-      </c>
-      <c r="D266" s="1" t="s">
-        <v>267</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="B265:D265"/>
-    <mergeCell ref="C228:F228"/>
-    <mergeCell ref="B233:D233"/>
-    <mergeCell ref="B234:D245"/>
-    <mergeCell ref="B249:D249"/>
-    <mergeCell ref="B250:D261"/>
-    <mergeCell ref="F166:H166"/>
-    <mergeCell ref="N166:P166"/>
-    <mergeCell ref="B169:D169"/>
-    <mergeCell ref="F169:H169"/>
-    <mergeCell ref="J169:L169"/>
-    <mergeCell ref="N169:P169"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="N125:P125"/>
-    <mergeCell ref="B128:D128"/>
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="J128:L128"/>
-    <mergeCell ref="N128:P128"/>
-    <mergeCell ref="N71:P71"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="N109:P109"/>
-    <mergeCell ref="B112:D112"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="J112:L112"/>
-    <mergeCell ref="N112:P112"/>
-    <mergeCell ref="N108:P108"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="J71:L71"/>
-    <mergeCell ref="B183:D183"/>
-    <mergeCell ref="B184:D184"/>
-    <mergeCell ref="B185:D185"/>
-    <mergeCell ref="B191:D191"/>
-    <mergeCell ref="C224:F224"/>
-    <mergeCell ref="B196:D196"/>
-    <mergeCell ref="B202:D202"/>
-    <mergeCell ref="B205:D205"/>
-    <mergeCell ref="B211:D211"/>
-    <mergeCell ref="B217:D217"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N51:P51"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="N67:P67"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="N68:P68"/>
-    <mergeCell ref="N52:P52"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="J55:L55"/>
-    <mergeCell ref="N55:P55"/>
     <mergeCell ref="N124:P124"/>
     <mergeCell ref="F124:H124"/>
     <mergeCell ref="N165:P165"/>
@@ -8086,6 +8027,67 @@
     <mergeCell ref="C226:F226"/>
     <mergeCell ref="C225:F225"/>
     <mergeCell ref="B182:D182"/>
+    <mergeCell ref="N67:P67"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="N68:P68"/>
+    <mergeCell ref="N52:P52"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="J55:L55"/>
+    <mergeCell ref="N55:P55"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N51:P51"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="B183:D183"/>
+    <mergeCell ref="B184:D184"/>
+    <mergeCell ref="B185:D185"/>
+    <mergeCell ref="B191:D191"/>
+    <mergeCell ref="C224:F224"/>
+    <mergeCell ref="B196:D196"/>
+    <mergeCell ref="B202:D202"/>
+    <mergeCell ref="B205:D205"/>
+    <mergeCell ref="B211:D211"/>
+    <mergeCell ref="B217:D217"/>
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="N71:P71"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="N109:P109"/>
+    <mergeCell ref="B112:D112"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="J112:L112"/>
+    <mergeCell ref="N112:P112"/>
+    <mergeCell ref="N108:P108"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="J71:L71"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="N125:P125"/>
+    <mergeCell ref="B128:D128"/>
+    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="J128:L128"/>
+    <mergeCell ref="N128:P128"/>
+    <mergeCell ref="F166:H166"/>
+    <mergeCell ref="N166:P166"/>
+    <mergeCell ref="B169:D169"/>
+    <mergeCell ref="F169:H169"/>
+    <mergeCell ref="J169:L169"/>
+    <mergeCell ref="N169:P169"/>
+    <mergeCell ref="B265:D265"/>
+    <mergeCell ref="C228:F228"/>
+    <mergeCell ref="B233:D233"/>
+    <mergeCell ref="B234:D245"/>
+    <mergeCell ref="B249:D249"/>
+    <mergeCell ref="B250:D261"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8097,22 +8099,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:H23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="6.83984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="23.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.26171875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="37.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="20.68359375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="24.26171875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="38" t="s">
         <v>84</v>
       </c>
@@ -8123,7 +8125,7 @@
       <c r="G3" s="38"/>
       <c r="H3" s="38"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="2" t="s">
         <v>75</v>
       </c>
@@ -8146,7 +8148,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="3" t="s">
         <v>77</v>
       </c>
@@ -8160,16 +8162,16 @@
         <v>189</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>184</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="3" t="s">
         <v>79</v>
       </c>
@@ -8183,16 +8185,16 @@
         <v>189</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G6" s="9" t="s">
         <v>184</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="3" t="s">
         <v>81</v>
       </c>
@@ -8206,16 +8208,16 @@
         <v>189</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G7" s="9" t="s">
         <v>184</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="3" t="s">
         <v>151</v>
       </c>
@@ -8229,16 +8231,16 @@
         <v>189</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G8" s="9" t="s">
         <v>184</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" s="3" t="s">
         <v>85</v>
       </c>
@@ -8252,16 +8254,16 @@
         <v>189</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G9" s="9" t="s">
         <v>184</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="3" t="s">
         <v>86</v>
       </c>
@@ -8275,16 +8277,16 @@
         <v>189</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>184</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="3" t="s">
         <v>96</v>
       </c>
@@ -8298,16 +8300,16 @@
         <v>189</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G11" s="9" t="s">
         <v>184</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="3" t="s">
         <v>97</v>
       </c>
@@ -8321,16 +8323,16 @@
         <v>189</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G12" s="9" t="s">
         <v>184</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="3" t="s">
         <v>123</v>
       </c>
@@ -8344,16 +8346,16 @@
         <v>189</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G13" s="9" t="s">
         <v>184</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="3" t="s">
         <v>124</v>
       </c>
@@ -8367,16 +8369,16 @@
         <v>189</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G14" s="9" t="s">
         <v>184</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="3" t="s">
         <v>125</v>
       </c>
@@ -8390,16 +8392,16 @@
         <v>189</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G15" s="9" t="s">
         <v>184</v>
       </c>
       <c r="H15" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="3" t="s">
         <v>126</v>
       </c>
@@ -8413,35 +8415,35 @@
         <v>189</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>184</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" s="3" t="s">
         <v>195</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="6"/>
       <c r="E17" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="38" t="s">
-        <v>196</v>
+        <v>334</v>
       </c>
       <c r="C20" s="38"/>
       <c r="D20" s="38"/>
@@ -8450,24 +8452,24 @@
       <c r="G20" s="38"/>
       <c r="H20" s="38"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="2"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="H21" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>199</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" s="2" t="s">
         <v>75</v>
       </c>
@@ -8490,7 +8492,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="3" t="s">
         <v>195</v>
       </c>
@@ -8520,30 +8522,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.15625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.15625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="16.68359375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="41" t="s">
         <v>90</v>
       </c>
       <c r="C3" s="41"/>
       <c r="E3" s="13" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="5" t="s">
         <v>91</v>
       </c>
@@ -8551,14 +8553,14 @@
         <v>94</v>
       </c>
       <c r="E4" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="F4" s="39" t="s">
         <v>304</v>
       </c>
-      <c r="F4" s="39" t="s">
-        <v>305</v>
-      </c>
       <c r="G4" s="40"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="5" t="s">
         <v>92</v>
       </c>
@@ -8566,37 +8568,37 @@
         <v>93</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F5" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="G5" s="40"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E6" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="F6" s="39" t="s">
         <v>306</v>
       </c>
-      <c r="G5" s="40"/>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E6" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="F6" s="39" t="s">
+      <c r="G6" s="40"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="E7" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="F7" s="39" t="s">
         <v>307</v>
       </c>
-      <c r="G6" s="40"/>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="E7" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="F7" s="39" t="s">
-        <v>308</v>
-      </c>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="E8" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G8" s="40"/>
     </row>

</xml_diff>

<commit_message>
Test failure because comparison with the default value is happened
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Datatype.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Datatype.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Berek\Desktop\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C62AD75-EF35-4501-A0EB-083141902416}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6675F90-92E6-4A63-96E0-0F4CA34782B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6165" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datatypes" sheetId="1" r:id="rId1"/>
@@ -38,30 +38,6 @@
   </authors>
   <commentList>
     <comment ref="D8" authorId="0" shapeId="0" xr:uid="{BFB3FD4F-B101-41AF-BB9A-03ACE301B314}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yury Molchan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Workaround to check all empty values</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{964788AE-23DA-4FCE-AA23-A1EF0DD19B4F}">
       <text>
         <r>
           <rPr>
@@ -589,12 +565,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="D269" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yury Molchan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Workaround to check all empty values</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="350">
   <si>
     <t>Integer</t>
   </si>
@@ -1609,15 +1609,61 @@
   <si>
     <t>Test evaluate evaluateTest</t>
   </si>
+  <si>
+    <t>_res_.person</t>
+  </si>
+  <si>
+    <t>=_res_.person.gender</t>
+  </si>
+  <si>
+    <t>_res_.person.gender</t>
+  </si>
+  <si>
+    <t>_res_.address</t>
+  </si>
+  <si>
+    <t>_res_.auto</t>
+  </si>
+  <si>
+    <t>personGender</t>
+  </si>
+  <si>
+    <t>_res_.person.bday</t>
+  </si>
+  <si>
+    <t>_res_.person.name</t>
+  </si>
+  <si>
+    <t>personBDay</t>
+  </si>
+  <si>
+    <t>personName</t>
+  </si>
+  <si>
+    <t>autoPower</t>
+  </si>
+  <si>
+    <t>_res_.auto.power</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>_res_.auto.model</t>
+  </si>
+  <si>
+    <t>autoModel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1825,9 +1871,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1846,13 +1891,39 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1882,32 +1953,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1921,8 +1966,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{85747B23-5477-4BE6-9006-95BD9824BD8B}"/>
+  <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1936,6 +1980,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2259,34 +2307,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:R266"/>
+  <dimension ref="B3:P312"/>
   <sheetViews>
     <sheetView topLeftCell="A127" workbookViewId="0">
       <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.68359375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.15625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="7.15625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="27.68359375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.41796875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="52.26171875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="7.15625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="24.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="19.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.68359375" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="7.109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="37.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="7.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="27.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="52.21875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="7.109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="24.5546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="13.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F3" s="13" t="s">
         <v>182</v>
       </c>
@@ -2298,41 +2346,36 @@
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F4" s="26" t="s">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F4" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="N4" s="26" t="s">
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="N4" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="F7" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
       <c r="N7" s="13" t="s">
         <v>138</v>
       </c>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
         <v>192</v>
       </c>
@@ -2340,17 +2383,6 @@
         <v>193</v>
       </c>
       <c r="D8" s="10">
-        <v>1</v>
-      </c>
-      <c r="F8" s="10" t="str">
-        <f t="shared" ref="F8:F41" si="0">"_res_." &amp; C8</f>
-        <v>_res_.test</v>
-      </c>
-      <c r="G8" s="10" t="str">
-        <f>C8</f>
-        <v>test</v>
-      </c>
-      <c r="H8" s="10">
         <v>1</v>
       </c>
       <c r="J8" s="10" t="s">
@@ -2370,7 +2402,7 @@
       </c>
       <c r="P8" s="10"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>10</v>
       </c>
@@ -2378,18 +2410,6 @@
         <v>21</v>
       </c>
       <c r="D9" s="10">
-        <v>1</v>
-      </c>
-      <c r="F9" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.byteValue</v>
-      </c>
-      <c r="G9" s="10" t="str">
-        <f t="shared" ref="G9:H22" si="2">C9</f>
-        <v>byteValue</v>
-      </c>
-      <c r="H9" s="10">
-        <f>D9</f>
         <v>1</v>
       </c>
       <c r="J9" s="10" t="s">
@@ -2409,7 +2429,7 @@
       </c>
       <c r="P9" s="10"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
         <v>11</v>
       </c>
@@ -2417,18 +2437,6 @@
         <v>22</v>
       </c>
       <c r="D10" s="10">
-        <v>2</v>
-      </c>
-      <c r="F10" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.shortValue</v>
-      </c>
-      <c r="G10" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>shortValue</v>
-      </c>
-      <c r="H10" s="10">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J10" s="10" t="s">
@@ -2448,7 +2456,7 @@
       </c>
       <c r="P10" s="10"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
         <v>0</v>
       </c>
@@ -2456,18 +2464,6 @@
         <v>23</v>
       </c>
       <c r="D11" s="10">
-        <v>3</v>
-      </c>
-      <c r="F11" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.intValue</v>
-      </c>
-      <c r="G11" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>intValue</v>
-      </c>
-      <c r="H11" s="10">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J11" s="10" t="s">
@@ -2487,7 +2483,7 @@
       </c>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
@@ -2495,18 +2491,6 @@
         <v>24</v>
       </c>
       <c r="D12" s="10">
-        <v>4</v>
-      </c>
-      <c r="F12" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.longValue</v>
-      </c>
-      <c r="G12" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>longValue</v>
-      </c>
-      <c r="H12" s="10">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J12" s="10" t="s">
@@ -2526,7 +2510,7 @@
       </c>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
@@ -2534,18 +2518,6 @@
         <v>25</v>
       </c>
       <c r="D13" s="10">
-        <v>5</v>
-      </c>
-      <c r="F13" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.floatValue</v>
-      </c>
-      <c r="G13" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>floatValue</v>
-      </c>
-      <c r="H13" s="10">
-        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J13" s="10" t="s">
@@ -2565,7 +2537,7 @@
       </c>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
         <v>8</v>
       </c>
@@ -2573,18 +2545,6 @@
         <v>26</v>
       </c>
       <c r="D14" s="10">
-        <v>6</v>
-      </c>
-      <c r="F14" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.doubleValue</v>
-      </c>
-      <c r="G14" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>doubleValue</v>
-      </c>
-      <c r="H14" s="10">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J14" s="10" t="s">
@@ -2604,7 +2564,7 @@
       </c>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
         <v>15</v>
       </c>
@@ -2613,18 +2573,6 @@
       </c>
       <c r="D15" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="F15" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.booleanValue</v>
-      </c>
-      <c r="G15" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>booleanValue</v>
-      </c>
-      <c r="H15" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>y</v>
       </c>
       <c r="J15" s="10" t="s">
         <v>15</v>
@@ -2643,7 +2591,7 @@
       </c>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
         <v>16</v>
       </c>
@@ -2652,18 +2600,6 @@
       </c>
       <c r="D16" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="F16" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.charValue</v>
-      </c>
-      <c r="G16" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>charValue</v>
-      </c>
-      <c r="H16" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>A</v>
       </c>
       <c r="J16" s="10" t="s">
         <v>16</v>
@@ -2682,7 +2618,7 @@
       </c>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
         <v>4</v>
       </c>
@@ -2691,18 +2627,6 @@
       </c>
       <c r="D17" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="F17" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.string</v>
-      </c>
-      <c r="G17" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>string</v>
-      </c>
-      <c r="H17" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>str</v>
       </c>
       <c r="J17" s="10" t="s">
         <v>4</v>
@@ -2721,7 +2645,7 @@
       </c>
       <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
         <v>1</v>
       </c>
@@ -2730,18 +2654,6 @@
       </c>
       <c r="D18" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="F18" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.date</v>
-      </c>
-      <c r="G18" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>date</v>
-      </c>
-      <c r="H18" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>03/31/2017</v>
       </c>
       <c r="J18" s="10" t="s">
         <v>1</v>
@@ -2760,7 +2672,7 @@
       </c>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="10" t="s">
         <v>299</v>
       </c>
@@ -2769,18 +2681,6 @@
       </c>
       <c r="D19" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="F19" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.localDate</v>
-      </c>
-      <c r="G19" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>localDate</v>
-      </c>
-      <c r="H19" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>03/31/2017</v>
       </c>
       <c r="J19" s="10" t="s">
         <v>299</v>
@@ -2799,7 +2699,7 @@
       </c>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="10" t="s">
         <v>308</v>
       </c>
@@ -2808,18 +2708,6 @@
       </c>
       <c r="D20" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="F20" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.localTime</v>
-      </c>
-      <c r="G20" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>localTime</v>
-      </c>
-      <c r="H20" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>21:30:25</v>
       </c>
       <c r="J20" s="10" t="s">
         <v>308</v>
@@ -2838,7 +2726,7 @@
       </c>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
         <v>309</v>
       </c>
@@ -2847,18 +2735,6 @@
       </c>
       <c r="D21" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="F21" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.localDateTime</v>
-      </c>
-      <c r="G21" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>localDateTime</v>
-      </c>
-      <c r="H21" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>9/20/2019 5:50 AM</v>
       </c>
       <c r="J21" s="10" t="s">
         <v>309</v>
@@ -2877,7 +2753,7 @@
       </c>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="10" t="s">
         <v>316</v>
       </c>
@@ -2886,18 +2762,6 @@
       </c>
       <c r="D22" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="F22" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.zonedDateTime</v>
-      </c>
-      <c r="G22" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>zonedDateTime</v>
-      </c>
-      <c r="H22" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>9/20/2019 5:50 AM America/Los_Angeles</v>
       </c>
       <c r="J22" s="10" t="s">
         <v>316</v>
@@ -2916,7 +2780,7 @@
       </c>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
         <v>328</v>
       </c>
@@ -2925,18 +2789,6 @@
       </c>
       <c r="D23" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="F23" s="12" t="str">
-        <f t="shared" ref="F23" si="4">"_res_." &amp; C23</f>
-        <v>_res_.instantDate</v>
-      </c>
-      <c r="G23" s="12" t="str">
-        <f t="shared" ref="G23" si="5">C23</f>
-        <v>instantDate</v>
-      </c>
-      <c r="H23" s="12" t="str">
-        <f t="shared" ref="H23" si="6">D23</f>
-        <v>9/20/2019 5:50 AM America/Los_Angeles</v>
       </c>
       <c r="J23" s="12" t="s">
         <v>328</v>
@@ -2955,7 +2807,7 @@
       </c>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="10" t="s">
         <v>17</v>
       </c>
@@ -2963,18 +2815,6 @@
         <v>220</v>
       </c>
       <c r="D24" s="10">
-        <v>7</v>
-      </c>
-      <c r="F24" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.bigInt</v>
-      </c>
-      <c r="G24" s="10" t="str">
-        <f>C24</f>
-        <v>bigInt</v>
-      </c>
-      <c r="H24" s="10">
-        <f>D24</f>
         <v>7</v>
       </c>
       <c r="J24" s="10" t="s">
@@ -2994,7 +2834,7 @@
       </c>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="10" t="s">
         <v>18</v>
       </c>
@@ -3002,18 +2842,6 @@
         <v>219</v>
       </c>
       <c r="D25" s="10">
-        <v>8</v>
-      </c>
-      <c r="F25" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.bigDec</v>
-      </c>
-      <c r="G25" s="10" t="str">
-        <f>C25</f>
-        <v>bigDec</v>
-      </c>
-      <c r="H25" s="10">
-        <f>D25</f>
         <v>8</v>
       </c>
       <c r="J25" s="10" t="s">
@@ -3033,7 +2861,7 @@
       </c>
       <c r="P25" s="10"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
         <v>145</v>
       </c>
@@ -3043,15 +2871,6 @@
       <c r="D26" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F26" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.col</v>
-      </c>
-      <c r="G26" s="10" t="str">
-        <f t="shared" ref="G26:H41" si="9">C26</f>
-        <v>col</v>
-      </c>
-      <c r="H26" s="10"/>
       <c r="J26" s="10" t="s">
         <v>145</v>
       </c>
@@ -3069,7 +2888,7 @@
       </c>
       <c r="P26" s="10"/>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" s="10" t="s">
         <v>33</v>
       </c>
@@ -3079,15 +2898,6 @@
       <c r="D27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.list</v>
-      </c>
-      <c r="G27" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>list</v>
-      </c>
-      <c r="H27" s="10"/>
       <c r="J27" s="10" t="s">
         <v>33</v>
       </c>
@@ -3105,7 +2915,7 @@
       </c>
       <c r="P27" s="10"/>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" s="10" t="s">
         <v>34</v>
       </c>
@@ -3115,15 +2925,6 @@
       <c r="D28" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.map</v>
-      </c>
-      <c r="G28" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>map</v>
-      </c>
-      <c r="H28" s="10"/>
       <c r="J28" s="10" t="s">
         <v>34</v>
       </c>
@@ -3141,7 +2942,7 @@
       </c>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" s="10" t="s">
         <v>37</v>
       </c>
@@ -3151,15 +2952,6 @@
       <c r="D29" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F29" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.set</v>
-      </c>
-      <c r="G29" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>set</v>
-      </c>
-      <c r="H29" s="10"/>
       <c r="J29" s="10" t="s">
         <v>37</v>
       </c>
@@ -3177,7 +2969,7 @@
       </c>
       <c r="P29" s="10"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
         <v>223</v>
       </c>
@@ -3187,15 +2979,6 @@
       <c r="D30" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F30" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.arrayList</v>
-      </c>
-      <c r="G30" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>arrayList</v>
-      </c>
-      <c r="H30" s="10"/>
       <c r="J30" s="10" t="s">
         <v>223</v>
       </c>
@@ -3213,7 +2996,7 @@
       </c>
       <c r="P30" s="10"/>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B31" s="10" t="s">
         <v>224</v>
       </c>
@@ -3223,15 +3006,6 @@
       <c r="D31" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.hashMap</v>
-      </c>
-      <c r="G31" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>hashMap</v>
-      </c>
-      <c r="H31" s="10"/>
       <c r="J31" s="10" t="s">
         <v>224</v>
       </c>
@@ -3249,7 +3023,7 @@
       </c>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
         <v>225</v>
       </c>
@@ -3259,15 +3033,6 @@
       <c r="D32" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F32" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.hashSet</v>
-      </c>
-      <c r="G32" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>hashSet</v>
-      </c>
-      <c r="H32" s="10"/>
       <c r="J32" s="10" t="s">
         <v>225</v>
       </c>
@@ -3285,7 +3050,7 @@
       </c>
       <c r="P32" s="10"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33" s="10" t="s">
         <v>249</v>
       </c>
@@ -3294,18 +3059,6 @@
       </c>
       <c r="D33" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="F33" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.roudingMode</v>
-      </c>
-      <c r="G33" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>roudingMode</v>
-      </c>
-      <c r="H33" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>HALF_EVEN</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>249</v>
@@ -3324,7 +3077,7 @@
       </c>
       <c r="P33" s="10"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B34" s="10" t="s">
         <v>192</v>
       </c>
@@ -3332,18 +3085,6 @@
         <v>255</v>
       </c>
       <c r="D34" s="10">
-        <v>10.1</v>
-      </c>
-      <c r="F34" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.dv</v>
-      </c>
-      <c r="G34" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>dv</v>
-      </c>
-      <c r="H34" s="10">
-        <f t="shared" si="9"/>
         <v>10.1</v>
       </c>
       <c r="J34" s="10" t="s">
@@ -3363,7 +3104,7 @@
       </c>
       <c r="P34" s="10"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
         <v>270</v>
       </c>
@@ -3371,18 +3112,6 @@
         <v>273</v>
       </c>
       <c r="D35" s="10">
-        <v>-3</v>
-      </c>
-      <c r="F35" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.intAlias</v>
-      </c>
-      <c r="G35" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>intAlias</v>
-      </c>
-      <c r="H35" s="10">
-        <f t="shared" si="9"/>
         <v>-3</v>
       </c>
       <c r="J35" s="10" t="s">
@@ -3404,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
         <v>271</v>
       </c>
@@ -3412,18 +3141,6 @@
         <v>274</v>
       </c>
       <c r="D36" s="10">
-        <v>3.3</v>
-      </c>
-      <c r="F36" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.doubleAlias</v>
-      </c>
-      <c r="G36" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>doubleAlias</v>
-      </c>
-      <c r="H36" s="10">
-        <f t="shared" si="9"/>
         <v>3.3</v>
       </c>
       <c r="J36" s="10" t="s">
@@ -3443,7 +3160,7 @@
       </c>
       <c r="P36" s="10"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B37" s="10" t="s">
         <v>272</v>
       </c>
@@ -3452,18 +3169,6 @@
       </c>
       <c r="D37" s="10" t="s">
         <v>276</v>
-      </c>
-      <c r="F37" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.boolAlias</v>
-      </c>
-      <c r="G37" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>boolAlias</v>
-      </c>
-      <c r="H37" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>n</v>
       </c>
       <c r="J37" s="10" t="s">
         <v>272</v>
@@ -3482,7 +3187,7 @@
       </c>
       <c r="P37" s="10"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B38" s="10" t="s">
         <v>242</v>
       </c>
@@ -3491,18 +3196,6 @@
       </c>
       <c r="D38" s="10" t="s">
         <v>239</v>
-      </c>
-      <c r="F38" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.gender</v>
-      </c>
-      <c r="G38" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>gender</v>
-      </c>
-      <c r="H38" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>Male</v>
       </c>
       <c r="J38" s="10" t="s">
         <v>242</v>
@@ -3521,7 +3214,7 @@
       </c>
       <c r="P38" s="10"/>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B39" s="10" t="s">
         <v>6</v>
       </c>
@@ -3531,15 +3224,6 @@
       <c r="D39" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.person</v>
-      </c>
-      <c r="G39" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>person</v>
-      </c>
-      <c r="H39" s="10"/>
       <c r="J39" s="10" t="s">
         <v>6</v>
       </c>
@@ -3557,7 +3241,7 @@
       </c>
       <c r="P39" s="10"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
         <v>209</v>
       </c>
@@ -3567,15 +3251,6 @@
       <c r="D40" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F40" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.auto</v>
-      </c>
-      <c r="G40" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>auto</v>
-      </c>
-      <c r="H40" s="10"/>
       <c r="J40" s="10" t="s">
         <v>209</v>
       </c>
@@ -3593,7 +3268,7 @@
       </c>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B41" s="10" t="s">
         <v>234</v>
       </c>
@@ -3603,15 +3278,6 @@
       <c r="D41" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F41" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.address</v>
-      </c>
-      <c r="G41" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>address</v>
-      </c>
-      <c r="H41" s="10"/>
       <c r="J41" s="10" t="s">
         <v>234</v>
       </c>
@@ -3629,76 +3295,15 @@
       </c>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F42" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="H42" s="10">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F43" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H43" s="10"/>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F44" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="H44" s="10">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F45" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="H45" s="10"/>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F46" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F47" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="H47" s="10"/>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F48" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="H48" s="10"/>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.3"/>
+    <row r="49"/>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F51" s="13" t="s">
         <v>181</v>
       </c>
@@ -3710,41 +3315,41 @@
       <c r="O51" s="13"/>
       <c r="P51" s="13"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F52" s="26" t="s">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F52" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="G52" s="26"/>
-      <c r="H52" s="26"/>
-      <c r="N52" s="26" t="s">
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="N52" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="O52" s="26"/>
-      <c r="P52" s="26"/>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O52" s="21"/>
+      <c r="P52" s="21"/>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B55" s="13" t="s">
         <v>88</v>
       </c>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
-      <c r="F55" s="27" t="s">
+      <c r="F55" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="G55" s="27"/>
-      <c r="H55" s="27"/>
-      <c r="J55" s="28" t="s">
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
+      <c r="J55" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="K55" s="28"/>
-      <c r="L55" s="28"/>
-      <c r="N55" s="27" t="s">
+      <c r="K55" s="23"/>
+      <c r="L55" s="23"/>
+      <c r="N55" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="O55" s="27"/>
-      <c r="P55" s="27"/>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O55" s="22"/>
+      <c r="P55" s="22"/>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B56" s="10" t="s">
         <v>192</v>
       </c>
@@ -3786,7 +3391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B57" s="10" t="s">
         <v>39</v>
       </c>
@@ -3827,7 +3432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
         <v>40</v>
       </c>
@@ -3868,7 +3473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B59" s="10" t="s">
         <v>41</v>
       </c>
@@ -3909,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B60" s="10" t="s">
         <v>42</v>
       </c>
@@ -3950,7 +3555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B61" s="10" t="s">
         <v>43</v>
       </c>
@@ -3991,7 +3596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B62" s="10" t="s">
         <v>44</v>
       </c>
@@ -4032,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B63" s="10" t="s">
         <v>46</v>
       </c>
@@ -4073,7 +3678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B64" s="10" t="s">
         <v>45</v>
       </c>
@@ -4112,7 +3717,7 @@
       </c>
       <c r="P64" s="10"/>
     </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F67" s="13" t="s">
         <v>179</v>
       </c>
@@ -4124,19 +3729,19 @@
       <c r="O67" s="13"/>
       <c r="P67" s="13"/>
     </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F68" s="26" t="s">
+    <row r="68" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F68" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="G68" s="26"/>
-      <c r="H68" s="26"/>
-      <c r="N68" s="26" t="s">
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="N68" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="O68" s="26"/>
-      <c r="P68" s="26"/>
-    </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O68" s="21"/>
+      <c r="P68" s="21"/>
+    </row>
+    <row r="71" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B71" s="13" t="s">
         <v>143</v>
       </c>
@@ -4147,18 +3752,18 @@
       </c>
       <c r="G71" s="13"/>
       <c r="H71" s="13"/>
-      <c r="J71" s="28" t="s">
+      <c r="J71" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="K71" s="28"/>
-      <c r="L71" s="28"/>
+      <c r="K71" s="23"/>
+      <c r="L71" s="23"/>
       <c r="N71" s="13" t="s">
         <v>159</v>
       </c>
       <c r="O71" s="13"/>
       <c r="P71" s="13"/>
     </row>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B72" s="10" t="s">
         <v>192</v>
       </c>
@@ -4200,7 +3805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B73" s="10" t="s">
         <v>98</v>
       </c>
@@ -4239,7 +3844,7 @@
       </c>
       <c r="P73" s="10"/>
     </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B74" s="10" t="s">
         <v>99</v>
       </c>
@@ -4278,7 +3883,7 @@
       </c>
       <c r="P74" s="10"/>
     </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B75" s="10" t="s">
         <v>100</v>
       </c>
@@ -4317,7 +3922,7 @@
       </c>
       <c r="P75" s="10"/>
     </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B76" s="10" t="s">
         <v>101</v>
       </c>
@@ -4356,7 +3961,7 @@
       </c>
       <c r="P76" s="10"/>
     </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B77" s="10" t="s">
         <v>102</v>
       </c>
@@ -4395,7 +4000,7 @@
       </c>
       <c r="P77" s="10"/>
     </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B78" s="10" t="s">
         <v>103</v>
       </c>
@@ -4434,7 +4039,7 @@
       </c>
       <c r="P78" s="10"/>
     </row>
-    <row r="79" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B79" s="10" t="s">
         <v>104</v>
       </c>
@@ -4473,7 +4078,7 @@
       </c>
       <c r="P79" s="10"/>
     </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B80" s="10" t="s">
         <v>105</v>
       </c>
@@ -4512,7 +4117,7 @@
       </c>
       <c r="P80" s="10"/>
     </row>
-    <row r="81" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B81" s="10" t="s">
         <v>58</v>
       </c>
@@ -4551,7 +4156,7 @@
       </c>
       <c r="P81" s="10"/>
     </row>
-    <row r="82" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B82" s="10" t="s">
         <v>59</v>
       </c>
@@ -4590,7 +4195,7 @@
       </c>
       <c r="P82" s="1"/>
     </row>
-    <row r="83" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B83" s="11" t="s">
         <v>319</v>
       </c>
@@ -4629,7 +4234,7 @@
       </c>
       <c r="P83" s="1"/>
     </row>
-    <row r="84" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B84" s="11" t="s">
         <v>320</v>
       </c>
@@ -4668,7 +4273,7 @@
       </c>
       <c r="P84" s="1"/>
     </row>
-    <row r="85" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B85" s="11" t="s">
         <v>321</v>
       </c>
@@ -4707,7 +4312,7 @@
       </c>
       <c r="P85" s="1"/>
     </row>
-    <row r="86" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B86" s="11" t="s">
         <v>322</v>
       </c>
@@ -4746,7 +4351,7 @@
       </c>
       <c r="P86" s="1"/>
     </row>
-    <row r="87" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B87" s="12" t="s">
         <v>330</v>
       </c>
@@ -4786,7 +4391,7 @@
       </c>
       <c r="P87" s="1"/>
     </row>
-    <row r="88" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B88" s="10" t="s">
         <v>60</v>
       </c>
@@ -4825,7 +4430,7 @@
       </c>
       <c r="P88" s="10"/>
     </row>
-    <row r="89" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B89" s="10" t="s">
         <v>61</v>
       </c>
@@ -4864,7 +4469,7 @@
       </c>
       <c r="P89" s="10"/>
     </row>
-    <row r="90" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B90" s="10" t="s">
         <v>148</v>
       </c>
@@ -4900,7 +4505,7 @@
       </c>
       <c r="P90" s="10"/>
     </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B91" s="10" t="s">
         <v>208</v>
       </c>
@@ -4936,7 +4541,7 @@
       </c>
       <c r="P91" s="10"/>
     </row>
-    <row r="92" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B92" s="10" t="s">
         <v>116</v>
       </c>
@@ -4972,7 +4577,7 @@
       </c>
       <c r="P92" s="10"/>
     </row>
-    <row r="93" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B93" s="10" t="s">
         <v>117</v>
       </c>
@@ -5008,7 +4613,7 @@
       </c>
       <c r="P93" s="10"/>
     </row>
-    <row r="94" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B94" s="10" t="s">
         <v>208</v>
       </c>
@@ -5044,7 +4649,7 @@
       </c>
       <c r="P94" s="10"/>
     </row>
-    <row r="95" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B95" s="10" t="s">
         <v>229</v>
       </c>
@@ -5080,7 +4685,7 @@
       </c>
       <c r="P95" s="10"/>
     </row>
-    <row r="96" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B96" s="10" t="s">
         <v>230</v>
       </c>
@@ -5116,7 +4721,7 @@
       </c>
       <c r="P96" s="10"/>
     </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B97" s="10" t="s">
         <v>277</v>
       </c>
@@ -5155,7 +4760,7 @@
       </c>
       <c r="P97" s="10"/>
     </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B98" s="10" t="s">
         <v>278</v>
       </c>
@@ -5194,7 +4799,7 @@
       </c>
       <c r="P98" s="10"/>
     </row>
-    <row r="99" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B99" s="10" t="s">
         <v>279</v>
       </c>
@@ -5233,7 +4838,7 @@
       </c>
       <c r="P99" s="10"/>
     </row>
-    <row r="100" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B100" s="10" t="s">
         <v>244</v>
       </c>
@@ -5272,7 +4877,7 @@
       </c>
       <c r="P100" s="10"/>
     </row>
-    <row r="101" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B101" s="10" t="s">
         <v>235</v>
       </c>
@@ -5308,7 +4913,7 @@
       </c>
       <c r="P101" s="10"/>
     </row>
-    <row r="102" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B102" s="10" t="s">
         <v>211</v>
       </c>
@@ -5344,7 +4949,7 @@
       </c>
       <c r="P102" s="10"/>
     </row>
-    <row r="103" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B103" s="10" t="s">
         <v>212</v>
       </c>
@@ -5380,7 +4985,7 @@
       </c>
       <c r="P103" s="10"/>
     </row>
-    <row r="104" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B104" s="10" t="s">
         <v>252</v>
       </c>
@@ -5419,7 +5024,7 @@
       </c>
       <c r="P104" s="10"/>
     </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B105" s="10" t="s">
         <v>256</v>
       </c>
@@ -5458,7 +5063,7 @@
       </c>
       <c r="P105" s="10"/>
     </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F108" s="13" t="s">
         <v>177</v>
       </c>
@@ -5470,19 +5075,19 @@
       <c r="O108" s="13"/>
       <c r="P108" s="13"/>
     </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F109" s="26" t="s">
+    <row r="109" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F109" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="G109" s="26"/>
-      <c r="H109" s="26"/>
-      <c r="N109" s="26" t="s">
+      <c r="G109" s="21"/>
+      <c r="H109" s="21"/>
+      <c r="N109" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="O109" s="26"/>
-      <c r="P109" s="26"/>
-    </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O109" s="21"/>
+      <c r="P109" s="21"/>
+    </row>
+    <row r="112" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B112" s="13" t="s">
         <v>144</v>
       </c>
@@ -5493,18 +5098,18 @@
       </c>
       <c r="G112" s="13"/>
       <c r="H112" s="13"/>
-      <c r="J112" s="28" t="s">
+      <c r="J112" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="K112" s="28"/>
-      <c r="L112" s="28"/>
-      <c r="N112" s="27" t="s">
+      <c r="K112" s="23"/>
+      <c r="L112" s="23"/>
+      <c r="N112" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="O112" s="27"/>
-      <c r="P112" s="27"/>
-    </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O112" s="22"/>
+      <c r="P112" s="22"/>
+    </row>
+    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B113" s="10" t="s">
         <v>192</v>
       </c>
@@ -5546,7 +5151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B114" s="10" t="s">
         <v>47</v>
       </c>
@@ -5584,7 +5189,7 @@
       </c>
       <c r="P114" s="10"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B115" s="10" t="s">
         <v>48</v>
       </c>
@@ -5622,7 +5227,7 @@
       </c>
       <c r="P115" s="10"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B116" s="10" t="s">
         <v>49</v>
       </c>
@@ -5660,7 +5265,7 @@
       </c>
       <c r="P116" s="10"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B117" s="10" t="s">
         <v>50</v>
       </c>
@@ -5698,7 +5303,7 @@
       </c>
       <c r="P117" s="10"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B118" s="10" t="s">
         <v>51</v>
       </c>
@@ -5736,7 +5341,7 @@
       </c>
       <c r="P118" s="10"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B119" s="10" t="s">
         <v>52</v>
       </c>
@@ -5774,7 +5379,7 @@
       </c>
       <c r="P119" s="10"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B120" s="10" t="s">
         <v>53</v>
       </c>
@@ -5812,7 +5417,7 @@
       </c>
       <c r="P120" s="10"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B121" s="10" t="s">
         <v>54</v>
       </c>
@@ -5850,7 +5455,7 @@
       </c>
       <c r="P121" s="10"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F124" s="13" t="s">
         <v>168</v>
       </c>
@@ -5862,19 +5467,19 @@
       <c r="O124" s="13"/>
       <c r="P124" s="13"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F125" s="26" t="s">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F125" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="G125" s="26"/>
-      <c r="H125" s="26"/>
-      <c r="N125" s="26" t="s">
+      <c r="G125" s="21"/>
+      <c r="H125" s="21"/>
+      <c r="N125" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="O125" s="26"/>
-      <c r="P125" s="26"/>
-    </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O125" s="21"/>
+      <c r="P125" s="21"/>
+    </row>
+    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B128" s="13" t="s">
         <v>155</v>
       </c>
@@ -5885,18 +5490,18 @@
       </c>
       <c r="G128" s="13"/>
       <c r="H128" s="13"/>
-      <c r="J128" s="28" t="s">
+      <c r="J128" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="K128" s="28"/>
-      <c r="L128" s="28"/>
+      <c r="K128" s="23"/>
+      <c r="L128" s="23"/>
       <c r="N128" s="13" t="s">
         <v>191</v>
       </c>
       <c r="O128" s="13"/>
       <c r="P128" s="13"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B129" s="10" t="s">
         <v>192</v>
       </c>
@@ -5938,7 +5543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B130" s="10" t="s">
         <v>106</v>
       </c>
@@ -5974,7 +5579,7 @@
       </c>
       <c r="P130" s="10"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B131" s="10" t="s">
         <v>107</v>
       </c>
@@ -6010,7 +5615,7 @@
       </c>
       <c r="P131" s="10"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B132" s="10" t="s">
         <v>108</v>
       </c>
@@ -6046,7 +5651,7 @@
       </c>
       <c r="P132" s="10"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B133" s="10" t="s">
         <v>109</v>
       </c>
@@ -6082,7 +5687,7 @@
       </c>
       <c r="P133" s="10"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B134" s="10" t="s">
         <v>110</v>
       </c>
@@ -6118,7 +5723,7 @@
       </c>
       <c r="P134" s="10"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B135" s="10" t="s">
         <v>111</v>
       </c>
@@ -6154,7 +5759,7 @@
       </c>
       <c r="P135" s="10"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B136" s="10" t="s">
         <v>112</v>
       </c>
@@ -6190,7 +5795,7 @@
       </c>
       <c r="P136" s="10"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B137" s="10" t="s">
         <v>113</v>
       </c>
@@ -6226,7 +5831,7 @@
       </c>
       <c r="P137" s="10"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B138" s="10" t="s">
         <v>71</v>
       </c>
@@ -6262,7 +5867,7 @@
       </c>
       <c r="P138" s="10"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B139" s="10" t="s">
         <v>72</v>
       </c>
@@ -6298,7 +5903,7 @@
       </c>
       <c r="P139" s="1"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B140" s="11" t="s">
         <v>324</v>
       </c>
@@ -6334,7 +5939,7 @@
       </c>
       <c r="P140" s="1"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B141" s="11" t="s">
         <v>325</v>
       </c>
@@ -6370,7 +5975,7 @@
       </c>
       <c r="P141" s="1"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B142" s="11" t="s">
         <v>326</v>
       </c>
@@ -6406,7 +6011,7 @@
       </c>
       <c r="P142" s="1"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B143" s="11" t="s">
         <v>327</v>
       </c>
@@ -6442,7 +6047,7 @@
       </c>
       <c r="P143" s="1"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B144" s="12" t="s">
         <v>332</v>
       </c>
@@ -6478,7 +6083,7 @@
       </c>
       <c r="P144" s="1"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B145" s="10" t="s">
         <v>73</v>
       </c>
@@ -6514,7 +6119,7 @@
       </c>
       <c r="P145" s="10"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B146" s="10" t="s">
         <v>74</v>
       </c>
@@ -6550,7 +6155,7 @@
       </c>
       <c r="P146" s="10"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B147" s="10" t="s">
         <v>147</v>
       </c>
@@ -6586,7 +6191,7 @@
       </c>
       <c r="P147" s="10"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B148" s="10" t="s">
         <v>118</v>
       </c>
@@ -6622,7 +6227,7 @@
       </c>
       <c r="P148" s="10"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B149" s="10" t="s">
         <v>119</v>
       </c>
@@ -6658,7 +6263,7 @@
       </c>
       <c r="P149" s="10"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B150" s="10" t="s">
         <v>120</v>
       </c>
@@ -6694,7 +6299,7 @@
       </c>
       <c r="P150" s="10"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B151" s="10" t="s">
         <v>231</v>
       </c>
@@ -6730,7 +6335,7 @@
       </c>
       <c r="P151" s="10"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B152" s="10" t="s">
         <v>232</v>
       </c>
@@ -6766,7 +6371,7 @@
       </c>
       <c r="P152" s="10"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B153" s="10" t="s">
         <v>233</v>
       </c>
@@ -6802,7 +6407,7 @@
       </c>
       <c r="P153" s="10"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B154" s="10" t="s">
         <v>283</v>
       </c>
@@ -6838,7 +6443,7 @@
       </c>
       <c r="P154" s="10"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B155" s="10" t="s">
         <v>284</v>
       </c>
@@ -6874,7 +6479,7 @@
       </c>
       <c r="P155" s="10"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B156" s="10" t="s">
         <v>285</v>
       </c>
@@ -6910,7 +6515,7 @@
       </c>
       <c r="P156" s="10"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B157" s="10" t="s">
         <v>245</v>
       </c>
@@ -6946,7 +6551,7 @@
       </c>
       <c r="P157" s="10"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B158" s="10" t="s">
         <v>236</v>
       </c>
@@ -6982,7 +6587,7 @@
       </c>
       <c r="P158" s="10"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B159" s="10" t="s">
         <v>213</v>
       </c>
@@ -7018,7 +6623,7 @@
       </c>
       <c r="P159" s="10"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B160" s="10" t="s">
         <v>214</v>
       </c>
@@ -7054,7 +6659,7 @@
       </c>
       <c r="P160" s="10"/>
     </row>
-    <row r="161" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B161" s="10" t="s">
         <v>254</v>
       </c>
@@ -7090,7 +6695,7 @@
       </c>
       <c r="P161" s="10"/>
     </row>
-    <row r="162" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B162" s="10" t="s">
         <v>258</v>
       </c>
@@ -7126,7 +6731,7 @@
       </c>
       <c r="P162" s="10"/>
     </row>
-    <row r="165" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F165" s="13" t="s">
         <v>175</v>
       </c>
@@ -7138,41 +6743,41 @@
       <c r="O165" s="13"/>
       <c r="P165" s="13"/>
     </row>
-    <row r="166" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F166" s="26" t="s">
+    <row r="166" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F166" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="G166" s="26"/>
-      <c r="H166" s="26"/>
-      <c r="N166" s="26" t="s">
+      <c r="G166" s="21"/>
+      <c r="H166" s="21"/>
+      <c r="N166" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="O166" s="26"/>
-      <c r="P166" s="26"/>
-    </row>
-    <row r="169" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O166" s="21"/>
+      <c r="P166" s="21"/>
+    </row>
+    <row r="169" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B169" s="13" t="s">
         <v>152</v>
       </c>
       <c r="C169" s="13"/>
       <c r="D169" s="13"/>
-      <c r="F169" s="27" t="s">
+      <c r="F169" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="G169" s="27"/>
-      <c r="H169" s="27"/>
-      <c r="J169" s="28" t="s">
+      <c r="G169" s="22"/>
+      <c r="H169" s="22"/>
+      <c r="J169" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="K169" s="28"/>
-      <c r="L169" s="28"/>
-      <c r="N169" s="27" t="s">
+      <c r="K169" s="23"/>
+      <c r="L169" s="23"/>
+      <c r="N169" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="O169" s="27"/>
-      <c r="P169" s="27"/>
-    </row>
-    <row r="170" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O169" s="22"/>
+      <c r="P169" s="22"/>
+    </row>
+    <row r="170" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B170" s="10" t="s">
         <v>192</v>
       </c>
@@ -7214,7 +6819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B171" s="10" t="s">
         <v>63</v>
       </c>
@@ -7250,7 +6855,7 @@
       </c>
       <c r="P171" s="10"/>
     </row>
-    <row r="172" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B172" s="10" t="s">
         <v>64</v>
       </c>
@@ -7286,7 +6891,7 @@
       </c>
       <c r="P172" s="10"/>
     </row>
-    <row r="173" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B173" s="10" t="s">
         <v>65</v>
       </c>
@@ -7322,7 +6927,7 @@
       </c>
       <c r="P173" s="10"/>
     </row>
-    <row r="174" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B174" s="10" t="s">
         <v>66</v>
       </c>
@@ -7358,7 +6963,7 @@
       </c>
       <c r="P174" s="10"/>
     </row>
-    <row r="175" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B175" s="10" t="s">
         <v>67</v>
       </c>
@@ -7394,7 +6999,7 @@
       </c>
       <c r="P175" s="10"/>
     </row>
-    <row r="176" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B176" s="10" t="s">
         <v>68</v>
       </c>
@@ -7430,7 +7035,7 @@
       </c>
       <c r="P176" s="10"/>
     </row>
-    <row r="177" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B177" s="10" t="s">
         <v>69</v>
       </c>
@@ -7466,7 +7071,7 @@
       </c>
       <c r="P177" s="10"/>
     </row>
-    <row r="178" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B178" s="10" t="s">
         <v>70</v>
       </c>
@@ -7502,119 +7107,119 @@
       </c>
       <c r="P178" s="10"/>
     </row>
-    <row r="182" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B182" s="13" t="s">
         <v>267</v>
       </c>
       <c r="C182" s="13"/>
       <c r="D182" s="13"/>
     </row>
-    <row r="183" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B183" s="29">
+    <row r="183" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B183" s="15">
         <v>5</v>
       </c>
-      <c r="C183" s="30"/>
-      <c r="D183" s="31"/>
-    </row>
-    <row r="184" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B184" s="32">
+      <c r="C183" s="16"/>
+      <c r="D183" s="17"/>
+    </row>
+    <row r="184" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B184" s="24">
         <v>-3</v>
       </c>
-      <c r="C184" s="30"/>
-      <c r="D184" s="31"/>
-    </row>
-    <row r="185" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B185" s="29">
+      <c r="C184" s="16"/>
+      <c r="D184" s="17"/>
+    </row>
+    <row r="185" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B185" s="15">
         <v>0</v>
       </c>
-      <c r="C185" s="30"/>
-      <c r="D185" s="31"/>
-    </row>
-    <row r="188" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="C185" s="16"/>
+      <c r="D185" s="17"/>
+    </row>
+    <row r="188" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B188" s="13" t="s">
         <v>268</v>
       </c>
       <c r="C188" s="13"/>
       <c r="D188" s="13"/>
     </row>
-    <row r="189" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B189" s="29">
+    <row r="189" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B189" s="15">
         <v>-5.5</v>
       </c>
-      <c r="C189" s="30"/>
-      <c r="D189" s="31"/>
-    </row>
-    <row r="190" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B190" s="29">
+      <c r="C189" s="16"/>
+      <c r="D189" s="17"/>
+    </row>
+    <row r="190" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B190" s="15">
         <v>3.3</v>
       </c>
-      <c r="C190" s="30"/>
-      <c r="D190" s="31"/>
-    </row>
-    <row r="191" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B191" s="29">
+      <c r="C190" s="16"/>
+      <c r="D190" s="17"/>
+    </row>
+    <row r="191" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B191" s="15">
         <v>-1</v>
       </c>
-      <c r="C191" s="30"/>
-      <c r="D191" s="31"/>
-    </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C191" s="16"/>
+      <c r="D191" s="17"/>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B194" s="13" t="s">
         <v>269</v>
       </c>
       <c r="C194" s="13"/>
       <c r="D194" s="13"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B195" s="29" t="b">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B195" s="15" t="b">
         <v>1</v>
       </c>
-      <c r="C195" s="30"/>
-      <c r="D195" s="31"/>
-    </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B196" s="29" t="b">
+      <c r="C195" s="16"/>
+      <c r="D195" s="17"/>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B196" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="C196" s="30"/>
-      <c r="D196" s="31"/>
-    </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C196" s="16"/>
+      <c r="D196" s="17"/>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B199" s="13" t="s">
         <v>238</v>
       </c>
       <c r="C199" s="13"/>
       <c r="D199" s="13"/>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B200" s="29" t="s">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B200" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="C200" s="30"/>
-      <c r="D200" s="31"/>
-    </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B201" s="29" t="s">
+      <c r="C200" s="16"/>
+      <c r="D200" s="17"/>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B201" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="C201" s="30"/>
-      <c r="D201" s="31"/>
-    </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B202" s="29" t="s">
+      <c r="C201" s="16"/>
+      <c r="D201" s="17"/>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B202" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="C202" s="30"/>
-      <c r="D202" s="31"/>
-    </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C202" s="16"/>
+      <c r="D202" s="17"/>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B205" s="13" t="s">
         <v>203</v>
       </c>
       <c r="C205" s="13"/>
       <c r="D205" s="13"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B206" s="10" t="s">
         <v>242</v>
       </c>
@@ -7625,7 +7230,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B207" s="10" t="s">
         <v>1</v>
       </c>
@@ -7634,7 +7239,7 @@
       </c>
       <c r="D207" s="10"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B208" s="10" t="s">
         <v>4</v>
       </c>
@@ -7643,14 +7248,14 @@
       </c>
       <c r="D208" s="10"/>
     </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B211" s="13" t="s">
         <v>205</v>
       </c>
       <c r="C211" s="13"/>
       <c r="D211" s="13"/>
     </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B212" s="10" t="s">
         <v>0</v>
       </c>
@@ -7661,7 +7266,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B213" s="10" t="s">
         <v>4</v>
       </c>
@@ -7670,7 +7275,7 @@
       </c>
       <c r="D213" s="10"/>
     </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B214" s="10" t="s">
         <v>6</v>
       </c>
@@ -7681,14 +7286,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B217" s="13" t="s">
         <v>204</v>
       </c>
       <c r="C217" s="13"/>
       <c r="D217" s="13"/>
     </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B218" s="10" t="s">
         <v>8</v>
       </c>
@@ -7699,7 +7304,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B219" s="10" t="s">
         <v>209</v>
       </c>
@@ -7710,7 +7315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B220" s="10" t="s">
         <v>6</v>
       </c>
@@ -7719,286 +7324,286 @@
       </c>
       <c r="D220" s="10"/>
     </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B223" s="28" t="s">
+    <row r="223" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B223" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="C223" s="28"/>
-      <c r="D223" s="28"/>
-      <c r="E223" s="28"/>
-      <c r="F223" s="28"/>
-    </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C223" s="23"/>
+      <c r="D223" s="23"/>
+      <c r="E223" s="23"/>
+      <c r="F223" s="23"/>
+    </row>
+    <row r="224" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B224" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C224" s="33" t="s">
+      <c r="C224" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="D224" s="34"/>
-      <c r="E224" s="34"/>
-      <c r="F224" s="35"/>
-    </row>
-    <row r="225" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D224" s="26"/>
+      <c r="E224" s="26"/>
+      <c r="F224" s="27"/>
+    </row>
+    <row r="225" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B225" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C225" s="29" t="s">
+      <c r="C225" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D225" s="30"/>
-      <c r="E225" s="30"/>
-      <c r="F225" s="31"/>
-    </row>
-    <row r="226" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D225" s="16"/>
+      <c r="E225" s="16"/>
+      <c r="F225" s="17"/>
+    </row>
+    <row r="226" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B226" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C226" s="37" t="s">
+      <c r="C226" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D226" s="15"/>
-      <c r="E226" s="15"/>
-      <c r="F226" s="16"/>
-    </row>
-    <row r="227" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D226" s="19"/>
+      <c r="E226" s="19"/>
+      <c r="F226" s="20"/>
+    </row>
+    <row r="227" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B227" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C227" s="36" t="s">
+      <c r="C227" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D227" s="36"/>
-      <c r="E227" s="36"/>
-      <c r="F227" s="36"/>
-    </row>
-    <row r="228" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D227" s="14"/>
+      <c r="E227" s="14"/>
+      <c r="F227" s="14"/>
+    </row>
+    <row r="228" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B228" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C228" s="14" t="s">
+      <c r="C228" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="D228" s="15"/>
-      <c r="E228" s="15"/>
-      <c r="F228" s="16"/>
-    </row>
-    <row r="233" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D228" s="19"/>
+      <c r="E228" s="19"/>
+      <c r="F228" s="20"/>
+    </row>
+    <row r="233" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B233" s="13" t="s">
         <v>259</v>
       </c>
       <c r="C233" s="13"/>
       <c r="D233" s="13"/>
     </row>
-    <row r="234" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B234" s="17" t="s">
+    <row r="234" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B234" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="C234" s="18"/>
-      <c r="D234" s="19"/>
-    </row>
-    <row r="235" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B235" s="20"/>
-      <c r="C235" s="21"/>
-      <c r="D235" s="22"/>
-    </row>
-    <row r="236" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B236" s="20"/>
-      <c r="C236" s="21"/>
-      <c r="D236" s="22"/>
-    </row>
-    <row r="237" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B237" s="20"/>
-      <c r="C237" s="21"/>
-      <c r="D237" s="22"/>
-    </row>
-    <row r="238" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B238" s="20"/>
-      <c r="C238" s="21"/>
-      <c r="D238" s="22"/>
-    </row>
-    <row r="239" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B239" s="20"/>
-      <c r="C239" s="21"/>
-      <c r="D239" s="22"/>
-    </row>
-    <row r="240" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B240" s="20"/>
-      <c r="C240" s="21"/>
-      <c r="D240" s="22"/>
-    </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B241" s="20"/>
-      <c r="C241" s="21"/>
-      <c r="D241" s="22"/>
-    </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B242" s="20"/>
-      <c r="C242" s="21"/>
-      <c r="D242" s="22"/>
-    </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B243" s="20"/>
-      <c r="C243" s="21"/>
-      <c r="D243" s="22"/>
-    </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B244" s="20"/>
-      <c r="C244" s="21"/>
-      <c r="D244" s="22"/>
-    </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B245" s="23"/>
-      <c r="C245" s="24"/>
-      <c r="D245" s="25"/>
-    </row>
-    <row r="249" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C234" s="30"/>
+      <c r="D234" s="31"/>
+    </row>
+    <row r="235" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B235" s="32"/>
+      <c r="C235" s="33"/>
+      <c r="D235" s="34"/>
+    </row>
+    <row r="236" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B236" s="32"/>
+      <c r="C236" s="33"/>
+      <c r="D236" s="34"/>
+    </row>
+    <row r="237" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B237" s="32"/>
+      <c r="C237" s="33"/>
+      <c r="D237" s="34"/>
+    </row>
+    <row r="238" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B238" s="32"/>
+      <c r="C238" s="33"/>
+      <c r="D238" s="34"/>
+    </row>
+    <row r="239" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B239" s="32"/>
+      <c r="C239" s="33"/>
+      <c r="D239" s="34"/>
+    </row>
+    <row r="240" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B240" s="32"/>
+      <c r="C240" s="33"/>
+      <c r="D240" s="34"/>
+    </row>
+    <row r="241" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B241" s="32"/>
+      <c r="C241" s="33"/>
+      <c r="D241" s="34"/>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B242" s="32"/>
+      <c r="C242" s="33"/>
+      <c r="D242" s="34"/>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B243" s="32"/>
+      <c r="C243" s="33"/>
+      <c r="D243" s="34"/>
+    </row>
+    <row r="244" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B244" s="32"/>
+      <c r="C244" s="33"/>
+      <c r="D244" s="34"/>
+    </row>
+    <row r="245" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B245" s="35"/>
+      <c r="C245" s="36"/>
+      <c r="D245" s="37"/>
+    </row>
+    <row r="249" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B249" s="13" t="s">
         <v>261</v>
       </c>
       <c r="C249" s="13"/>
       <c r="D249" s="13"/>
     </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B250" s="17" t="s">
+    <row r="250" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B250" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="C250" s="18" t="s">
+      <c r="C250" s="30" t="s">
         <v>260</v>
       </c>
-      <c r="D250" s="19" t="s">
+      <c r="D250" s="31" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B251" s="20" t="s">
+    <row r="251" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B251" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C251" s="21" t="s">
+      <c r="C251" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D251" s="22" t="s">
+      <c r="D251" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B252" s="20" t="s">
+    <row r="252" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B252" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C252" s="21" t="s">
+      <c r="C252" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D252" s="22" t="s">
+      <c r="D252" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="253" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B253" s="20" t="s">
+    <row r="253" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B253" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C253" s="21" t="s">
+      <c r="C253" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D253" s="22" t="s">
+      <c r="D253" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="254" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B254" s="20" t="s">
+    <row r="254" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B254" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C254" s="21" t="s">
+      <c r="C254" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D254" s="22" t="s">
+      <c r="D254" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="255" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B255" s="20" t="s">
+    <row r="255" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B255" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C255" s="21" t="s">
+      <c r="C255" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D255" s="22" t="s">
+      <c r="D255" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="256" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B256" s="20" t="s">
+    <row r="256" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B256" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C256" s="21" t="s">
+      <c r="C256" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D256" s="22" t="s">
+      <c r="D256" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="257" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B257" s="20" t="s">
+    <row r="257" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B257" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C257" s="21" t="s">
+      <c r="C257" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D257" s="22" t="s">
+      <c r="D257" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="258" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B258" s="20" t="s">
+    <row r="258" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B258" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C258" s="21" t="s">
+      <c r="C258" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D258" s="22" t="s">
+      <c r="D258" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="259" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B259" s="20" t="s">
+    <row r="259" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B259" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C259" s="21" t="s">
+      <c r="C259" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D259" s="22" t="s">
+      <c r="D259" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="260" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B260" s="20" t="s">
+    <row r="260" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B260" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C260" s="21" t="s">
+      <c r="C260" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D260" s="22" t="s">
+      <c r="D260" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="261" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B261" s="23" t="s">
+    <row r="261" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B261" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="C261" s="24" t="s">
+      <c r="C261" s="36" t="s">
         <v>260</v>
       </c>
-      <c r="D261" s="25" t="s">
+      <c r="D261" s="37" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="265" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B265" s="13" t="s">
         <v>263</v>
       </c>
       <c r="C265" s="13"/>
       <c r="D265" s="13"/>
     </row>
-    <row r="266" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B266" s="10" t="s">
         <v>264</v>
       </c>
@@ -8009,8 +7614,618 @@
         <v>266</v>
       </c>
     </row>
+    <row r="268">
+      <c r="B268" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C268" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D268" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="B269" t="str" s="10">
+        <f>"_res_."&amp;C8</f>
+        <v>_res_.test</v>
+      </c>
+      <c r="C269" t="str" s="10">
+        <f>C8</f>
+        <v>test</v>
+      </c>
+      <c r="D269" t="n" s="10">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="B270" t="str" s="10">
+        <f>"_res_."&amp;C9</f>
+        <v>_res_.byteValue</v>
+      </c>
+      <c r="C270" t="str" s="10">
+        <f>C9</f>
+        <v>byteValue</v>
+      </c>
+      <c r="D270" t="n" s="10">
+        <f>D9</f>
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="B271" t="str" s="10">
+        <f>"_res_."&amp;C10</f>
+        <v>_res_.shortValue</v>
+      </c>
+      <c r="C271" t="str" s="10">
+        <f>C10</f>
+        <v>shortValue</v>
+      </c>
+      <c r="D271" t="n" s="10">
+        <f>D10</f>
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="B272" t="str" s="10">
+        <f>"_res_."&amp;C11</f>
+        <v>_res_.intValue</v>
+      </c>
+      <c r="C272" t="str" s="10">
+        <f>C11</f>
+        <v>intValue</v>
+      </c>
+      <c r="D272" t="n" s="10">
+        <f>D11</f>
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="B273" t="str" s="10">
+        <f>"_res_."&amp;C12</f>
+        <v>_res_.longValue</v>
+      </c>
+      <c r="C273" t="str" s="10">
+        <f>C12</f>
+        <v>longValue</v>
+      </c>
+      <c r="D273" t="n" s="10">
+        <f>D12</f>
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="B274" t="str" s="10">
+        <f>"_res_."&amp;C13</f>
+        <v>_res_.floatValue</v>
+      </c>
+      <c r="C274" t="str" s="10">
+        <f>C13</f>
+        <v>floatValue</v>
+      </c>
+      <c r="D274" t="n" s="10">
+        <f>D13</f>
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="B275" t="str" s="10">
+        <f>"_res_."&amp;C14</f>
+        <v>_res_.doubleValue</v>
+      </c>
+      <c r="C275" t="str" s="10">
+        <f>C14</f>
+        <v>doubleValue</v>
+      </c>
+      <c r="D275" t="n" s="10">
+        <f>D14</f>
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="B276" t="str" s="10">
+        <f>"_res_."&amp;C15</f>
+        <v>_res_.booleanValue</v>
+      </c>
+      <c r="C276" t="str" s="10">
+        <f>C15</f>
+        <v>booleanValue</v>
+      </c>
+      <c r="D276" t="str" s="10">
+        <f>D15</f>
+        <v>y</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="B277" t="str" s="10">
+        <f>"_res_."&amp;C16</f>
+        <v>_res_.charValue</v>
+      </c>
+      <c r="C277" t="str" s="10">
+        <f>C16</f>
+        <v>charValue</v>
+      </c>
+      <c r="D277" t="str" s="10">
+        <f>D16</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="B278" t="str" s="10">
+        <f>"_res_."&amp;C17</f>
+        <v>_res_.string</v>
+      </c>
+      <c r="C278" t="str" s="10">
+        <f>C17</f>
+        <v>string</v>
+      </c>
+      <c r="D278" t="str" s="10">
+        <f>D17</f>
+        <v>str</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="B279" t="str" s="10">
+        <f>"_res_."&amp;C18</f>
+        <v>_res_.date</v>
+      </c>
+      <c r="C279" t="str" s="10">
+        <f>C18</f>
+        <v>date</v>
+      </c>
+      <c r="D279" t="str" s="10">
+        <f>D18</f>
+        <v>03/31/2017</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="B280" t="str" s="10">
+        <f>"_res_."&amp;C19</f>
+        <v>_res_.localDate</v>
+      </c>
+      <c r="C280" t="str" s="10">
+        <f>C19</f>
+        <v>localDate</v>
+      </c>
+      <c r="D280" t="str" s="10">
+        <f>D19</f>
+        <v>03/31/2017</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="B281" t="str" s="10">
+        <f>"_res_."&amp;C20</f>
+        <v>_res_.localTime</v>
+      </c>
+      <c r="C281" t="str" s="10">
+        <f>C20</f>
+        <v>localTime</v>
+      </c>
+      <c r="D281" t="str" s="10">
+        <f>D20</f>
+        <v>21:30:25</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="B282" t="str" s="10">
+        <f>"_res_."&amp;C21</f>
+        <v>_res_.localDateTime</v>
+      </c>
+      <c r="C282" t="str" s="10">
+        <f>C21</f>
+        <v>localDateTime</v>
+      </c>
+      <c r="D282" t="str" s="10">
+        <f>D21</f>
+        <v>9/20/2019 5:50 AM</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="B283" t="str" s="10">
+        <f>"_res_."&amp;C22</f>
+        <v>_res_.zonedDateTime</v>
+      </c>
+      <c r="C283" t="str" s="10">
+        <f>C22</f>
+        <v>zonedDateTime</v>
+      </c>
+      <c r="D283" t="str" s="10">
+        <f>D22</f>
+        <v>9/20/2019 5:50 AM America/Los_Angeles</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="B284" t="str" s="12">
+        <f>"_res_."&amp;C23</f>
+        <v>_res_.instantDate</v>
+      </c>
+      <c r="C284" t="str" s="12">
+        <f>C23</f>
+        <v>instantDate</v>
+      </c>
+      <c r="D284" t="str" s="12">
+        <f>D23</f>
+        <v>9/20/2019 5:50 AM America/Los_Angeles</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="B285" t="str" s="10">
+        <f>"_res_."&amp;C24</f>
+        <v>_res_.bigInt</v>
+      </c>
+      <c r="C285" t="str" s="10">
+        <f>C24</f>
+        <v>bigInt</v>
+      </c>
+      <c r="D285" t="n" s="10">
+        <f>D24</f>
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="B286" t="str" s="10">
+        <f>"_res_."&amp;C25</f>
+        <v>_res_.bigDec</v>
+      </c>
+      <c r="C286" t="str" s="10">
+        <f>C25</f>
+        <v>bigDec</v>
+      </c>
+      <c r="D286" t="n" s="10">
+        <f>D25</f>
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="B287" t="str" s="10">
+        <f>"_res_."&amp;C26</f>
+        <v>_res_.col</v>
+      </c>
+      <c r="C287" t="str" s="10">
+        <f>C26</f>
+        <v>col</v>
+      </c>
+      <c r="D287" s="10"/>
+    </row>
+    <row r="288">
+      <c r="B288" t="str" s="10">
+        <f>"_res_."&amp;C27</f>
+        <v>_res_.list</v>
+      </c>
+      <c r="C288" t="str" s="10">
+        <f>C27</f>
+        <v>list</v>
+      </c>
+      <c r="D288" s="10"/>
+    </row>
+    <row r="289">
+      <c r="B289" t="str" s="10">
+        <f>"_res_."&amp;C28</f>
+        <v>_res_.map</v>
+      </c>
+      <c r="C289" t="str" s="10">
+        <f>C28</f>
+        <v>map</v>
+      </c>
+      <c r="D289" s="10"/>
+    </row>
+    <row r="290">
+      <c r="B290" t="str" s="10">
+        <f>"_res_."&amp;C29</f>
+        <v>_res_.set</v>
+      </c>
+      <c r="C290" t="str" s="10">
+        <f>C29</f>
+        <v>set</v>
+      </c>
+      <c r="D290" s="10"/>
+    </row>
+    <row r="291">
+      <c r="B291" t="str" s="10">
+        <f>"_res_."&amp;C30</f>
+        <v>_res_.arrayList</v>
+      </c>
+      <c r="C291" t="str" s="10">
+        <f>C30</f>
+        <v>arrayList</v>
+      </c>
+      <c r="D291" s="10"/>
+    </row>
+    <row r="292">
+      <c r="B292" t="str" s="10">
+        <f>"_res_."&amp;C31</f>
+        <v>_res_.hashMap</v>
+      </c>
+      <c r="C292" t="str" s="10">
+        <f>C31</f>
+        <v>hashMap</v>
+      </c>
+      <c r="D292" s="10"/>
+    </row>
+    <row r="293">
+      <c r="B293" t="str" s="10">
+        <f>"_res_."&amp;C32</f>
+        <v>_res_.hashSet</v>
+      </c>
+      <c r="C293" t="str" s="10">
+        <f>C32</f>
+        <v>hashSet</v>
+      </c>
+      <c r="D293" s="10"/>
+    </row>
+    <row r="294">
+      <c r="B294" t="str" s="10">
+        <f>"_res_."&amp;C33</f>
+        <v>_res_.roudingMode</v>
+      </c>
+      <c r="C294" t="str" s="10">
+        <f>C33</f>
+        <v>roudingMode</v>
+      </c>
+      <c r="D294" t="str" s="10">
+        <f>D33</f>
+        <v>HALF_EVEN</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="B295" t="str" s="10">
+        <f>"_res_."&amp;C34</f>
+        <v>_res_.dv</v>
+      </c>
+      <c r="C295" t="str" s="10">
+        <f>C34</f>
+        <v>dv</v>
+      </c>
+      <c r="D295" t="n" s="10">
+        <f>D34</f>
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="B296" t="str" s="10">
+        <f>"_res_."&amp;C35</f>
+        <v>_res_.intAlias</v>
+      </c>
+      <c r="C296" t="str" s="10">
+        <f>C35</f>
+        <v>intAlias</v>
+      </c>
+      <c r="D296" t="n" s="10">
+        <f>D35</f>
+        <v>-3.0</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="B297" t="str" s="10">
+        <f>"_res_."&amp;C36</f>
+        <v>_res_.doubleAlias</v>
+      </c>
+      <c r="C297" t="str" s="10">
+        <f>C36</f>
+        <v>doubleAlias</v>
+      </c>
+      <c r="D297" t="n" s="10">
+        <f>D36</f>
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="B298" t="str" s="10">
+        <f>"_res_."&amp;C37</f>
+        <v>_res_.boolAlias</v>
+      </c>
+      <c r="C298" t="str" s="10">
+        <f>C37</f>
+        <v>boolAlias</v>
+      </c>
+      <c r="D298" t="str" s="10">
+        <f>D37</f>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="B299" t="str" s="10">
+        <f>"_res_."&amp;C38</f>
+        <v>_res_.gender</v>
+      </c>
+      <c r="C299" t="str" s="10">
+        <f>C38</f>
+        <v>gender</v>
+      </c>
+      <c r="D299" t="str" s="10">
+        <f>D38</f>
+        <v>Male</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="B300" t="s" s="10">
+        <v>337</v>
+      </c>
+      <c r="C300" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="D300" t="s" s="10">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="B301" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="C301" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="D301" s="10"/>
+    </row>
+    <row r="302">
+      <c r="B302" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="C302" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="D302" s="10"/>
+    </row>
+    <row r="303">
+      <c r="B303" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="C303" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="D303" s="10" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="B304" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="C304" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="D304" s="10"/>
+    </row>
+    <row r="305">
+      <c r="B305" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="C305" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="D305" s="10"/>
+    </row>
+    <row r="306">
+      <c r="B306" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="C306" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="D306" s="10" t="n">
+        <v>150.0</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="B307" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="C307" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D307" s="10"/>
+    </row>
+    <row r="308">
+      <c r="B308" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="C308" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="D308" s="10" t="n">
+        <v>150.0</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="B309" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="C309" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="D309" s="10"/>
+    </row>
+    <row r="310">
+      <c r="B310" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C310" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="D310" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="B311" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="C311" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D311" s="10"/>
+    </row>
+    <row r="312">
+      <c r="B312" t="s" s="10">
+        <v>295</v>
+      </c>
+      <c r="C312" t="s" s="10">
+        <v>297</v>
+      </c>
+      <c r="D312" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="77">
+  <mergeCells count="78">
+    <mergeCell ref="B265:D265"/>
+    <mergeCell ref="C228:F228"/>
+    <mergeCell ref="B233:D233"/>
+    <mergeCell ref="B234:D245"/>
+    <mergeCell ref="B249:D249"/>
+    <mergeCell ref="B250:D261"/>
+    <mergeCell ref="F166:H166"/>
+    <mergeCell ref="N166:P166"/>
+    <mergeCell ref="B169:D169"/>
+    <mergeCell ref="F169:H169"/>
+    <mergeCell ref="J169:L169"/>
+    <mergeCell ref="N169:P169"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="N125:P125"/>
+    <mergeCell ref="B128:D128"/>
+    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="J128:L128"/>
+    <mergeCell ref="N128:P128"/>
+    <mergeCell ref="N71:P71"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="N109:P109"/>
+    <mergeCell ref="B112:D112"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="J112:L112"/>
+    <mergeCell ref="N112:P112"/>
+    <mergeCell ref="N108:P108"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="J71:L71"/>
+    <mergeCell ref="B183:D183"/>
+    <mergeCell ref="B184:D184"/>
+    <mergeCell ref="B185:D185"/>
+    <mergeCell ref="B191:D191"/>
+    <mergeCell ref="C224:F224"/>
+    <mergeCell ref="B196:D196"/>
+    <mergeCell ref="B202:D202"/>
+    <mergeCell ref="B205:D205"/>
+    <mergeCell ref="B211:D211"/>
+    <mergeCell ref="B217:D217"/>
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N51:P51"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="N67:P67"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="N68:P68"/>
+    <mergeCell ref="N52:P52"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="J55:L55"/>
+    <mergeCell ref="N55:P55"/>
     <mergeCell ref="N124:P124"/>
     <mergeCell ref="F124:H124"/>
     <mergeCell ref="N165:P165"/>
@@ -8027,70 +8242,11 @@
     <mergeCell ref="C226:F226"/>
     <mergeCell ref="C225:F225"/>
     <mergeCell ref="B182:D182"/>
-    <mergeCell ref="N67:P67"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="N68:P68"/>
-    <mergeCell ref="N52:P52"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="J55:L55"/>
-    <mergeCell ref="N55:P55"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N51:P51"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="B183:D183"/>
-    <mergeCell ref="B184:D184"/>
-    <mergeCell ref="B185:D185"/>
-    <mergeCell ref="B191:D191"/>
-    <mergeCell ref="C224:F224"/>
-    <mergeCell ref="B196:D196"/>
-    <mergeCell ref="B202:D202"/>
-    <mergeCell ref="B205:D205"/>
-    <mergeCell ref="B211:D211"/>
-    <mergeCell ref="B217:D217"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="N71:P71"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="N109:P109"/>
-    <mergeCell ref="B112:D112"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="J112:L112"/>
-    <mergeCell ref="N112:P112"/>
-    <mergeCell ref="N108:P108"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="J71:L71"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="N125:P125"/>
-    <mergeCell ref="B128:D128"/>
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="J128:L128"/>
-    <mergeCell ref="N128:P128"/>
-    <mergeCell ref="F166:H166"/>
-    <mergeCell ref="N166:P166"/>
-    <mergeCell ref="B169:D169"/>
-    <mergeCell ref="F169:H169"/>
-    <mergeCell ref="J169:L169"/>
-    <mergeCell ref="N169:P169"/>
-    <mergeCell ref="B265:D265"/>
-    <mergeCell ref="C228:F228"/>
-    <mergeCell ref="B233:D233"/>
-    <mergeCell ref="B234:D245"/>
-    <mergeCell ref="B249:D249"/>
-    <mergeCell ref="B250:D261"/>
+    <mergeCell ref="B268:D268"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId4"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -8103,18 +8259,18 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.26171875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.26171875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.21875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="37.6640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="24.21875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="38" t="s">
         <v>84</v>
       </c>
@@ -8125,7 +8281,7 @@
       <c r="G3" s="38"/>
       <c r="H3" s="38"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>75</v>
       </c>
@@ -8148,7 +8304,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>77</v>
       </c>
@@ -8171,7 +8327,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>79</v>
       </c>
@@ -8194,7 +8350,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>81</v>
       </c>
@@ -8217,7 +8373,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>151</v>
       </c>
@@ -8240,7 +8396,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>85</v>
       </c>
@@ -8263,7 +8419,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>86</v>
       </c>
@@ -8286,7 +8442,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>96</v>
       </c>
@@ -8309,7 +8465,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>97</v>
       </c>
@@ -8332,7 +8488,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>123</v>
       </c>
@@ -8355,7 +8511,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>124</v>
       </c>
@@ -8378,7 +8534,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>125</v>
       </c>
@@ -8401,7 +8557,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>126</v>
       </c>
@@ -8424,7 +8580,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>195</v>
       </c>
@@ -8441,7 +8597,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="38" t="s">
         <v>334</v>
       </c>
@@ -8452,7 +8608,7 @@
       <c r="G20" s="38"/>
       <c r="H20" s="38"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -8469,7 +8625,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>75</v>
       </c>
@@ -8492,7 +8648,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>195</v>
       </c>
@@ -8526,15 +8682,15 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.68359375" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="41" t="s">
         <v>90</v>
       </c>
@@ -8545,7 +8701,7 @@
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>91</v>
       </c>
@@ -8560,7 +8716,7 @@
       </c>
       <c r="G4" s="40"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>92</v>
       </c>
@@ -8575,7 +8731,7 @@
       </c>
       <c r="G5" s="40"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E6" s="7" t="s">
         <v>303</v>
       </c>
@@ -8584,7 +8740,7 @@
       </c>
       <c r="G6" s="40"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E7" s="7" t="s">
         <v>303</v>
       </c>
@@ -8593,7 +8749,7 @@
       </c>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E8" s="7" t="s">
         <v>303</v>
       </c>

</xml_diff>

<commit_message>
EPBDS-12066 Test failure because comparison with the default value is happened (#227)
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Datatype.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Datatype.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Berek\Desktop\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C62AD75-EF35-4501-A0EB-083141902416}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6675F90-92E6-4A63-96E0-0F4CA34782B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="6165" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Datatypes" sheetId="1" r:id="rId1"/>
@@ -38,30 +38,6 @@
   </authors>
   <commentList>
     <comment ref="D8" authorId="0" shapeId="0" xr:uid="{BFB3FD4F-B101-41AF-BB9A-03ACE301B314}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Yury Molchan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Workaround to check all empty values</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H8" authorId="0" shapeId="0" xr:uid="{964788AE-23DA-4FCE-AA23-A1EF0DD19B4F}">
       <text>
         <r>
           <rPr>
@@ -589,12 +565,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="D269" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Yury Molchan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Workaround to check all empty values</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1006" uniqueCount="350">
   <si>
     <t>Integer</t>
   </si>
@@ -1609,15 +1609,61 @@
   <si>
     <t>Test evaluate evaluateTest</t>
   </si>
+  <si>
+    <t>_res_.person</t>
+  </si>
+  <si>
+    <t>=_res_.person.gender</t>
+  </si>
+  <si>
+    <t>_res_.person.gender</t>
+  </si>
+  <si>
+    <t>_res_.address</t>
+  </si>
+  <si>
+    <t>_res_.auto</t>
+  </si>
+  <si>
+    <t>personGender</t>
+  </si>
+  <si>
+    <t>_res_.person.bday</t>
+  </si>
+  <si>
+    <t>_res_.person.name</t>
+  </si>
+  <si>
+    <t>personBDay</t>
+  </si>
+  <si>
+    <t>personName</t>
+  </si>
+  <si>
+    <t>autoPower</t>
+  </si>
+  <si>
+    <t>_res_.auto.power</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>_res_.auto.model</t>
+  </si>
+  <si>
+    <t>autoModel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1825,9 +1871,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1846,13 +1891,39 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1882,32 +1953,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1921,8 +1966,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{85747B23-5477-4BE6-9006-95BD9824BD8B}"/>
+  <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1936,6 +1980,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2259,34 +2307,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:R266"/>
+  <dimension ref="B3:P312"/>
   <sheetViews>
     <sheetView topLeftCell="A127" workbookViewId="0">
       <selection activeCell="B147" sqref="B147"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.68359375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="20.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="37.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.15625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="32" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.41796875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="37.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="7.15625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="27.68359375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="19.41796875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="52.26171875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="7.15625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="24.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="19.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="15.68359375" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="12.578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="13.578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.5546875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="7.109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.44140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="37.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="7.109375" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="27.6640625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="19.44140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="52.21875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="7.109375" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="24.5546875" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="13.5546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F3" s="13" t="s">
         <v>182</v>
       </c>
@@ -2298,41 +2346,36 @@
       <c r="O3" s="13"/>
       <c r="P3" s="13"/>
     </row>
-    <row r="4" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F4" s="26" t="s">
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F4" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="N4" s="26" t="s">
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="N4" s="21" t="s">
         <v>140</v>
       </c>
-      <c r="O4" s="26"/>
-      <c r="P4" s="26"/>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7" s="13" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="F7" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="J7" s="28" t="s">
+      <c r="J7" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
       <c r="N7" s="13" t="s">
         <v>138</v>
       </c>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
     </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
         <v>192</v>
       </c>
@@ -2340,17 +2383,6 @@
         <v>193</v>
       </c>
       <c r="D8" s="10">
-        <v>1</v>
-      </c>
-      <c r="F8" s="10" t="str">
-        <f t="shared" ref="F8:F41" si="0">"_res_." &amp; C8</f>
-        <v>_res_.test</v>
-      </c>
-      <c r="G8" s="10" t="str">
-        <f>C8</f>
-        <v>test</v>
-      </c>
-      <c r="H8" s="10">
         <v>1</v>
       </c>
       <c r="J8" s="10" t="s">
@@ -2370,7 +2402,7 @@
       </c>
       <c r="P8" s="10"/>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>10</v>
       </c>
@@ -2378,18 +2410,6 @@
         <v>21</v>
       </c>
       <c r="D9" s="10">
-        <v>1</v>
-      </c>
-      <c r="F9" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.byteValue</v>
-      </c>
-      <c r="G9" s="10" t="str">
-        <f t="shared" ref="G9:H22" si="2">C9</f>
-        <v>byteValue</v>
-      </c>
-      <c r="H9" s="10">
-        <f>D9</f>
         <v>1</v>
       </c>
       <c r="J9" s="10" t="s">
@@ -2409,7 +2429,7 @@
       </c>
       <c r="P9" s="10"/>
     </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
         <v>11</v>
       </c>
@@ -2417,18 +2437,6 @@
         <v>22</v>
       </c>
       <c r="D10" s="10">
-        <v>2</v>
-      </c>
-      <c r="F10" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.shortValue</v>
-      </c>
-      <c r="G10" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>shortValue</v>
-      </c>
-      <c r="H10" s="10">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="J10" s="10" t="s">
@@ -2448,7 +2456,7 @@
       </c>
       <c r="P10" s="10"/>
     </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
         <v>0</v>
       </c>
@@ -2456,18 +2464,6 @@
         <v>23</v>
       </c>
       <c r="D11" s="10">
-        <v>3</v>
-      </c>
-      <c r="F11" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.intValue</v>
-      </c>
-      <c r="G11" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>intValue</v>
-      </c>
-      <c r="H11" s="10">
-        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="J11" s="10" t="s">
@@ -2487,7 +2483,7 @@
       </c>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
         <v>12</v>
       </c>
@@ -2495,18 +2491,6 @@
         <v>24</v>
       </c>
       <c r="D12" s="10">
-        <v>4</v>
-      </c>
-      <c r="F12" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.longValue</v>
-      </c>
-      <c r="G12" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>longValue</v>
-      </c>
-      <c r="H12" s="10">
-        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J12" s="10" t="s">
@@ -2526,7 +2510,7 @@
       </c>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13" s="10" t="s">
         <v>13</v>
       </c>
@@ -2534,18 +2518,6 @@
         <v>25</v>
       </c>
       <c r="D13" s="10">
-        <v>5</v>
-      </c>
-      <c r="F13" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.floatValue</v>
-      </c>
-      <c r="G13" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>floatValue</v>
-      </c>
-      <c r="H13" s="10">
-        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J13" s="10" t="s">
@@ -2565,7 +2537,7 @@
       </c>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14" s="10" t="s">
         <v>8</v>
       </c>
@@ -2573,18 +2545,6 @@
         <v>26</v>
       </c>
       <c r="D14" s="10">
-        <v>6</v>
-      </c>
-      <c r="F14" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.doubleValue</v>
-      </c>
-      <c r="G14" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>doubleValue</v>
-      </c>
-      <c r="H14" s="10">
-        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="J14" s="10" t="s">
@@ -2604,7 +2564,7 @@
       </c>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15" s="10" t="s">
         <v>15</v>
       </c>
@@ -2613,18 +2573,6 @@
       </c>
       <c r="D15" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="F15" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.booleanValue</v>
-      </c>
-      <c r="G15" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>booleanValue</v>
-      </c>
-      <c r="H15" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>y</v>
       </c>
       <c r="J15" s="10" t="s">
         <v>15</v>
@@ -2643,7 +2591,7 @@
       </c>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="s">
         <v>16</v>
       </c>
@@ -2652,18 +2600,6 @@
       </c>
       <c r="D16" s="10" t="s">
         <v>114</v>
-      </c>
-      <c r="F16" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.charValue</v>
-      </c>
-      <c r="G16" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>charValue</v>
-      </c>
-      <c r="H16" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>A</v>
       </c>
       <c r="J16" s="10" t="s">
         <v>16</v>
@@ -2682,7 +2618,7 @@
       </c>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B17" s="10" t="s">
         <v>4</v>
       </c>
@@ -2691,18 +2627,6 @@
       </c>
       <c r="D17" s="10" t="s">
         <v>20</v>
-      </c>
-      <c r="F17" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.string</v>
-      </c>
-      <c r="G17" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>string</v>
-      </c>
-      <c r="H17" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>str</v>
       </c>
       <c r="J17" s="10" t="s">
         <v>4</v>
@@ -2721,7 +2645,7 @@
       </c>
       <c r="P17" s="10"/>
     </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
         <v>1</v>
       </c>
@@ -2730,18 +2654,6 @@
       </c>
       <c r="D18" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="F18" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.date</v>
-      </c>
-      <c r="G18" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>date</v>
-      </c>
-      <c r="H18" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>03/31/2017</v>
       </c>
       <c r="J18" s="10" t="s">
         <v>1</v>
@@ -2760,7 +2672,7 @@
       </c>
       <c r="P18" s="1"/>
     </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B19" s="10" t="s">
         <v>299</v>
       </c>
@@ -2769,18 +2681,6 @@
       </c>
       <c r="D19" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="F19" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.localDate</v>
-      </c>
-      <c r="G19" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>localDate</v>
-      </c>
-      <c r="H19" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>03/31/2017</v>
       </c>
       <c r="J19" s="10" t="s">
         <v>299</v>
@@ -2799,7 +2699,7 @@
       </c>
       <c r="P19" s="1"/>
     </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B20" s="10" t="s">
         <v>308</v>
       </c>
@@ -2808,18 +2708,6 @@
       </c>
       <c r="D20" s="1" t="s">
         <v>312</v>
-      </c>
-      <c r="F20" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.localTime</v>
-      </c>
-      <c r="G20" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>localTime</v>
-      </c>
-      <c r="H20" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>21:30:25</v>
       </c>
       <c r="J20" s="10" t="s">
         <v>308</v>
@@ -2838,7 +2726,7 @@
       </c>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B21" s="10" t="s">
         <v>309</v>
       </c>
@@ -2847,18 +2735,6 @@
       </c>
       <c r="D21" s="1" t="s">
         <v>315</v>
-      </c>
-      <c r="F21" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.localDateTime</v>
-      </c>
-      <c r="G21" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>localDateTime</v>
-      </c>
-      <c r="H21" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>9/20/2019 5:50 AM</v>
       </c>
       <c r="J21" s="10" t="s">
         <v>309</v>
@@ -2877,7 +2753,7 @@
       </c>
       <c r="P21" s="1"/>
     </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B22" s="10" t="s">
         <v>316</v>
       </c>
@@ -2886,18 +2762,6 @@
       </c>
       <c r="D22" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="F22" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.zonedDateTime</v>
-      </c>
-      <c r="G22" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>zonedDateTime</v>
-      </c>
-      <c r="H22" s="10" t="str">
-        <f t="shared" si="2"/>
-        <v>9/20/2019 5:50 AM America/Los_Angeles</v>
       </c>
       <c r="J22" s="10" t="s">
         <v>316</v>
@@ -2916,7 +2780,7 @@
       </c>
       <c r="P22" s="1"/>
     </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B23" s="12" t="s">
         <v>328</v>
       </c>
@@ -2925,18 +2789,6 @@
       </c>
       <c r="D23" s="1" t="s">
         <v>318</v>
-      </c>
-      <c r="F23" s="12" t="str">
-        <f t="shared" ref="F23" si="4">"_res_." &amp; C23</f>
-        <v>_res_.instantDate</v>
-      </c>
-      <c r="G23" s="12" t="str">
-        <f t="shared" ref="G23" si="5">C23</f>
-        <v>instantDate</v>
-      </c>
-      <c r="H23" s="12" t="str">
-        <f t="shared" ref="H23" si="6">D23</f>
-        <v>9/20/2019 5:50 AM America/Los_Angeles</v>
       </c>
       <c r="J23" s="12" t="s">
         <v>328</v>
@@ -2955,7 +2807,7 @@
       </c>
       <c r="P23" s="1"/>
     </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B24" s="10" t="s">
         <v>17</v>
       </c>
@@ -2963,18 +2815,6 @@
         <v>220</v>
       </c>
       <c r="D24" s="10">
-        <v>7</v>
-      </c>
-      <c r="F24" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.bigInt</v>
-      </c>
-      <c r="G24" s="10" t="str">
-        <f>C24</f>
-        <v>bigInt</v>
-      </c>
-      <c r="H24" s="10">
-        <f>D24</f>
         <v>7</v>
       </c>
       <c r="J24" s="10" t="s">
@@ -2994,7 +2834,7 @@
       </c>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B25" s="10" t="s">
         <v>18</v>
       </c>
@@ -3002,18 +2842,6 @@
         <v>219</v>
       </c>
       <c r="D25" s="10">
-        <v>8</v>
-      </c>
-      <c r="F25" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.bigDec</v>
-      </c>
-      <c r="G25" s="10" t="str">
-        <f>C25</f>
-        <v>bigDec</v>
-      </c>
-      <c r="H25" s="10">
-        <f>D25</f>
         <v>8</v>
       </c>
       <c r="J25" s="10" t="s">
@@ -3033,7 +2861,7 @@
       </c>
       <c r="P25" s="10"/>
     </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B26" s="10" t="s">
         <v>145</v>
       </c>
@@ -3043,15 +2871,6 @@
       <c r="D26" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F26" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.col</v>
-      </c>
-      <c r="G26" s="10" t="str">
-        <f t="shared" ref="G26:H41" si="9">C26</f>
-        <v>col</v>
-      </c>
-      <c r="H26" s="10"/>
       <c r="J26" s="10" t="s">
         <v>145</v>
       </c>
@@ -3069,7 +2888,7 @@
       </c>
       <c r="P26" s="10"/>
     </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B27" s="10" t="s">
         <v>33</v>
       </c>
@@ -3079,15 +2898,6 @@
       <c r="D27" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F27" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.list</v>
-      </c>
-      <c r="G27" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>list</v>
-      </c>
-      <c r="H27" s="10"/>
       <c r="J27" s="10" t="s">
         <v>33</v>
       </c>
@@ -3105,7 +2915,7 @@
       </c>
       <c r="P27" s="10"/>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B28" s="10" t="s">
         <v>34</v>
       </c>
@@ -3115,15 +2925,6 @@
       <c r="D28" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F28" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.map</v>
-      </c>
-      <c r="G28" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>map</v>
-      </c>
-      <c r="H28" s="10"/>
       <c r="J28" s="10" t="s">
         <v>34</v>
       </c>
@@ -3141,7 +2942,7 @@
       </c>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B29" s="10" t="s">
         <v>37</v>
       </c>
@@ -3151,15 +2952,6 @@
       <c r="D29" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F29" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.set</v>
-      </c>
-      <c r="G29" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>set</v>
-      </c>
-      <c r="H29" s="10"/>
       <c r="J29" s="10" t="s">
         <v>37</v>
       </c>
@@ -3177,7 +2969,7 @@
       </c>
       <c r="P29" s="10"/>
     </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B30" s="10" t="s">
         <v>223</v>
       </c>
@@ -3187,15 +2979,6 @@
       <c r="D30" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F30" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.arrayList</v>
-      </c>
-      <c r="G30" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>arrayList</v>
-      </c>
-      <c r="H30" s="10"/>
       <c r="J30" s="10" t="s">
         <v>223</v>
       </c>
@@ -3213,7 +2996,7 @@
       </c>
       <c r="P30" s="10"/>
     </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B31" s="10" t="s">
         <v>224</v>
       </c>
@@ -3223,15 +3006,6 @@
       <c r="D31" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F31" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.hashMap</v>
-      </c>
-      <c r="G31" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>hashMap</v>
-      </c>
-      <c r="H31" s="10"/>
       <c r="J31" s="10" t="s">
         <v>224</v>
       </c>
@@ -3249,7 +3023,7 @@
       </c>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
         <v>225</v>
       </c>
@@ -3259,15 +3033,6 @@
       <c r="D32" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F32" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.hashSet</v>
-      </c>
-      <c r="G32" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>hashSet</v>
-      </c>
-      <c r="H32" s="10"/>
       <c r="J32" s="10" t="s">
         <v>225</v>
       </c>
@@ -3285,7 +3050,7 @@
       </c>
       <c r="P32" s="10"/>
     </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B33" s="10" t="s">
         <v>249</v>
       </c>
@@ -3294,18 +3059,6 @@
       </c>
       <c r="D33" s="10" t="s">
         <v>251</v>
-      </c>
-      <c r="F33" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.roudingMode</v>
-      </c>
-      <c r="G33" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>roudingMode</v>
-      </c>
-      <c r="H33" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>HALF_EVEN</v>
       </c>
       <c r="J33" s="10" t="s">
         <v>249</v>
@@ -3324,7 +3077,7 @@
       </c>
       <c r="P33" s="10"/>
     </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B34" s="10" t="s">
         <v>192</v>
       </c>
@@ -3332,18 +3085,6 @@
         <v>255</v>
       </c>
       <c r="D34" s="10">
-        <v>10.1</v>
-      </c>
-      <c r="F34" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.dv</v>
-      </c>
-      <c r="G34" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>dv</v>
-      </c>
-      <c r="H34" s="10">
-        <f t="shared" si="9"/>
         <v>10.1</v>
       </c>
       <c r="J34" s="10" t="s">
@@ -3363,7 +3104,7 @@
       </c>
       <c r="P34" s="10"/>
     </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B35" s="10" t="s">
         <v>270</v>
       </c>
@@ -3371,18 +3112,6 @@
         <v>273</v>
       </c>
       <c r="D35" s="10">
-        <v>-3</v>
-      </c>
-      <c r="F35" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.intAlias</v>
-      </c>
-      <c r="G35" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>intAlias</v>
-      </c>
-      <c r="H35" s="10">
-        <f t="shared" si="9"/>
         <v>-3</v>
       </c>
       <c r="J35" s="10" t="s">
@@ -3404,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B36" s="10" t="s">
         <v>271</v>
       </c>
@@ -3412,18 +3141,6 @@
         <v>274</v>
       </c>
       <c r="D36" s="10">
-        <v>3.3</v>
-      </c>
-      <c r="F36" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.doubleAlias</v>
-      </c>
-      <c r="G36" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>doubleAlias</v>
-      </c>
-      <c r="H36" s="10">
-        <f t="shared" si="9"/>
         <v>3.3</v>
       </c>
       <c r="J36" s="10" t="s">
@@ -3443,7 +3160,7 @@
       </c>
       <c r="P36" s="10"/>
     </row>
-    <row r="37" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B37" s="10" t="s">
         <v>272</v>
       </c>
@@ -3452,18 +3169,6 @@
       </c>
       <c r="D37" s="10" t="s">
         <v>276</v>
-      </c>
-      <c r="F37" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.boolAlias</v>
-      </c>
-      <c r="G37" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>boolAlias</v>
-      </c>
-      <c r="H37" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>n</v>
       </c>
       <c r="J37" s="10" t="s">
         <v>272</v>
@@ -3482,7 +3187,7 @@
       </c>
       <c r="P37" s="10"/>
     </row>
-    <row r="38" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B38" s="10" t="s">
         <v>242</v>
       </c>
@@ -3491,18 +3196,6 @@
       </c>
       <c r="D38" s="10" t="s">
         <v>239</v>
-      </c>
-      <c r="F38" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.gender</v>
-      </c>
-      <c r="G38" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>gender</v>
-      </c>
-      <c r="H38" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>Male</v>
       </c>
       <c r="J38" s="10" t="s">
         <v>242</v>
@@ -3521,7 +3214,7 @@
       </c>
       <c r="P38" s="10"/>
     </row>
-    <row r="39" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B39" s="10" t="s">
         <v>6</v>
       </c>
@@ -3531,15 +3224,6 @@
       <c r="D39" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F39" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.person</v>
-      </c>
-      <c r="G39" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>person</v>
-      </c>
-      <c r="H39" s="10"/>
       <c r="J39" s="10" t="s">
         <v>6</v>
       </c>
@@ -3557,7 +3241,7 @@
       </c>
       <c r="P39" s="10"/>
     </row>
-    <row r="40" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B40" s="10" t="s">
         <v>209</v>
       </c>
@@ -3567,15 +3251,6 @@
       <c r="D40" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F40" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.auto</v>
-      </c>
-      <c r="G40" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>auto</v>
-      </c>
-      <c r="H40" s="10"/>
       <c r="J40" s="10" t="s">
         <v>209</v>
       </c>
@@ -3593,7 +3268,7 @@
       </c>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B41" s="10" t="s">
         <v>234</v>
       </c>
@@ -3603,15 +3278,6 @@
       <c r="D41" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F41" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>_res_.address</v>
-      </c>
-      <c r="G41" s="10" t="str">
-        <f t="shared" si="9"/>
-        <v>address</v>
-      </c>
-      <c r="H41" s="10"/>
       <c r="J41" s="10" t="s">
         <v>234</v>
       </c>
@@ -3629,76 +3295,15 @@
       </c>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F42" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="H42" s="10">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="43" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F43" s="10" t="s">
-        <v>288</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H43" s="10"/>
-    </row>
-    <row r="44" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F44" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="G44" s="10" t="s">
-        <v>289</v>
-      </c>
-      <c r="H44" s="10">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="45" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F45" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="H45" s="10"/>
-    </row>
-    <row r="46" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F46" s="10" t="s">
-        <v>293</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>242</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="47" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F47" s="10" t="s">
-        <v>294</v>
-      </c>
-      <c r="G47" s="10" t="s">
-        <v>296</v>
-      </c>
-      <c r="H47" s="10"/>
-    </row>
-    <row r="48" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F48" s="10" t="s">
-        <v>295</v>
-      </c>
-      <c r="G48" s="10" t="s">
-        <v>297</v>
-      </c>
-      <c r="H48" s="10"/>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="2:16" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="2:16" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:16" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="2:16" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="2:16" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="2:16" x14ac:dyDescent="0.3"/>
+    <row r="49"/>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F51" s="13" t="s">
         <v>181</v>
       </c>
@@ -3710,41 +3315,41 @@
       <c r="O51" s="13"/>
       <c r="P51" s="13"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F52" s="26" t="s">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F52" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="G52" s="26"/>
-      <c r="H52" s="26"/>
-      <c r="N52" s="26" t="s">
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="N52" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="O52" s="26"/>
-      <c r="P52" s="26"/>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O52" s="21"/>
+      <c r="P52" s="21"/>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B55" s="13" t="s">
         <v>88</v>
       </c>
       <c r="C55" s="13"/>
       <c r="D55" s="13"/>
-      <c r="F55" s="27" t="s">
+      <c r="F55" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="G55" s="27"/>
-      <c r="H55" s="27"/>
-      <c r="J55" s="28" t="s">
+      <c r="G55" s="22"/>
+      <c r="H55" s="22"/>
+      <c r="J55" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="K55" s="28"/>
-      <c r="L55" s="28"/>
-      <c r="N55" s="27" t="s">
+      <c r="K55" s="23"/>
+      <c r="L55" s="23"/>
+      <c r="N55" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="O55" s="27"/>
-      <c r="P55" s="27"/>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O55" s="22"/>
+      <c r="P55" s="22"/>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B56" s="10" t="s">
         <v>192</v>
       </c>
@@ -3786,7 +3391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B57" s="10" t="s">
         <v>39</v>
       </c>
@@ -3827,7 +3432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
         <v>40</v>
       </c>
@@ -3868,7 +3473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B59" s="10" t="s">
         <v>41</v>
       </c>
@@ -3909,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B60" s="10" t="s">
         <v>42</v>
       </c>
@@ -3950,7 +3555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B61" s="10" t="s">
         <v>43</v>
       </c>
@@ -3991,7 +3596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B62" s="10" t="s">
         <v>44</v>
       </c>
@@ -4032,7 +3637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B63" s="10" t="s">
         <v>46</v>
       </c>
@@ -4073,7 +3678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B64" s="10" t="s">
         <v>45</v>
       </c>
@@ -4112,7 +3717,7 @@
       </c>
       <c r="P64" s="10"/>
     </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F67" s="13" t="s">
         <v>179</v>
       </c>
@@ -4124,19 +3729,19 @@
       <c r="O67" s="13"/>
       <c r="P67" s="13"/>
     </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F68" s="26" t="s">
+    <row r="68" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F68" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="G68" s="26"/>
-      <c r="H68" s="26"/>
-      <c r="N68" s="26" t="s">
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="N68" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="O68" s="26"/>
-      <c r="P68" s="26"/>
-    </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O68" s="21"/>
+      <c r="P68" s="21"/>
+    </row>
+    <row r="71" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B71" s="13" t="s">
         <v>143</v>
       </c>
@@ -4147,18 +3752,18 @@
       </c>
       <c r="G71" s="13"/>
       <c r="H71" s="13"/>
-      <c r="J71" s="28" t="s">
+      <c r="J71" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="K71" s="28"/>
-      <c r="L71" s="28"/>
+      <c r="K71" s="23"/>
+      <c r="L71" s="23"/>
       <c r="N71" s="13" t="s">
         <v>159</v>
       </c>
       <c r="O71" s="13"/>
       <c r="P71" s="13"/>
     </row>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B72" s="10" t="s">
         <v>192</v>
       </c>
@@ -4200,7 +3805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B73" s="10" t="s">
         <v>98</v>
       </c>
@@ -4239,7 +3844,7 @@
       </c>
       <c r="P73" s="10"/>
     </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B74" s="10" t="s">
         <v>99</v>
       </c>
@@ -4278,7 +3883,7 @@
       </c>
       <c r="P74" s="10"/>
     </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B75" s="10" t="s">
         <v>100</v>
       </c>
@@ -4317,7 +3922,7 @@
       </c>
       <c r="P75" s="10"/>
     </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B76" s="10" t="s">
         <v>101</v>
       </c>
@@ -4356,7 +3961,7 @@
       </c>
       <c r="P76" s="10"/>
     </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B77" s="10" t="s">
         <v>102</v>
       </c>
@@ -4395,7 +4000,7 @@
       </c>
       <c r="P77" s="10"/>
     </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B78" s="10" t="s">
         <v>103</v>
       </c>
@@ -4434,7 +4039,7 @@
       </c>
       <c r="P78" s="10"/>
     </row>
-    <row r="79" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B79" s="10" t="s">
         <v>104</v>
       </c>
@@ -4473,7 +4078,7 @@
       </c>
       <c r="P79" s="10"/>
     </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B80" s="10" t="s">
         <v>105</v>
       </c>
@@ -4512,7 +4117,7 @@
       </c>
       <c r="P80" s="10"/>
     </row>
-    <row r="81" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B81" s="10" t="s">
         <v>58</v>
       </c>
@@ -4551,7 +4156,7 @@
       </c>
       <c r="P81" s="10"/>
     </row>
-    <row r="82" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B82" s="10" t="s">
         <v>59</v>
       </c>
@@ -4590,7 +4195,7 @@
       </c>
       <c r="P82" s="1"/>
     </row>
-    <row r="83" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B83" s="11" t="s">
         <v>319</v>
       </c>
@@ -4629,7 +4234,7 @@
       </c>
       <c r="P83" s="1"/>
     </row>
-    <row r="84" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B84" s="11" t="s">
         <v>320</v>
       </c>
@@ -4668,7 +4273,7 @@
       </c>
       <c r="P84" s="1"/>
     </row>
-    <row r="85" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B85" s="11" t="s">
         <v>321</v>
       </c>
@@ -4707,7 +4312,7 @@
       </c>
       <c r="P85" s="1"/>
     </row>
-    <row r="86" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B86" s="11" t="s">
         <v>322</v>
       </c>
@@ -4746,7 +4351,7 @@
       </c>
       <c r="P86" s="1"/>
     </row>
-    <row r="87" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B87" s="12" t="s">
         <v>330</v>
       </c>
@@ -4786,7 +4391,7 @@
       </c>
       <c r="P87" s="1"/>
     </row>
-    <row r="88" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B88" s="10" t="s">
         <v>60</v>
       </c>
@@ -4825,7 +4430,7 @@
       </c>
       <c r="P88" s="10"/>
     </row>
-    <row r="89" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B89" s="10" t="s">
         <v>61</v>
       </c>
@@ -4864,7 +4469,7 @@
       </c>
       <c r="P89" s="10"/>
     </row>
-    <row r="90" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B90" s="10" t="s">
         <v>148</v>
       </c>
@@ -4900,7 +4505,7 @@
       </c>
       <c r="P90" s="10"/>
     </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B91" s="10" t="s">
         <v>208</v>
       </c>
@@ -4936,7 +4541,7 @@
       </c>
       <c r="P91" s="10"/>
     </row>
-    <row r="92" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B92" s="10" t="s">
         <v>116</v>
       </c>
@@ -4972,7 +4577,7 @@
       </c>
       <c r="P92" s="10"/>
     </row>
-    <row r="93" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B93" s="10" t="s">
         <v>117</v>
       </c>
@@ -5008,7 +4613,7 @@
       </c>
       <c r="P93" s="10"/>
     </row>
-    <row r="94" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B94" s="10" t="s">
         <v>208</v>
       </c>
@@ -5044,7 +4649,7 @@
       </c>
       <c r="P94" s="10"/>
     </row>
-    <row r="95" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B95" s="10" t="s">
         <v>229</v>
       </c>
@@ -5080,7 +4685,7 @@
       </c>
       <c r="P95" s="10"/>
     </row>
-    <row r="96" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B96" s="10" t="s">
         <v>230</v>
       </c>
@@ -5116,7 +4721,7 @@
       </c>
       <c r="P96" s="10"/>
     </row>
-    <row r="97" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B97" s="10" t="s">
         <v>277</v>
       </c>
@@ -5155,7 +4760,7 @@
       </c>
       <c r="P97" s="10"/>
     </row>
-    <row r="98" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B98" s="10" t="s">
         <v>278</v>
       </c>
@@ -5194,7 +4799,7 @@
       </c>
       <c r="P98" s="10"/>
     </row>
-    <row r="99" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B99" s="10" t="s">
         <v>279</v>
       </c>
@@ -5233,7 +4838,7 @@
       </c>
       <c r="P99" s="10"/>
     </row>
-    <row r="100" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B100" s="10" t="s">
         <v>244</v>
       </c>
@@ -5272,7 +4877,7 @@
       </c>
       <c r="P100" s="10"/>
     </row>
-    <row r="101" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B101" s="10" t="s">
         <v>235</v>
       </c>
@@ -5308,7 +4913,7 @@
       </c>
       <c r="P101" s="10"/>
     </row>
-    <row r="102" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B102" s="10" t="s">
         <v>211</v>
       </c>
@@ -5344,7 +4949,7 @@
       </c>
       <c r="P102" s="10"/>
     </row>
-    <row r="103" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B103" s="10" t="s">
         <v>212</v>
       </c>
@@ -5380,7 +4985,7 @@
       </c>
       <c r="P103" s="10"/>
     </row>
-    <row r="104" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B104" s="10" t="s">
         <v>252</v>
       </c>
@@ -5419,7 +5024,7 @@
       </c>
       <c r="P104" s="10"/>
     </row>
-    <row r="105" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B105" s="10" t="s">
         <v>256</v>
       </c>
@@ -5458,7 +5063,7 @@
       </c>
       <c r="P105" s="10"/>
     </row>
-    <row r="108" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F108" s="13" t="s">
         <v>177</v>
       </c>
@@ -5470,19 +5075,19 @@
       <c r="O108" s="13"/>
       <c r="P108" s="13"/>
     </row>
-    <row r="109" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F109" s="26" t="s">
+    <row r="109" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F109" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="G109" s="26"/>
-      <c r="H109" s="26"/>
-      <c r="N109" s="26" t="s">
+      <c r="G109" s="21"/>
+      <c r="H109" s="21"/>
+      <c r="N109" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="O109" s="26"/>
-      <c r="P109" s="26"/>
-    </row>
-    <row r="112" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O109" s="21"/>
+      <c r="P109" s="21"/>
+    </row>
+    <row r="112" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B112" s="13" t="s">
         <v>144</v>
       </c>
@@ -5493,18 +5098,18 @@
       </c>
       <c r="G112" s="13"/>
       <c r="H112" s="13"/>
-      <c r="J112" s="28" t="s">
+      <c r="J112" s="23" t="s">
         <v>142</v>
       </c>
-      <c r="K112" s="28"/>
-      <c r="L112" s="28"/>
-      <c r="N112" s="27" t="s">
+      <c r="K112" s="23"/>
+      <c r="L112" s="23"/>
+      <c r="N112" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="O112" s="27"/>
-      <c r="P112" s="27"/>
-    </row>
-    <row r="113" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O112" s="22"/>
+      <c r="P112" s="22"/>
+    </row>
+    <row r="113" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B113" s="10" t="s">
         <v>192</v>
       </c>
@@ -5546,7 +5151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B114" s="10" t="s">
         <v>47</v>
       </c>
@@ -5584,7 +5189,7 @@
       </c>
       <c r="P114" s="10"/>
     </row>
-    <row r="115" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B115" s="10" t="s">
         <v>48</v>
       </c>
@@ -5622,7 +5227,7 @@
       </c>
       <c r="P115" s="10"/>
     </row>
-    <row r="116" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B116" s="10" t="s">
         <v>49</v>
       </c>
@@ -5660,7 +5265,7 @@
       </c>
       <c r="P116" s="10"/>
     </row>
-    <row r="117" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B117" s="10" t="s">
         <v>50</v>
       </c>
@@ -5698,7 +5303,7 @@
       </c>
       <c r="P117" s="10"/>
     </row>
-    <row r="118" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B118" s="10" t="s">
         <v>51</v>
       </c>
@@ -5736,7 +5341,7 @@
       </c>
       <c r="P118" s="10"/>
     </row>
-    <row r="119" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B119" s="10" t="s">
         <v>52</v>
       </c>
@@ -5774,7 +5379,7 @@
       </c>
       <c r="P119" s="10"/>
     </row>
-    <row r="120" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B120" s="10" t="s">
         <v>53</v>
       </c>
@@ -5812,7 +5417,7 @@
       </c>
       <c r="P120" s="10"/>
     </row>
-    <row r="121" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B121" s="10" t="s">
         <v>54</v>
       </c>
@@ -5850,7 +5455,7 @@
       </c>
       <c r="P121" s="10"/>
     </row>
-    <row r="124" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F124" s="13" t="s">
         <v>168</v>
       </c>
@@ -5862,19 +5467,19 @@
       <c r="O124" s="13"/>
       <c r="P124" s="13"/>
     </row>
-    <row r="125" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F125" s="26" t="s">
+    <row r="125" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F125" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="G125" s="26"/>
-      <c r="H125" s="26"/>
-      <c r="N125" s="26" t="s">
+      <c r="G125" s="21"/>
+      <c r="H125" s="21"/>
+      <c r="N125" s="21" t="s">
         <v>166</v>
       </c>
-      <c r="O125" s="26"/>
-      <c r="P125" s="26"/>
-    </row>
-    <row r="128" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O125" s="21"/>
+      <c r="P125" s="21"/>
+    </row>
+    <row r="128" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B128" s="13" t="s">
         <v>155</v>
       </c>
@@ -5885,18 +5490,18 @@
       </c>
       <c r="G128" s="13"/>
       <c r="H128" s="13"/>
-      <c r="J128" s="28" t="s">
+      <c r="J128" s="23" t="s">
         <v>154</v>
       </c>
-      <c r="K128" s="28"/>
-      <c r="L128" s="28"/>
+      <c r="K128" s="23"/>
+      <c r="L128" s="23"/>
       <c r="N128" s="13" t="s">
         <v>191</v>
       </c>
       <c r="O128" s="13"/>
       <c r="P128" s="13"/>
     </row>
-    <row r="129" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B129" s="10" t="s">
         <v>192</v>
       </c>
@@ -5938,7 +5543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B130" s="10" t="s">
         <v>106</v>
       </c>
@@ -5974,7 +5579,7 @@
       </c>
       <c r="P130" s="10"/>
     </row>
-    <row r="131" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B131" s="10" t="s">
         <v>107</v>
       </c>
@@ -6010,7 +5615,7 @@
       </c>
       <c r="P131" s="10"/>
     </row>
-    <row r="132" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B132" s="10" t="s">
         <v>108</v>
       </c>
@@ -6046,7 +5651,7 @@
       </c>
       <c r="P132" s="10"/>
     </row>
-    <row r="133" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B133" s="10" t="s">
         <v>109</v>
       </c>
@@ -6082,7 +5687,7 @@
       </c>
       <c r="P133" s="10"/>
     </row>
-    <row r="134" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B134" s="10" t="s">
         <v>110</v>
       </c>
@@ -6118,7 +5723,7 @@
       </c>
       <c r="P134" s="10"/>
     </row>
-    <row r="135" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B135" s="10" t="s">
         <v>111</v>
       </c>
@@ -6154,7 +5759,7 @@
       </c>
       <c r="P135" s="10"/>
     </row>
-    <row r="136" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B136" s="10" t="s">
         <v>112</v>
       </c>
@@ -6190,7 +5795,7 @@
       </c>
       <c r="P136" s="10"/>
     </row>
-    <row r="137" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B137" s="10" t="s">
         <v>113</v>
       </c>
@@ -6226,7 +5831,7 @@
       </c>
       <c r="P137" s="10"/>
     </row>
-    <row r="138" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B138" s="10" t="s">
         <v>71</v>
       </c>
@@ -6262,7 +5867,7 @@
       </c>
       <c r="P138" s="10"/>
     </row>
-    <row r="139" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B139" s="10" t="s">
         <v>72</v>
       </c>
@@ -6298,7 +5903,7 @@
       </c>
       <c r="P139" s="1"/>
     </row>
-    <row r="140" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B140" s="11" t="s">
         <v>324</v>
       </c>
@@ -6334,7 +5939,7 @@
       </c>
       <c r="P140" s="1"/>
     </row>
-    <row r="141" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B141" s="11" t="s">
         <v>325</v>
       </c>
@@ -6370,7 +5975,7 @@
       </c>
       <c r="P141" s="1"/>
     </row>
-    <row r="142" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B142" s="11" t="s">
         <v>326</v>
       </c>
@@ -6406,7 +6011,7 @@
       </c>
       <c r="P142" s="1"/>
     </row>
-    <row r="143" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B143" s="11" t="s">
         <v>327</v>
       </c>
@@ -6442,7 +6047,7 @@
       </c>
       <c r="P143" s="1"/>
     </row>
-    <row r="144" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B144" s="12" t="s">
         <v>332</v>
       </c>
@@ -6478,7 +6083,7 @@
       </c>
       <c r="P144" s="1"/>
     </row>
-    <row r="145" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B145" s="10" t="s">
         <v>73</v>
       </c>
@@ -6514,7 +6119,7 @@
       </c>
       <c r="P145" s="10"/>
     </row>
-    <row r="146" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B146" s="10" t="s">
         <v>74</v>
       </c>
@@ -6550,7 +6155,7 @@
       </c>
       <c r="P146" s="10"/>
     </row>
-    <row r="147" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B147" s="10" t="s">
         <v>147</v>
       </c>
@@ -6586,7 +6191,7 @@
       </c>
       <c r="P147" s="10"/>
     </row>
-    <row r="148" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B148" s="10" t="s">
         <v>118</v>
       </c>
@@ -6622,7 +6227,7 @@
       </c>
       <c r="P148" s="10"/>
     </row>
-    <row r="149" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B149" s="10" t="s">
         <v>119</v>
       </c>
@@ -6658,7 +6263,7 @@
       </c>
       <c r="P149" s="10"/>
     </row>
-    <row r="150" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B150" s="10" t="s">
         <v>120</v>
       </c>
@@ -6694,7 +6299,7 @@
       </c>
       <c r="P150" s="10"/>
     </row>
-    <row r="151" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B151" s="10" t="s">
         <v>231</v>
       </c>
@@ -6730,7 +6335,7 @@
       </c>
       <c r="P151" s="10"/>
     </row>
-    <row r="152" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B152" s="10" t="s">
         <v>232</v>
       </c>
@@ -6766,7 +6371,7 @@
       </c>
       <c r="P152" s="10"/>
     </row>
-    <row r="153" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B153" s="10" t="s">
         <v>233</v>
       </c>
@@ -6802,7 +6407,7 @@
       </c>
       <c r="P153" s="10"/>
     </row>
-    <row r="154" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B154" s="10" t="s">
         <v>283</v>
       </c>
@@ -6838,7 +6443,7 @@
       </c>
       <c r="P154" s="10"/>
     </row>
-    <row r="155" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B155" s="10" t="s">
         <v>284</v>
       </c>
@@ -6874,7 +6479,7 @@
       </c>
       <c r="P155" s="10"/>
     </row>
-    <row r="156" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B156" s="10" t="s">
         <v>285</v>
       </c>
@@ -6910,7 +6515,7 @@
       </c>
       <c r="P156" s="10"/>
     </row>
-    <row r="157" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B157" s="10" t="s">
         <v>245</v>
       </c>
@@ -6946,7 +6551,7 @@
       </c>
       <c r="P157" s="10"/>
     </row>
-    <row r="158" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B158" s="10" t="s">
         <v>236</v>
       </c>
@@ -6982,7 +6587,7 @@
       </c>
       <c r="P158" s="10"/>
     </row>
-    <row r="159" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B159" s="10" t="s">
         <v>213</v>
       </c>
@@ -7018,7 +6623,7 @@
       </c>
       <c r="P159" s="10"/>
     </row>
-    <row r="160" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B160" s="10" t="s">
         <v>214</v>
       </c>
@@ -7054,7 +6659,7 @@
       </c>
       <c r="P160" s="10"/>
     </row>
-    <row r="161" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B161" s="10" t="s">
         <v>254</v>
       </c>
@@ -7090,7 +6695,7 @@
       </c>
       <c r="P161" s="10"/>
     </row>
-    <row r="162" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B162" s="10" t="s">
         <v>258</v>
       </c>
@@ -7126,7 +6731,7 @@
       </c>
       <c r="P162" s="10"/>
     </row>
-    <row r="165" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="2:16" x14ac:dyDescent="0.3">
       <c r="F165" s="13" t="s">
         <v>175</v>
       </c>
@@ -7138,41 +6743,41 @@
       <c r="O165" s="13"/>
       <c r="P165" s="13"/>
     </row>
-    <row r="166" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="F166" s="26" t="s">
+    <row r="166" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F166" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="G166" s="26"/>
-      <c r="H166" s="26"/>
-      <c r="N166" s="26" t="s">
+      <c r="G166" s="21"/>
+      <c r="H166" s="21"/>
+      <c r="N166" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="O166" s="26"/>
-      <c r="P166" s="26"/>
-    </row>
-    <row r="169" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O166" s="21"/>
+      <c r="P166" s="21"/>
+    </row>
+    <row r="169" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B169" s="13" t="s">
         <v>152</v>
       </c>
       <c r="C169" s="13"/>
       <c r="D169" s="13"/>
-      <c r="F169" s="27" t="s">
+      <c r="F169" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="G169" s="27"/>
-      <c r="H169" s="27"/>
-      <c r="J169" s="28" t="s">
+      <c r="G169" s="22"/>
+      <c r="H169" s="22"/>
+      <c r="J169" s="23" t="s">
         <v>153</v>
       </c>
-      <c r="K169" s="28"/>
-      <c r="L169" s="28"/>
-      <c r="N169" s="27" t="s">
+      <c r="K169" s="23"/>
+      <c r="L169" s="23"/>
+      <c r="N169" s="22" t="s">
         <v>173</v>
       </c>
-      <c r="O169" s="27"/>
-      <c r="P169" s="27"/>
-    </row>
-    <row r="170" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="O169" s="22"/>
+      <c r="P169" s="22"/>
+    </row>
+    <row r="170" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B170" s="10" t="s">
         <v>192</v>
       </c>
@@ -7214,7 +6819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B171" s="10" t="s">
         <v>63</v>
       </c>
@@ -7250,7 +6855,7 @@
       </c>
       <c r="P171" s="10"/>
     </row>
-    <row r="172" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B172" s="10" t="s">
         <v>64</v>
       </c>
@@ -7286,7 +6891,7 @@
       </c>
       <c r="P172" s="10"/>
     </row>
-    <row r="173" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B173" s="10" t="s">
         <v>65</v>
       </c>
@@ -7322,7 +6927,7 @@
       </c>
       <c r="P173" s="10"/>
     </row>
-    <row r="174" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B174" s="10" t="s">
         <v>66</v>
       </c>
@@ -7358,7 +6963,7 @@
       </c>
       <c r="P174" s="10"/>
     </row>
-    <row r="175" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B175" s="10" t="s">
         <v>67</v>
       </c>
@@ -7394,7 +6999,7 @@
       </c>
       <c r="P175" s="10"/>
     </row>
-    <row r="176" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B176" s="10" t="s">
         <v>68</v>
       </c>
@@ -7430,7 +7035,7 @@
       </c>
       <c r="P176" s="10"/>
     </row>
-    <row r="177" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B177" s="10" t="s">
         <v>69</v>
       </c>
@@ -7466,7 +7071,7 @@
       </c>
       <c r="P177" s="10"/>
     </row>
-    <row r="178" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B178" s="10" t="s">
         <v>70</v>
       </c>
@@ -7502,119 +7107,119 @@
       </c>
       <c r="P178" s="10"/>
     </row>
-    <row r="182" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B182" s="13" t="s">
         <v>267</v>
       </c>
       <c r="C182" s="13"/>
       <c r="D182" s="13"/>
     </row>
-    <row r="183" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B183" s="29">
+    <row r="183" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B183" s="15">
         <v>5</v>
       </c>
-      <c r="C183" s="30"/>
-      <c r="D183" s="31"/>
-    </row>
-    <row r="184" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B184" s="32">
+      <c r="C183" s="16"/>
+      <c r="D183" s="17"/>
+    </row>
+    <row r="184" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B184" s="24">
         <v>-3</v>
       </c>
-      <c r="C184" s="30"/>
-      <c r="D184" s="31"/>
-    </row>
-    <row r="185" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B185" s="29">
+      <c r="C184" s="16"/>
+      <c r="D184" s="17"/>
+    </row>
+    <row r="185" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B185" s="15">
         <v>0</v>
       </c>
-      <c r="C185" s="30"/>
-      <c r="D185" s="31"/>
-    </row>
-    <row r="188" spans="2:16" x14ac:dyDescent="0.55000000000000004">
+      <c r="C185" s="16"/>
+      <c r="D185" s="17"/>
+    </row>
+    <row r="188" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B188" s="13" t="s">
         <v>268</v>
       </c>
       <c r="C188" s="13"/>
       <c r="D188" s="13"/>
     </row>
-    <row r="189" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B189" s="29">
+    <row r="189" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B189" s="15">
         <v>-5.5</v>
       </c>
-      <c r="C189" s="30"/>
-      <c r="D189" s="31"/>
-    </row>
-    <row r="190" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B190" s="29">
+      <c r="C189" s="16"/>
+      <c r="D189" s="17"/>
+    </row>
+    <row r="190" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B190" s="15">
         <v>3.3</v>
       </c>
-      <c r="C190" s="30"/>
-      <c r="D190" s="31"/>
-    </row>
-    <row r="191" spans="2:16" x14ac:dyDescent="0.55000000000000004">
-      <c r="B191" s="29">
+      <c r="C190" s="16"/>
+      <c r="D190" s="17"/>
+    </row>
+    <row r="191" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B191" s="15">
         <v>-1</v>
       </c>
-      <c r="C191" s="30"/>
-      <c r="D191" s="31"/>
-    </row>
-    <row r="194" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C191" s="16"/>
+      <c r="D191" s="17"/>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B194" s="13" t="s">
         <v>269</v>
       </c>
       <c r="C194" s="13"/>
       <c r="D194" s="13"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B195" s="29" t="b">
+    <row r="195" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B195" s="15" t="b">
         <v>1</v>
       </c>
-      <c r="C195" s="30"/>
-      <c r="D195" s="31"/>
-    </row>
-    <row r="196" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B196" s="29" t="b">
+      <c r="C195" s="16"/>
+      <c r="D195" s="17"/>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B196" s="15" t="b">
         <v>0</v>
       </c>
-      <c r="C196" s="30"/>
-      <c r="D196" s="31"/>
-    </row>
-    <row r="199" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C196" s="16"/>
+      <c r="D196" s="17"/>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B199" s="13" t="s">
         <v>238</v>
       </c>
       <c r="C199" s="13"/>
       <c r="D199" s="13"/>
     </row>
-    <row r="200" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B200" s="29" t="s">
+    <row r="200" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B200" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="C200" s="30"/>
-      <c r="D200" s="31"/>
-    </row>
-    <row r="201" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B201" s="29" t="s">
+      <c r="C200" s="16"/>
+      <c r="D200" s="17"/>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B201" s="15" t="s">
         <v>240</v>
       </c>
-      <c r="C201" s="30"/>
-      <c r="D201" s="31"/>
-    </row>
-    <row r="202" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B202" s="29" t="s">
+      <c r="C201" s="16"/>
+      <c r="D201" s="17"/>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B202" s="15" t="s">
         <v>241</v>
       </c>
-      <c r="C202" s="30"/>
-      <c r="D202" s="31"/>
-    </row>
-    <row r="205" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C202" s="16"/>
+      <c r="D202" s="17"/>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B205" s="13" t="s">
         <v>203</v>
       </c>
       <c r="C205" s="13"/>
       <c r="D205" s="13"/>
     </row>
-    <row r="206" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B206" s="10" t="s">
         <v>242</v>
       </c>
@@ -7625,7 +7230,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="207" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B207" s="10" t="s">
         <v>1</v>
       </c>
@@ -7634,7 +7239,7 @@
       </c>
       <c r="D207" s="10"/>
     </row>
-    <row r="208" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B208" s="10" t="s">
         <v>4</v>
       </c>
@@ -7643,14 +7248,14 @@
       </c>
       <c r="D208" s="10"/>
     </row>
-    <row r="211" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B211" s="13" t="s">
         <v>205</v>
       </c>
       <c r="C211" s="13"/>
       <c r="D211" s="13"/>
     </row>
-    <row r="212" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B212" s="10" t="s">
         <v>0</v>
       </c>
@@ -7661,7 +7266,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="213" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B213" s="10" t="s">
         <v>4</v>
       </c>
@@ -7670,7 +7275,7 @@
       </c>
       <c r="D213" s="10"/>
     </row>
-    <row r="214" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B214" s="10" t="s">
         <v>6</v>
       </c>
@@ -7681,14 +7286,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B217" s="13" t="s">
         <v>204</v>
       </c>
       <c r="C217" s="13"/>
       <c r="D217" s="13"/>
     </row>
-    <row r="218" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B218" s="10" t="s">
         <v>8</v>
       </c>
@@ -7699,7 +7304,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="219" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="219" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B219" s="10" t="s">
         <v>209</v>
       </c>
@@ -7710,7 +7315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="220" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B220" s="10" t="s">
         <v>6</v>
       </c>
@@ -7719,286 +7324,286 @@
       </c>
       <c r="D220" s="10"/>
     </row>
-    <row r="223" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B223" s="28" t="s">
+    <row r="223" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B223" s="23" t="s">
         <v>247</v>
       </c>
-      <c r="C223" s="28"/>
-      <c r="D223" s="28"/>
-      <c r="E223" s="28"/>
-      <c r="F223" s="28"/>
-    </row>
-    <row r="224" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="C223" s="23"/>
+      <c r="D223" s="23"/>
+      <c r="E223" s="23"/>
+      <c r="F223" s="23"/>
+    </row>
+    <row r="224" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B224" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C224" s="33" t="s">
+      <c r="C224" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="D224" s="34"/>
-      <c r="E224" s="34"/>
-      <c r="F224" s="35"/>
-    </row>
-    <row r="225" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D224" s="26"/>
+      <c r="E224" s="26"/>
+      <c r="F224" s="27"/>
+    </row>
+    <row r="225" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B225" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C225" s="29" t="s">
+      <c r="C225" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="D225" s="30"/>
-      <c r="E225" s="30"/>
-      <c r="F225" s="31"/>
-    </row>
-    <row r="226" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D225" s="16"/>
+      <c r="E225" s="16"/>
+      <c r="F225" s="17"/>
+    </row>
+    <row r="226" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B226" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C226" s="37" t="s">
+      <c r="C226" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="D226" s="15"/>
-      <c r="E226" s="15"/>
-      <c r="F226" s="16"/>
-    </row>
-    <row r="227" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D226" s="19"/>
+      <c r="E226" s="19"/>
+      <c r="F226" s="20"/>
+    </row>
+    <row r="227" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B227" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C227" s="36" t="s">
+      <c r="C227" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="D227" s="36"/>
-      <c r="E227" s="36"/>
-      <c r="F227" s="36"/>
-    </row>
-    <row r="228" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D227" s="14"/>
+      <c r="E227" s="14"/>
+      <c r="F227" s="14"/>
+    </row>
+    <row r="228" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B228" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C228" s="14" t="s">
+      <c r="C228" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="D228" s="15"/>
-      <c r="E228" s="15"/>
-      <c r="F228" s="16"/>
-    </row>
-    <row r="233" spans="2:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D228" s="19"/>
+      <c r="E228" s="19"/>
+      <c r="F228" s="20"/>
+    </row>
+    <row r="233" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B233" s="13" t="s">
         <v>259</v>
       </c>
       <c r="C233" s="13"/>
       <c r="D233" s="13"/>
     </row>
-    <row r="234" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B234" s="17" t="s">
+    <row r="234" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B234" s="29" t="s">
         <v>260</v>
       </c>
-      <c r="C234" s="18"/>
-      <c r="D234" s="19"/>
-    </row>
-    <row r="235" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B235" s="20"/>
-      <c r="C235" s="21"/>
-      <c r="D235" s="22"/>
-    </row>
-    <row r="236" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B236" s="20"/>
-      <c r="C236" s="21"/>
-      <c r="D236" s="22"/>
-    </row>
-    <row r="237" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B237" s="20"/>
-      <c r="C237" s="21"/>
-      <c r="D237" s="22"/>
-    </row>
-    <row r="238" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B238" s="20"/>
-      <c r="C238" s="21"/>
-      <c r="D238" s="22"/>
-    </row>
-    <row r="239" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B239" s="20"/>
-      <c r="C239" s="21"/>
-      <c r="D239" s="22"/>
-    </row>
-    <row r="240" spans="2:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="B240" s="20"/>
-      <c r="C240" s="21"/>
-      <c r="D240" s="22"/>
-    </row>
-    <row r="241" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B241" s="20"/>
-      <c r="C241" s="21"/>
-      <c r="D241" s="22"/>
-    </row>
-    <row r="242" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B242" s="20"/>
-      <c r="C242" s="21"/>
-      <c r="D242" s="22"/>
-    </row>
-    <row r="243" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B243" s="20"/>
-      <c r="C243" s="21"/>
-      <c r="D243" s="22"/>
-    </row>
-    <row r="244" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B244" s="20"/>
-      <c r="C244" s="21"/>
-      <c r="D244" s="22"/>
-    </row>
-    <row r="245" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B245" s="23"/>
-      <c r="C245" s="24"/>
-      <c r="D245" s="25"/>
-    </row>
-    <row r="249" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="C234" s="30"/>
+      <c r="D234" s="31"/>
+    </row>
+    <row r="235" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B235" s="32"/>
+      <c r="C235" s="33"/>
+      <c r="D235" s="34"/>
+    </row>
+    <row r="236" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B236" s="32"/>
+      <c r="C236" s="33"/>
+      <c r="D236" s="34"/>
+    </row>
+    <row r="237" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B237" s="32"/>
+      <c r="C237" s="33"/>
+      <c r="D237" s="34"/>
+    </row>
+    <row r="238" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B238" s="32"/>
+      <c r="C238" s="33"/>
+      <c r="D238" s="34"/>
+    </row>
+    <row r="239" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B239" s="32"/>
+      <c r="C239" s="33"/>
+      <c r="D239" s="34"/>
+    </row>
+    <row r="240" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B240" s="32"/>
+      <c r="C240" s="33"/>
+      <c r="D240" s="34"/>
+    </row>
+    <row r="241" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B241" s="32"/>
+      <c r="C241" s="33"/>
+      <c r="D241" s="34"/>
+    </row>
+    <row r="242" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B242" s="32"/>
+      <c r="C242" s="33"/>
+      <c r="D242" s="34"/>
+    </row>
+    <row r="243" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B243" s="32"/>
+      <c r="C243" s="33"/>
+      <c r="D243" s="34"/>
+    </row>
+    <row r="244" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B244" s="32"/>
+      <c r="C244" s="33"/>
+      <c r="D244" s="34"/>
+    </row>
+    <row r="245" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B245" s="35"/>
+      <c r="C245" s="36"/>
+      <c r="D245" s="37"/>
+    </row>
+    <row r="249" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B249" s="13" t="s">
         <v>261</v>
       </c>
       <c r="C249" s="13"/>
       <c r="D249" s="13"/>
     </row>
-    <row r="250" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B250" s="17" t="s">
+    <row r="250" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B250" s="29" t="s">
         <v>262</v>
       </c>
-      <c r="C250" s="18" t="s">
+      <c r="C250" s="30" t="s">
         <v>260</v>
       </c>
-      <c r="D250" s="19" t="s">
+      <c r="D250" s="31" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="251" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B251" s="20" t="s">
+    <row r="251" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B251" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C251" s="21" t="s">
+      <c r="C251" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D251" s="22" t="s">
+      <c r="D251" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="252" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B252" s="20" t="s">
+    <row r="252" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B252" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C252" s="21" t="s">
+      <c r="C252" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D252" s="22" t="s">
+      <c r="D252" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="253" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B253" s="20" t="s">
+    <row r="253" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B253" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C253" s="21" t="s">
+      <c r="C253" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D253" s="22" t="s">
+      <c r="D253" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="254" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B254" s="20" t="s">
+    <row r="254" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B254" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C254" s="21" t="s">
+      <c r="C254" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D254" s="22" t="s">
+      <c r="D254" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="255" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B255" s="20" t="s">
+    <row r="255" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B255" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C255" s="21" t="s">
+      <c r="C255" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D255" s="22" t="s">
+      <c r="D255" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="256" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B256" s="20" t="s">
+    <row r="256" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B256" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C256" s="21" t="s">
+      <c r="C256" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D256" s="22" t="s">
+      <c r="D256" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="257" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B257" s="20" t="s">
+    <row r="257" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B257" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C257" s="21" t="s">
+      <c r="C257" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D257" s="22" t="s">
+      <c r="D257" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="258" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B258" s="20" t="s">
+    <row r="258" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B258" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C258" s="21" t="s">
+      <c r="C258" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D258" s="22" t="s">
+      <c r="D258" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="259" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B259" s="20" t="s">
+    <row r="259" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B259" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C259" s="21" t="s">
+      <c r="C259" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D259" s="22" t="s">
+      <c r="D259" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="260" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B260" s="20" t="s">
+    <row r="260" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B260" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="C260" s="21" t="s">
+      <c r="C260" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="D260" s="22" t="s">
+      <c r="D260" s="34" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="261" spans="2:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="B261" s="23" t="s">
+    <row r="261" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B261" s="35" t="s">
         <v>260</v>
       </c>
-      <c r="C261" s="24" t="s">
+      <c r="C261" s="36" t="s">
         <v>260</v>
       </c>
-      <c r="D261" s="25" t="s">
+      <c r="D261" s="37" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="265" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B265" s="13" t="s">
         <v>263</v>
       </c>
       <c r="C265" s="13"/>
       <c r="D265" s="13"/>
     </row>
-    <row r="266" spans="2:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B266" s="10" t="s">
         <v>264</v>
       </c>
@@ -8009,8 +7614,618 @@
         <v>266</v>
       </c>
     </row>
+    <row r="268">
+      <c r="B268" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="C268" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="D268" s="13" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="B269" t="str" s="10">
+        <f>"_res_."&amp;C8</f>
+        <v>_res_.test</v>
+      </c>
+      <c r="C269" t="str" s="10">
+        <f>C8</f>
+        <v>test</v>
+      </c>
+      <c r="D269" t="n" s="10">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="B270" t="str" s="10">
+        <f>"_res_."&amp;C9</f>
+        <v>_res_.byteValue</v>
+      </c>
+      <c r="C270" t="str" s="10">
+        <f>C9</f>
+        <v>byteValue</v>
+      </c>
+      <c r="D270" t="n" s="10">
+        <f>D9</f>
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="B271" t="str" s="10">
+        <f>"_res_."&amp;C10</f>
+        <v>_res_.shortValue</v>
+      </c>
+      <c r="C271" t="str" s="10">
+        <f>C10</f>
+        <v>shortValue</v>
+      </c>
+      <c r="D271" t="n" s="10">
+        <f>D10</f>
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="B272" t="str" s="10">
+        <f>"_res_."&amp;C11</f>
+        <v>_res_.intValue</v>
+      </c>
+      <c r="C272" t="str" s="10">
+        <f>C11</f>
+        <v>intValue</v>
+      </c>
+      <c r="D272" t="n" s="10">
+        <f>D11</f>
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="B273" t="str" s="10">
+        <f>"_res_."&amp;C12</f>
+        <v>_res_.longValue</v>
+      </c>
+      <c r="C273" t="str" s="10">
+        <f>C12</f>
+        <v>longValue</v>
+      </c>
+      <c r="D273" t="n" s="10">
+        <f>D12</f>
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="B274" t="str" s="10">
+        <f>"_res_."&amp;C13</f>
+        <v>_res_.floatValue</v>
+      </c>
+      <c r="C274" t="str" s="10">
+        <f>C13</f>
+        <v>floatValue</v>
+      </c>
+      <c r="D274" t="n" s="10">
+        <f>D13</f>
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="B275" t="str" s="10">
+        <f>"_res_."&amp;C14</f>
+        <v>_res_.doubleValue</v>
+      </c>
+      <c r="C275" t="str" s="10">
+        <f>C14</f>
+        <v>doubleValue</v>
+      </c>
+      <c r="D275" t="n" s="10">
+        <f>D14</f>
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="B276" t="str" s="10">
+        <f>"_res_."&amp;C15</f>
+        <v>_res_.booleanValue</v>
+      </c>
+      <c r="C276" t="str" s="10">
+        <f>C15</f>
+        <v>booleanValue</v>
+      </c>
+      <c r="D276" t="str" s="10">
+        <f>D15</f>
+        <v>y</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="B277" t="str" s="10">
+        <f>"_res_."&amp;C16</f>
+        <v>_res_.charValue</v>
+      </c>
+      <c r="C277" t="str" s="10">
+        <f>C16</f>
+        <v>charValue</v>
+      </c>
+      <c r="D277" t="str" s="10">
+        <f>D16</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="B278" t="str" s="10">
+        <f>"_res_."&amp;C17</f>
+        <v>_res_.string</v>
+      </c>
+      <c r="C278" t="str" s="10">
+        <f>C17</f>
+        <v>string</v>
+      </c>
+      <c r="D278" t="str" s="10">
+        <f>D17</f>
+        <v>str</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="B279" t="str" s="10">
+        <f>"_res_."&amp;C18</f>
+        <v>_res_.date</v>
+      </c>
+      <c r="C279" t="str" s="10">
+        <f>C18</f>
+        <v>date</v>
+      </c>
+      <c r="D279" t="str" s="10">
+        <f>D18</f>
+        <v>03/31/2017</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="B280" t="str" s="10">
+        <f>"_res_."&amp;C19</f>
+        <v>_res_.localDate</v>
+      </c>
+      <c r="C280" t="str" s="10">
+        <f>C19</f>
+        <v>localDate</v>
+      </c>
+      <c r="D280" t="str" s="10">
+        <f>D19</f>
+        <v>03/31/2017</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="B281" t="str" s="10">
+        <f>"_res_."&amp;C20</f>
+        <v>_res_.localTime</v>
+      </c>
+      <c r="C281" t="str" s="10">
+        <f>C20</f>
+        <v>localTime</v>
+      </c>
+      <c r="D281" t="str" s="10">
+        <f>D20</f>
+        <v>21:30:25</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="B282" t="str" s="10">
+        <f>"_res_."&amp;C21</f>
+        <v>_res_.localDateTime</v>
+      </c>
+      <c r="C282" t="str" s="10">
+        <f>C21</f>
+        <v>localDateTime</v>
+      </c>
+      <c r="D282" t="str" s="10">
+        <f>D21</f>
+        <v>9/20/2019 5:50 AM</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="B283" t="str" s="10">
+        <f>"_res_."&amp;C22</f>
+        <v>_res_.zonedDateTime</v>
+      </c>
+      <c r="C283" t="str" s="10">
+        <f>C22</f>
+        <v>zonedDateTime</v>
+      </c>
+      <c r="D283" t="str" s="10">
+        <f>D22</f>
+        <v>9/20/2019 5:50 AM America/Los_Angeles</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="B284" t="str" s="12">
+        <f>"_res_."&amp;C23</f>
+        <v>_res_.instantDate</v>
+      </c>
+      <c r="C284" t="str" s="12">
+        <f>C23</f>
+        <v>instantDate</v>
+      </c>
+      <c r="D284" t="str" s="12">
+        <f>D23</f>
+        <v>9/20/2019 5:50 AM America/Los_Angeles</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="B285" t="str" s="10">
+        <f>"_res_."&amp;C24</f>
+        <v>_res_.bigInt</v>
+      </c>
+      <c r="C285" t="str" s="10">
+        <f>C24</f>
+        <v>bigInt</v>
+      </c>
+      <c r="D285" t="n" s="10">
+        <f>D24</f>
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="B286" t="str" s="10">
+        <f>"_res_."&amp;C25</f>
+        <v>_res_.bigDec</v>
+      </c>
+      <c r="C286" t="str" s="10">
+        <f>C25</f>
+        <v>bigDec</v>
+      </c>
+      <c r="D286" t="n" s="10">
+        <f>D25</f>
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="B287" t="str" s="10">
+        <f>"_res_."&amp;C26</f>
+        <v>_res_.col</v>
+      </c>
+      <c r="C287" t="str" s="10">
+        <f>C26</f>
+        <v>col</v>
+      </c>
+      <c r="D287" s="10"/>
+    </row>
+    <row r="288">
+      <c r="B288" t="str" s="10">
+        <f>"_res_."&amp;C27</f>
+        <v>_res_.list</v>
+      </c>
+      <c r="C288" t="str" s="10">
+        <f>C27</f>
+        <v>list</v>
+      </c>
+      <c r="D288" s="10"/>
+    </row>
+    <row r="289">
+      <c r="B289" t="str" s="10">
+        <f>"_res_."&amp;C28</f>
+        <v>_res_.map</v>
+      </c>
+      <c r="C289" t="str" s="10">
+        <f>C28</f>
+        <v>map</v>
+      </c>
+      <c r="D289" s="10"/>
+    </row>
+    <row r="290">
+      <c r="B290" t="str" s="10">
+        <f>"_res_."&amp;C29</f>
+        <v>_res_.set</v>
+      </c>
+      <c r="C290" t="str" s="10">
+        <f>C29</f>
+        <v>set</v>
+      </c>
+      <c r="D290" s="10"/>
+    </row>
+    <row r="291">
+      <c r="B291" t="str" s="10">
+        <f>"_res_."&amp;C30</f>
+        <v>_res_.arrayList</v>
+      </c>
+      <c r="C291" t="str" s="10">
+        <f>C30</f>
+        <v>arrayList</v>
+      </c>
+      <c r="D291" s="10"/>
+    </row>
+    <row r="292">
+      <c r="B292" t="str" s="10">
+        <f>"_res_."&amp;C31</f>
+        <v>_res_.hashMap</v>
+      </c>
+      <c r="C292" t="str" s="10">
+        <f>C31</f>
+        <v>hashMap</v>
+      </c>
+      <c r="D292" s="10"/>
+    </row>
+    <row r="293">
+      <c r="B293" t="str" s="10">
+        <f>"_res_."&amp;C32</f>
+        <v>_res_.hashSet</v>
+      </c>
+      <c r="C293" t="str" s="10">
+        <f>C32</f>
+        <v>hashSet</v>
+      </c>
+      <c r="D293" s="10"/>
+    </row>
+    <row r="294">
+      <c r="B294" t="str" s="10">
+        <f>"_res_."&amp;C33</f>
+        <v>_res_.roudingMode</v>
+      </c>
+      <c r="C294" t="str" s="10">
+        <f>C33</f>
+        <v>roudingMode</v>
+      </c>
+      <c r="D294" t="str" s="10">
+        <f>D33</f>
+        <v>HALF_EVEN</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="B295" t="str" s="10">
+        <f>"_res_."&amp;C34</f>
+        <v>_res_.dv</v>
+      </c>
+      <c r="C295" t="str" s="10">
+        <f>C34</f>
+        <v>dv</v>
+      </c>
+      <c r="D295" t="n" s="10">
+        <f>D34</f>
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="B296" t="str" s="10">
+        <f>"_res_."&amp;C35</f>
+        <v>_res_.intAlias</v>
+      </c>
+      <c r="C296" t="str" s="10">
+        <f>C35</f>
+        <v>intAlias</v>
+      </c>
+      <c r="D296" t="n" s="10">
+        <f>D35</f>
+        <v>-3.0</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="B297" t="str" s="10">
+        <f>"_res_."&amp;C36</f>
+        <v>_res_.doubleAlias</v>
+      </c>
+      <c r="C297" t="str" s="10">
+        <f>C36</f>
+        <v>doubleAlias</v>
+      </c>
+      <c r="D297" t="n" s="10">
+        <f>D36</f>
+        <v>3.3</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="B298" t="str" s="10">
+        <f>"_res_."&amp;C37</f>
+        <v>_res_.boolAlias</v>
+      </c>
+      <c r="C298" t="str" s="10">
+        <f>C37</f>
+        <v>boolAlias</v>
+      </c>
+      <c r="D298" t="str" s="10">
+        <f>D37</f>
+        <v>n</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="B299" t="str" s="10">
+        <f>"_res_."&amp;C38</f>
+        <v>_res_.gender</v>
+      </c>
+      <c r="C299" t="str" s="10">
+        <f>C38</f>
+        <v>gender</v>
+      </c>
+      <c r="D299" t="str" s="10">
+        <f>D38</f>
+        <v>Male</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="B300" t="s" s="10">
+        <v>337</v>
+      </c>
+      <c r="C300" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="D300" t="s" s="10">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="B301" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="C301" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="D301" s="10"/>
+    </row>
+    <row r="302">
+      <c r="B302" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="C302" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="D302" s="10"/>
+    </row>
+    <row r="303">
+      <c r="B303" s="10" t="s">
+        <v>346</v>
+      </c>
+      <c r="C303" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="D303" s="10" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="B304" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="C304" s="10" t="s">
+        <v>349</v>
+      </c>
+      <c r="D304" s="10"/>
+    </row>
+    <row r="305">
+      <c r="B305" s="10" t="s">
+        <v>338</v>
+      </c>
+      <c r="C305" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="D305" s="10"/>
+    </row>
+    <row r="306">
+      <c r="B306" s="10" t="s">
+        <v>286</v>
+      </c>
+      <c r="C306" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="D306" s="10" t="n">
+        <v>150.0</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="B307" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="C307" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D307" s="10"/>
+    </row>
+    <row r="308">
+      <c r="B308" s="10" t="s">
+        <v>290</v>
+      </c>
+      <c r="C308" s="10" t="s">
+        <v>289</v>
+      </c>
+      <c r="D308" s="10" t="n">
+        <v>150.0</v>
+      </c>
+    </row>
+    <row r="309">
+      <c r="B309" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="C309" s="10" t="s">
+        <v>292</v>
+      </c>
+      <c r="D309" s="10"/>
+    </row>
+    <row r="310">
+      <c r="B310" s="10" t="s">
+        <v>293</v>
+      </c>
+      <c r="C310" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="D310" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="B311" s="10" t="s">
+        <v>294</v>
+      </c>
+      <c r="C311" s="10" t="s">
+        <v>296</v>
+      </c>
+      <c r="D311" s="10"/>
+    </row>
+    <row r="312">
+      <c r="B312" t="s" s="10">
+        <v>295</v>
+      </c>
+      <c r="C312" t="s" s="10">
+        <v>297</v>
+      </c>
+      <c r="D312" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="77">
+  <mergeCells count="78">
+    <mergeCell ref="B265:D265"/>
+    <mergeCell ref="C228:F228"/>
+    <mergeCell ref="B233:D233"/>
+    <mergeCell ref="B234:D245"/>
+    <mergeCell ref="B249:D249"/>
+    <mergeCell ref="B250:D261"/>
+    <mergeCell ref="F166:H166"/>
+    <mergeCell ref="N166:P166"/>
+    <mergeCell ref="B169:D169"/>
+    <mergeCell ref="F169:H169"/>
+    <mergeCell ref="J169:L169"/>
+    <mergeCell ref="N169:P169"/>
+    <mergeCell ref="F125:H125"/>
+    <mergeCell ref="N125:P125"/>
+    <mergeCell ref="B128:D128"/>
+    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="J128:L128"/>
+    <mergeCell ref="N128:P128"/>
+    <mergeCell ref="N71:P71"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="N109:P109"/>
+    <mergeCell ref="B112:D112"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="J112:L112"/>
+    <mergeCell ref="N112:P112"/>
+    <mergeCell ref="N108:P108"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="J71:L71"/>
+    <mergeCell ref="B183:D183"/>
+    <mergeCell ref="B184:D184"/>
+    <mergeCell ref="B185:D185"/>
+    <mergeCell ref="B191:D191"/>
+    <mergeCell ref="C224:F224"/>
+    <mergeCell ref="B196:D196"/>
+    <mergeCell ref="B202:D202"/>
+    <mergeCell ref="B205:D205"/>
+    <mergeCell ref="B211:D211"/>
+    <mergeCell ref="B217:D217"/>
+    <mergeCell ref="B223:F223"/>
+    <mergeCell ref="N3:P3"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="N7:P7"/>
+    <mergeCell ref="N51:P51"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F51:H51"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="N67:P67"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="F67:H67"/>
+    <mergeCell ref="F52:H52"/>
+    <mergeCell ref="F68:H68"/>
+    <mergeCell ref="N68:P68"/>
+    <mergeCell ref="N52:P52"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="J55:L55"/>
+    <mergeCell ref="N55:P55"/>
     <mergeCell ref="N124:P124"/>
     <mergeCell ref="F124:H124"/>
     <mergeCell ref="N165:P165"/>
@@ -8027,70 +8242,11 @@
     <mergeCell ref="C226:F226"/>
     <mergeCell ref="C225:F225"/>
     <mergeCell ref="B182:D182"/>
-    <mergeCell ref="N67:P67"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="F67:H67"/>
-    <mergeCell ref="F52:H52"/>
-    <mergeCell ref="F68:H68"/>
-    <mergeCell ref="N68:P68"/>
-    <mergeCell ref="N52:P52"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="F55:H55"/>
-    <mergeCell ref="J55:L55"/>
-    <mergeCell ref="N55:P55"/>
-    <mergeCell ref="N3:P3"/>
-    <mergeCell ref="N4:P4"/>
-    <mergeCell ref="N7:P7"/>
-    <mergeCell ref="N51:P51"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F51:H51"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="B183:D183"/>
-    <mergeCell ref="B184:D184"/>
-    <mergeCell ref="B185:D185"/>
-    <mergeCell ref="B191:D191"/>
-    <mergeCell ref="C224:F224"/>
-    <mergeCell ref="B196:D196"/>
-    <mergeCell ref="B202:D202"/>
-    <mergeCell ref="B205:D205"/>
-    <mergeCell ref="B211:D211"/>
-    <mergeCell ref="B217:D217"/>
-    <mergeCell ref="B223:F223"/>
-    <mergeCell ref="N71:P71"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="N109:P109"/>
-    <mergeCell ref="B112:D112"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="J112:L112"/>
-    <mergeCell ref="N112:P112"/>
-    <mergeCell ref="N108:P108"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="F71:H71"/>
-    <mergeCell ref="J71:L71"/>
-    <mergeCell ref="F125:H125"/>
-    <mergeCell ref="N125:P125"/>
-    <mergeCell ref="B128:D128"/>
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="J128:L128"/>
-    <mergeCell ref="N128:P128"/>
-    <mergeCell ref="F166:H166"/>
-    <mergeCell ref="N166:P166"/>
-    <mergeCell ref="B169:D169"/>
-    <mergeCell ref="F169:H169"/>
-    <mergeCell ref="J169:L169"/>
-    <mergeCell ref="N169:P169"/>
-    <mergeCell ref="B265:D265"/>
-    <mergeCell ref="C228:F228"/>
-    <mergeCell ref="B233:D233"/>
-    <mergeCell ref="B234:D245"/>
-    <mergeCell ref="B249:D249"/>
-    <mergeCell ref="B250:D261"/>
+    <mergeCell ref="B268:D268"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId4"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -8103,18 +8259,18 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.83984375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23.26171875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="23.26171875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="37.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="20.68359375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="24.26171875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="6.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="23.21875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="23.21875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.6640625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="37.6640625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.6640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="24.21875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="38" t="s">
         <v>84</v>
       </c>
@@ -8125,7 +8281,7 @@
       <c r="G3" s="38"/>
       <c r="H3" s="38"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>75</v>
       </c>
@@ -8148,7 +8304,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>77</v>
       </c>
@@ -8171,7 +8327,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
         <v>79</v>
       </c>
@@ -8194,7 +8350,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
         <v>81</v>
       </c>
@@ -8217,7 +8373,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
         <v>151</v>
       </c>
@@ -8240,7 +8396,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
         <v>85</v>
       </c>
@@ -8263,7 +8419,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B10" s="3" t="s">
         <v>86</v>
       </c>
@@ -8286,7 +8442,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B11" s="3" t="s">
         <v>96</v>
       </c>
@@ -8309,7 +8465,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B12" s="3" t="s">
         <v>97</v>
       </c>
@@ -8332,7 +8488,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="3" t="s">
         <v>123</v>
       </c>
@@ -8355,7 +8511,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>124</v>
       </c>
@@ -8378,7 +8534,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="3" t="s">
         <v>125</v>
       </c>
@@ -8401,7 +8557,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="3" t="s">
         <v>126</v>
       </c>
@@ -8424,7 +8580,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="3" t="s">
         <v>195</v>
       </c>
@@ -8441,7 +8597,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="38" t="s">
         <v>334</v>
       </c>
@@ -8452,7 +8608,7 @@
       <c r="G20" s="38"/>
       <c r="H20" s="38"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -8469,7 +8625,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>75</v>
       </c>
@@ -8492,7 +8648,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>195</v>
       </c>
@@ -8526,15 +8682,15 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.15625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.68359375" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="16.109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="41" t="s">
         <v>90</v>
       </c>
@@ -8545,7 +8701,7 @@
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
         <v>91</v>
       </c>
@@ -8560,7 +8716,7 @@
       </c>
       <c r="G4" s="40"/>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>92</v>
       </c>
@@ -8575,7 +8731,7 @@
       </c>
       <c r="G5" s="40"/>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E6" s="7" t="s">
         <v>303</v>
       </c>
@@ -8584,7 +8740,7 @@
       </c>
       <c r="G6" s="40"/>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E7" s="7" t="s">
         <v>303</v>
       </c>
@@ -8593,7 +8749,7 @@
       </c>
       <c r="G7" s="40"/>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E8" s="7" t="s">
         <v>303</v>
       </c>

</xml_diff>